<commit_message>
Newer hyperparameter search results
</commit_message>
<xml_diff>
--- a/experiments/hyperparameters/hyperparemeter_search.xlsx
+++ b/experiments/hyperparameters/hyperparemeter_search.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="174" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="349" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="119">
   <si>
     <t>EXPERIMENT 1</t>
   </si>
@@ -266,7 +266,7 @@
     <t>run52</t>
   </si>
   <si>
-    <t>Alpha divided by 10 after 30 epochs, and then again after 10 epochs</t>
+    <t>Alpha divided by 10 at epoch 30, and again at epoch 40</t>
   </si>
   <si>
     <t>EXPERIMENT 2</t>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>run59</t>
+  </si>
+  <si>
+    <t>converges to same point</t>
   </si>
   <si>
     <t>run60</t>
@@ -450,7 +453,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -469,10 +472,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -494,8 +493,8 @@
   </sheetPr>
   <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F110" activeCellId="0" sqref="F110"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C77" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D77" activeCellId="0" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2015,30 +2014,30 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
@@ -2082,6 +2081,15 @@
       <c r="D82" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E82" s="0" t="n">
+        <v>0.047</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>0.119</v>
+      </c>
+      <c r="G82" s="0" t="n">
+        <v>0.84</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="n">
@@ -2096,6 +2104,15 @@
       <c r="D83" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="E83" s="0" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="G83" s="0" t="n">
+        <v>0.78</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="n">
@@ -2110,6 +2127,15 @@
       <c r="D84" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E84" s="0" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="F84" s="0" t="n">
+        <v>0.119</v>
+      </c>
+      <c r="G84" s="0" t="n">
+        <v>0.74</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="n">
@@ -2124,6 +2150,15 @@
       <c r="D85" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="E85" s="0" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="F85" s="0" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G85" s="0" t="n">
+        <v>0.71</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="n">
@@ -2138,6 +2173,15 @@
       <c r="D86" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="E86" s="0" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="F86" s="0" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G86" s="0" t="n">
+        <v>0.68</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="n">
@@ -2152,6 +2196,15 @@
       <c r="D87" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="E87" s="0" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="G87" s="0" t="n">
+        <v>0.58</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="n">
@@ -2166,6 +2219,21 @@
       <c r="D88" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="E88" s="0" t="n">
+        <v>0.071</v>
+      </c>
+      <c r="F88" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G88" s="0" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="H88" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="I88" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="n">
@@ -2175,10 +2243,19 @@
         <v>0.00363581666441528</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>8</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <v>0.038</v>
+      </c>
+      <c r="F89" s="0" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="G89" s="0" t="n">
+        <v>0.54</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2189,10 +2266,16 @@
         <v>0.385037978791714</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>9</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="I90" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2203,10 +2286,16 @@
         <v>0.046693736064734</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D91" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="E91" s="0" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="I91" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2217,10 +2306,22 @@
         <v>0.162706410105612</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D92" s="0" t="n">
         <v>11</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>0.047</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="G92" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I92" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,10 +2332,19 @@
         <v>0.000189095715104318</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D93" s="0" t="n">
         <v>12</v>
+      </c>
+      <c r="E93" s="0" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="F93" s="0" t="n">
+        <v>0.124</v>
+      </c>
+      <c r="G93" s="0" t="n">
+        <v>0.66</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2245,7 +2355,7 @@
         <v>1.13708526519229</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D94" s="0" t="n">
         <v>13</v>
@@ -2259,7 +2369,7 @@
         <v>0.00657401455755455</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D95" s="0" t="n">
         <v>14</v>
@@ -2273,7 +2383,7 @@
         <v>0.457935644905112</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D96" s="0" t="n">
         <v>15</v>
@@ -2287,7 +2397,7 @@
         <v>0.0299086467558126</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D97" s="0" t="n">
         <v>1</v>
@@ -2301,7 +2411,7 @@
         <v>1.35138015113964</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D98" s="0" t="n">
         <v>2</v>
@@ -2315,7 +2425,7 @@
         <v>0.132421974305338</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D99" s="0" t="n">
         <v>3</v>
@@ -2329,7 +2439,7 @@
         <v>1.98269006319899</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D100" s="0" t="n">
         <v>4</v>
@@ -2343,7 +2453,7 @@
         <v>3.39161236924989</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D101" s="0" t="n">
         <v>5</v>
@@ -2357,7 +2467,7 @@
         <v>0.0017523256961147</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D102" s="0" t="n">
         <v>6</v>
@@ -2371,7 +2481,7 @@
         <v>0.448429759066528</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D103" s="0" t="n">
         <v>7</v>
@@ -2385,7 +2495,7 @@
         <v>0.00467719681179643</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D104" s="0" t="n">
         <v>8</v>
@@ -2399,7 +2509,7 @@
         <v>0.0496849799771728</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D105" s="0" t="n">
         <v>9</v>
@@ -2413,7 +2523,7 @@
         <v>0.00730849961283516</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D106" s="0" t="n">
         <v>10</v>
@@ -2427,7 +2537,7 @@
         <v>0.357772344667488</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D107" s="0" t="n">
         <v>11</v>
@@ -2441,7 +2551,7 @@
         <v>1.78066366225851</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D108" s="0" t="n">
         <v>12</v>
@@ -2455,7 +2565,7 @@
         <v>0.510827647752</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D109" s="0" t="n">
         <v>13</v>
@@ -2469,7 +2579,7 @@
         <v>0.00185294947891615</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D110" s="0" t="n">
         <v>14</v>
@@ -2483,7 +2593,7 @@
         <v>2.84541673997607</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D111" s="0" t="n">
         <v>15</v>
@@ -2499,7 +2609,7 @@
         <v>48</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2507,7 +2617,7 @@
         <v>3</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hyperparameter search and final results for experiment 2
</commit_message>
<xml_diff>
--- a/experiments/hyperparameters/hyperparemeter_search.xlsx
+++ b/experiments/hyperparameters/hyperparemeter_search.xlsx
@@ -514,8 +514,8 @@
   </sheetPr>
   <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B87" activeCellId="0" sqref="B87"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B95" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E123" activeCellId="0" sqref="E123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2951,6 +2951,15 @@
       <c r="D119" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E119" s="0" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="F119" s="0" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="G119" s="0" t="n">
+        <v>0.66</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="s">
@@ -3006,6 +3015,15 @@
       </c>
       <c r="D123" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="E123" s="0" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="F123" s="0" t="n">
+        <v>0.131</v>
+      </c>
+      <c r="G123" s="0" t="n">
+        <v>0.67</v>
       </c>
       <c r="I123" s="0" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
Added new hyperparameter search ranges
</commit_message>
<xml_diff>
--- a/experiments/hyperparameters/hyperparemeter_search.xlsx
+++ b/experiments/hyperparameters/hyperparemeter_search.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="349" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="174" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="160">
   <si>
     <t>EXPERIMENT 1</t>
   </si>
@@ -393,6 +393,108 @@
   </si>
   <si>
     <t>Network with 0.96/0.04 loss weights</t>
+  </si>
+  <si>
+    <t>EXPERIMENT 3</t>
+  </si>
+  <si>
+    <t>HYPERPARAMETER SEARCH 5</t>
+  </si>
+  <si>
+    <t>run85</t>
+  </si>
+  <si>
+    <t>run86</t>
+  </si>
+  <si>
+    <t>run87</t>
+  </si>
+  <si>
+    <t>run88</t>
+  </si>
+  <si>
+    <t>run89</t>
+  </si>
+  <si>
+    <t>run90</t>
+  </si>
+  <si>
+    <t>run91</t>
+  </si>
+  <si>
+    <t>run92</t>
+  </si>
+  <si>
+    <t>run93</t>
+  </si>
+  <si>
+    <t>run94</t>
+  </si>
+  <si>
+    <t>run95</t>
+  </si>
+  <si>
+    <t>run96</t>
+  </si>
+  <si>
+    <t>run97</t>
+  </si>
+  <si>
+    <t>run98</t>
+  </si>
+  <si>
+    <t>run99</t>
+  </si>
+  <si>
+    <t>run100</t>
+  </si>
+  <si>
+    <t>run101</t>
+  </si>
+  <si>
+    <t>run102</t>
+  </si>
+  <si>
+    <t>run103</t>
+  </si>
+  <si>
+    <t>run104</t>
+  </si>
+  <si>
+    <t>run105</t>
+  </si>
+  <si>
+    <t>run106</t>
+  </si>
+  <si>
+    <t>run107</t>
+  </si>
+  <si>
+    <t>run108</t>
+  </si>
+  <si>
+    <t>run109</t>
+  </si>
+  <si>
+    <t>run110</t>
+  </si>
+  <si>
+    <t>run111</t>
+  </si>
+  <si>
+    <t>run112</t>
+  </si>
+  <si>
+    <t>run113</t>
+  </si>
+  <si>
+    <t>run114</t>
+  </si>
+  <si>
+    <t>10 .^ unifrnd(-6,-2,30,1)</t>
+  </si>
+  <si>
+    <t>10 .^ unifrnd(-5, 0, 30, 1)</t>
   </si>
 </sst>
 </file>
@@ -512,10 +614,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I165"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B95" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E123" activeCellId="0" sqref="E123"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A110" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E155" activeCellId="0" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3029,8 +3131,557 @@
         <v>125</v>
       </c>
     </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="1"/>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B127" s="2"/>
+      <c r="C127" s="2"/>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
+      <c r="H127" s="2"/>
+      <c r="I127" s="2"/>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="4" t="n">
+        <v>1.5654E-006</v>
+      </c>
+      <c r="B129" s="4" t="n">
+        <v>0.26921</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D129" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E129" s="4"/>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="4" t="n">
+        <v>3.5554E-006</v>
+      </c>
+      <c r="B130" s="4" t="n">
+        <v>3.0387E-005</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="D130" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="4" t="n">
+        <v>1.1537E-005</v>
+      </c>
+      <c r="B131" s="4" t="n">
+        <v>0.2741</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="D131" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E131" s="4"/>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="4" t="n">
+        <v>1.1713E-005</v>
+      </c>
+      <c r="B132" s="4" t="n">
+        <v>0.00073872</v>
+      </c>
+      <c r="C132" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D132" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="4" t="n">
+        <v>1.3078E-005</v>
+      </c>
+      <c r="B133" s="4" t="n">
+        <v>5.5114E-005</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D133" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="4" t="n">
+        <v>1.6275E-005</v>
+      </c>
+      <c r="B134" s="4" t="n">
+        <v>7.581E-005</v>
+      </c>
+      <c r="C134" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D134" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="4" t="n">
+        <v>1.8201E-005</v>
+      </c>
+      <c r="B135" s="4" t="n">
+        <v>5.0484E-005</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D135" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="E135" s="4"/>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="4" t="n">
+        <v>2.0148E-005</v>
+      </c>
+      <c r="B136" s="4" t="n">
+        <v>0.0012329</v>
+      </c>
+      <c r="C136" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D136" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E136" s="4"/>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="4" t="n">
+        <v>2.2684E-005</v>
+      </c>
+      <c r="B137" s="4" t="n">
+        <v>0.0007946</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D137" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="4" t="n">
+        <v>3.361E-005</v>
+      </c>
+      <c r="B138" s="4" t="n">
+        <v>0.00052887</v>
+      </c>
+      <c r="C138" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D138" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="4" t="n">
+        <v>3.8006E-005</v>
+      </c>
+      <c r="B139" s="4" t="n">
+        <v>0.00048127</v>
+      </c>
+      <c r="C139" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="D139" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="4" t="n">
+        <v>4.0787E-005</v>
+      </c>
+      <c r="B140" s="4" t="n">
+        <v>0.001023</v>
+      </c>
+      <c r="C140" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="D140" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="4" t="n">
+        <v>4.1844E-005</v>
+      </c>
+      <c r="B141" s="4" t="n">
+        <v>0.00084802</v>
+      </c>
+      <c r="C141" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D141" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="4" t="n">
+        <v>6.5612E-005</v>
+      </c>
+      <c r="B142" s="4" t="n">
+        <v>0.003607</v>
+      </c>
+      <c r="C142" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D142" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="4" t="n">
+        <v>6.827E-005</v>
+      </c>
+      <c r="B143" s="4" t="n">
+        <v>0.18602</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="D143" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="4" t="n">
+        <v>0.00011998</v>
+      </c>
+      <c r="B144" s="4" t="n">
+        <v>0.045356</v>
+      </c>
+      <c r="C144" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="D144" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="4" t="n">
+        <v>0.000143</v>
+      </c>
+      <c r="B145" s="4" t="n">
+        <v>0.00028769</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="D145" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E145" s="4"/>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="4" t="n">
+        <v>0.00025927</v>
+      </c>
+      <c r="B146" s="4" t="n">
+        <v>0.00014377</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="D146" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="4" t="n">
+        <v>0.00037919</v>
+      </c>
+      <c r="B147" s="4" t="n">
+        <v>0.0029846</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D147" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E147" s="4"/>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="4" t="n">
+        <v>0.00039582</v>
+      </c>
+      <c r="B148" s="4" t="n">
+        <v>0.027861</v>
+      </c>
+      <c r="C148" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="D148" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E148" s="4"/>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="4" t="n">
+        <v>0.00055286</v>
+      </c>
+      <c r="B149" s="4" t="n">
+        <v>0.13127</v>
+      </c>
+      <c r="C149" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D149" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="4" t="n">
+        <v>0.0016262</v>
+      </c>
+      <c r="B150" s="4" t="n">
+        <v>2.8017E-005</v>
+      </c>
+      <c r="C150" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="D150" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="4" t="n">
+        <v>0.0016451</v>
+      </c>
+      <c r="B151" s="4" t="n">
+        <v>0.01021</v>
+      </c>
+      <c r="C151" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="D151" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E151" s="4"/>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="4" t="n">
+        <v>0.0018396</v>
+      </c>
+      <c r="B152" s="4" t="n">
+        <v>0.004497</v>
+      </c>
+      <c r="C152" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="D152" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="E152" s="4"/>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="4" t="n">
+        <v>0.0021531</v>
+      </c>
+      <c r="B153" s="4" t="n">
+        <v>0.0044713</v>
+      </c>
+      <c r="C153" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="D153" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="4" t="n">
+        <v>0.00378</v>
+      </c>
+      <c r="B154" s="4" t="n">
+        <v>0.19318</v>
+      </c>
+      <c r="C154" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D154" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="4" t="n">
+        <v>0.0037956</v>
+      </c>
+      <c r="B155" s="4" t="n">
+        <v>0.0014238</v>
+      </c>
+      <c r="C155" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D155" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="4" t="n">
+        <v>0.0044606</v>
+      </c>
+      <c r="B156" s="4" t="n">
+        <v>0.11008</v>
+      </c>
+      <c r="C156" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D156" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E156" s="4"/>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="4" t="n">
+        <v>0.0058469</v>
+      </c>
+      <c r="B157" s="4" t="n">
+        <v>9.3986E-005</v>
+      </c>
+      <c r="C157" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="D157" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E157" s="4"/>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="4" t="n">
+        <v>0.0094124</v>
+      </c>
+      <c r="B158" s="4" t="n">
+        <v>4.3753E-005</v>
+      </c>
+      <c r="C158" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D158" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B160" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B164" s="2"/>
+      <c r="C164" s="2"/>
+      <c r="D164" s="2"/>
+      <c r="E164" s="2"/>
+      <c r="F164" s="2"/>
+      <c r="G164" s="2"/>
+      <c r="H164" s="2"/>
+      <c r="I164" s="2"/>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G165" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H165" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I165" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A41:I41"/>
@@ -3040,6 +3691,9 @@
     <mergeCell ref="A80:I80"/>
     <mergeCell ref="A117:I117"/>
     <mergeCell ref="A121:I121"/>
+    <mergeCell ref="A126:I126"/>
+    <mergeCell ref="A127:I127"/>
+    <mergeCell ref="A164:I164"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Hyperparemeter search for Expeirment 3 done
</commit_message>
<xml_diff>
--- a/experiments/hyperparameters/hyperparemeter_search.xlsx
+++ b/experiments/hyperparameters/hyperparemeter_search.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="164">
   <si>
     <t>EXPERIMENT 1</t>
   </si>
@@ -482,6 +482,9 @@
     <t>run111</t>
   </si>
   <si>
+    <t>higher</t>
+  </si>
+  <si>
     <t>run112</t>
   </si>
   <si>
@@ -491,10 +494,19 @@
     <t>run114</t>
   </si>
   <si>
+    <t>Notes:</t>
+  </si>
+  <si>
     <t>10 .^ unifrnd(-6,-2,30,1)</t>
   </si>
   <si>
+    <t>For plots deleted points with 6 highest alphas or 6 highest lambdas (if repreated)</t>
+  </si>
+  <si>
     <t>10 .^ unifrnd(-5, 0, 30, 1)</t>
+  </si>
+  <si>
+    <t>run115</t>
   </si>
 </sst>
 </file>
@@ -614,10 +626,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I165"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A110" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E155" activeCellId="0" sqref="E155"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A131" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D166" activeCellId="0" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2874,7 +2886,7 @@
       <c r="D108" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="E108" s="4" t="n">
+      <c r="E108" s="0" t="n">
         <v>7.74</v>
       </c>
       <c r="F108" s="0" t="n">
@@ -3199,7 +3211,15 @@
       <c r="D129" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E129" s="4"/>
+      <c r="E129" s="0" t="n">
+        <v>0.059</v>
+      </c>
+      <c r="F129" s="0" t="n">
+        <v>0.055</v>
+      </c>
+      <c r="G129" s="0" t="n">
+        <v>0.52</v>
+      </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="4" t="n">
@@ -3214,6 +3234,15 @@
       <c r="D130" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="E130" s="0" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="F130" s="0" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="G130" s="0" t="n">
+        <v>0.89</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="4" t="n">
@@ -3228,7 +3257,15 @@
       <c r="D131" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E131" s="4"/>
+      <c r="E131" s="0" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="F131" s="0" t="n">
+        <v>0.107</v>
+      </c>
+      <c r="G131" s="0" t="n">
+        <v>0.45</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="4" t="n">
@@ -3243,6 +3280,15 @@
       <c r="D132" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="E132" s="0" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="F132" s="0" t="n">
+        <v>0.128</v>
+      </c>
+      <c r="G132" s="0" t="n">
+        <v>0.85</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="4" t="n">
@@ -3257,6 +3303,15 @@
       <c r="D133" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="E133" s="0" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="F133" s="0" t="n">
+        <v>0.129</v>
+      </c>
+      <c r="G133" s="0" t="n">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="4" t="n">
@@ -3271,6 +3326,15 @@
       <c r="D134" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="E134" s="0" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="F134" s="0" t="n">
+        <v>0.129</v>
+      </c>
+      <c r="G134" s="0" t="n">
+        <v>0.88</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="4" t="n">
@@ -3285,7 +3349,15 @@
       <c r="D135" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="E135" s="4"/>
+      <c r="E135" s="0" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="F135" s="0" t="n">
+        <v>0.127</v>
+      </c>
+      <c r="G135" s="0" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="4" t="n">
@@ -3300,7 +3372,15 @@
       <c r="D136" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="E136" s="4"/>
+      <c r="E136" s="0" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="F136" s="0" t="n">
+        <v>0.126</v>
+      </c>
+      <c r="G136" s="0" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="4" t="n">
@@ -3315,6 +3395,15 @@
       <c r="D137" s="0" t="n">
         <v>9</v>
       </c>
+      <c r="E137" s="0" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="F137" s="0" t="n">
+        <v>0.124</v>
+      </c>
+      <c r="G137" s="0" t="n">
+        <v>0.77</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="4" t="n">
@@ -3329,6 +3418,15 @@
       <c r="D138" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="E138" s="0" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="F138" s="0" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="G138" s="0" t="n">
+        <v>0.71</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="4" t="n">
@@ -3343,6 +3441,15 @@
       <c r="D139" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="E139" s="0" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="F139" s="0" t="n">
+        <v>0.127</v>
+      </c>
+      <c r="G139" s="0" t="n">
+        <v>0.78</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="4" t="n">
@@ -3357,6 +3464,15 @@
       <c r="D140" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="E140" s="0" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="F140" s="0" t="n">
+        <v>0.128</v>
+      </c>
+      <c r="G140" s="0" t="n">
+        <v>0.74</v>
+      </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="4" t="n">
@@ -3371,6 +3487,15 @@
       <c r="D141" s="0" t="n">
         <v>13</v>
       </c>
+      <c r="E141" s="0" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="F141" s="0" t="n">
+        <v>0.123</v>
+      </c>
+      <c r="G141" s="0" t="n">
+        <v>0.63</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="4" t="n">
@@ -3385,6 +3510,15 @@
       <c r="D142" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="E142" s="0" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="F142" s="0" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="G142" s="0" t="n">
+        <v>0.71</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="4" t="n">
@@ -3399,6 +3533,18 @@
       <c r="D143" s="0" t="n">
         <v>15</v>
       </c>
+      <c r="E143" s="0" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="F143" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G143" s="0" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="I143" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="4" t="n">
@@ -3413,6 +3559,18 @@
       <c r="D144" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="E144" s="0" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="F144" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G144" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="I144" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="4" t="n">
@@ -3427,7 +3585,15 @@
       <c r="D145" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E145" s="4"/>
+      <c r="E145" s="0" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="F145" s="0" t="n">
+        <v>0.136</v>
+      </c>
+      <c r="G145" s="0" t="n">
+        <v>0.66</v>
+      </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="4" t="n">
@@ -3442,6 +3608,15 @@
       <c r="D146" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="E146" s="0" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="F146" s="0" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="G146" s="0" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="4" t="n">
@@ -3456,7 +3631,15 @@
       <c r="D147" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E147" s="4"/>
+      <c r="E147" s="0" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="F147" s="0" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="G147" s="0" t="n">
+        <v>0.52</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="4" t="n">
@@ -3471,7 +3654,18 @@
       <c r="D148" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="E148" s="4"/>
+      <c r="E148" s="0" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="F148" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G148" s="0" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="I148" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="4" t="n">
@@ -3486,6 +3680,18 @@
       <c r="D149" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="E149" s="0" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="F149" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G149" s="0" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="I149" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="4" t="n">
@@ -3500,6 +3706,15 @@
       <c r="D150" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="E150" s="0" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="F150" s="0" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="G150" s="0" t="n">
+        <v>0.11</v>
+      </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="4" t="n">
@@ -3514,7 +3729,18 @@
       <c r="D151" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="E151" s="4"/>
+      <c r="E151" s="0" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="F151" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G151" s="0" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="I151" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="4" t="n">
@@ -3529,7 +3755,15 @@
       <c r="D152" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="E152" s="4"/>
+      <c r="E152" s="0" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="F152" s="0" t="n">
+        <v>0.127</v>
+      </c>
+      <c r="G152" s="0" t="n">
+        <v>0.44</v>
+      </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="4" t="n">
@@ -3544,6 +3778,18 @@
       <c r="D153" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="E153" s="0" t="n">
+        <v>0.129</v>
+      </c>
+      <c r="F153" s="0" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="G153" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="I153" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="4" t="n">
@@ -3558,6 +3804,18 @@
       <c r="D154" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="E154" s="0" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="F154" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G154" s="0" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="I154" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="4" t="n">
@@ -3572,6 +3830,21 @@
       <c r="D155" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="E155" s="0" t="n">
+        <v>162.36</v>
+      </c>
+      <c r="F155" s="0" t="n">
+        <v>0.062</v>
+      </c>
+      <c r="G155" s="0" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="H155" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="I155" s="0" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="4" t="n">
@@ -3581,12 +3854,23 @@
         <v>0.11008</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D156" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="E156" s="4"/>
+      <c r="E156" s="0" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="F156" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G156" s="0" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="I156" s="0" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="4" t="n">
@@ -3596,12 +3880,26 @@
         <v>9.3986E-005</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D157" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="E157" s="4"/>
+      <c r="E157" s="0" t="n">
+        <v>2443.44</v>
+      </c>
+      <c r="F157" s="0" t="n">
+        <v>0.085</v>
+      </c>
+      <c r="G157" s="0" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="H157" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="I157" s="0" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="4" t="n">
@@ -3611,23 +3909,44 @@
         <v>4.3753E-005</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D158" s="0" t="n">
         <v>15</v>
+      </c>
+      <c r="E158" s="0" t="n">
+        <v>174586</v>
+      </c>
+      <c r="F158" s="0" t="n">
+        <v>0.058</v>
+      </c>
+      <c r="G158" s="0" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="H158" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="I158" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B160" s="0" t="s">
         <v>46</v>
       </c>
+      <c r="G160" s="0" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
         <v>48</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
+      </c>
+      <c r="G161" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3635,7 +3954,7 @@
         <v>3</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3678,6 +3997,20 @@
       </c>
       <c r="I165" s="3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="n">
+        <v>4E-005</v>
+      </c>
+      <c r="B166" s="0" t="n">
+        <v>7E-005</v>
+      </c>
+      <c r="C166" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="D166" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated results from model_v3
</commit_message>
<xml_diff>
--- a/experiments/hyperparameters/hyperparemeter_search.xlsx
+++ b/experiments/hyperparameters/hyperparemeter_search.xlsx
@@ -629,7 +629,7 @@
   <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A131" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D166" activeCellId="0" sqref="D166"/>
+      <selection pane="topLeft" activeCell="F163" activeCellId="0" sqref="F163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4011,6 +4011,15 @@
       </c>
       <c r="D166" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="E166" s="0" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="F166" s="0" t="n">
+        <v>0.149</v>
+      </c>
+      <c r="G166" s="0" t="n">
+        <v>0.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New results for some hyperparameter search with fixed IOU
</commit_message>
<xml_diff>
--- a/experiments/hyperparameters/hyperparemeter_search.xlsx
+++ b/experiments/hyperparameters/hyperparemeter_search.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="174" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="348" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="161">
   <si>
     <t>EXPERIMENT 1</t>
   </si>
@@ -44,7 +44,10 @@
     <t>Best Threshold</t>
   </si>
   <si>
-    <t>Threshold selection</t>
+    <t>IOU2</t>
+  </si>
+  <si>
+    <t>Thresh2</t>
   </si>
   <si>
     <t>Notes</t>
@@ -53,18 +56,12 @@
     <t>run1</t>
   </si>
   <si>
-    <t>Higher</t>
-  </si>
-  <si>
     <t>run2</t>
   </si>
   <si>
     <t>run3</t>
   </si>
   <si>
-    <t>Only one</t>
-  </si>
-  <si>
     <t>run4</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>run17</t>
   </si>
   <si>
-    <t>Lower</t>
-  </si>
-  <si>
     <t>run18</t>
   </si>
   <si>
@@ -140,9 +134,6 @@
     <t>run26</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>run27</t>
   </si>
   <si>
@@ -167,7 +158,7 @@
     <t>10 .^ unifrnd(-6,0,30,1)</t>
   </si>
   <si>
-    <t>IOU 0.01514 is the product of predicting the entire image as 1 (low threshold)</t>
+    <t>IOU 0.015  is the product of predicting the entire image as 1 (low threshold)</t>
   </si>
   <si>
     <t>10 .^ unifrnd(-3, 3, 30, 1)</t>
@@ -179,51 +170,51 @@
     <t>HYPERPARAMETER SEARCH 2</t>
   </si>
   <si>
+    <t>run31</t>
+  </si>
+  <si>
+    <t>run32</t>
+  </si>
+  <si>
+    <t>run33</t>
+  </si>
+  <si>
+    <t>run34</t>
+  </si>
+  <si>
+    <t>run35</t>
+  </si>
+  <si>
+    <t>run36</t>
+  </si>
+  <si>
+    <t>run37</t>
+  </si>
+  <si>
+    <t>run38</t>
+  </si>
+  <si>
+    <t>run39</t>
+  </si>
+  <si>
+    <t>run40</t>
+  </si>
+  <si>
+    <t>run41</t>
+  </si>
+  <si>
+    <t>run42</t>
+  </si>
+  <si>
     <t>run43</t>
   </si>
   <si>
     <t>run44</t>
   </si>
   <si>
-    <t>run32</t>
-  </si>
-  <si>
-    <t>run33</t>
-  </si>
-  <si>
-    <t>run34</t>
-  </si>
-  <si>
-    <t>run36</t>
-  </si>
-  <si>
     <t>run45</t>
   </si>
   <si>
-    <t>run35</t>
-  </si>
-  <si>
-    <t>run41</t>
-  </si>
-  <si>
-    <t>run42</t>
-  </si>
-  <si>
-    <t>run40</t>
-  </si>
-  <si>
-    <t>run38</t>
-  </si>
-  <si>
-    <t>run39</t>
-  </si>
-  <si>
-    <t>run31</t>
-  </si>
-  <si>
-    <t>run37</t>
-  </si>
-  <si>
     <t>10 .^ unifrnd(-6,-4,15,1)</t>
   </si>
   <si>
@@ -386,6 +377,9 @@
     <t>run83</t>
   </si>
   <si>
+    <t>run116</t>
+  </si>
+  <si>
     <t>EXPERIMENT 2.5</t>
   </si>
   <si>
@@ -480,9 +474,6 @@
   </si>
   <si>
     <t>run111</t>
-  </si>
-  <si>
-    <t>higher</t>
   </si>
   <si>
     <t>run112</t>
@@ -626,10 +617,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:J167"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A131" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F163" activeCellId="0" sqref="F163"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I53" activeCellId="0" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -641,8 +632,9 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.02551020408163"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.030612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.49489795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.18877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -657,6 +649,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -670,6 +663,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -699,6 +693,9 @@
       <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="J3" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
@@ -708,7 +705,7 @@
         <v>19.8148065443621</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -717,13 +714,16 @@
         <v>0.403</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>0.0151</v>
+        <v>0.015</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>12</v>
+        <v>0.04</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.04</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -743,13 +743,16 @@
         <v>0.503</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0.0151</v>
+        <v>0.015</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>12</v>
+        <v>0.25</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -769,13 +772,16 @@
         <v>0.226</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>0.0328</v>
+        <v>0.073</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>15</v>
+        <v>0.25</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -786,7 +792,7 @@
         <v>20.109230821923</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>4</v>
@@ -795,13 +801,16 @@
         <v>0.527</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>0.0151</v>
+        <v>0.015</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>12</v>
+        <v>0.38</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.38</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,7 +821,7 @@
         <v>0.0342846451308202</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>5</v>
@@ -821,13 +830,16 @@
         <v>0.238</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>0.0802</v>
+        <v>0.13</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>15</v>
+        <v>0.46</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.194</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,7 +850,7 @@
         <v>0.003815984082409</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>6</v>
@@ -847,13 +859,16 @@
         <v>0.204</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>0.0963</v>
+        <v>0.17</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>15</v>
+        <v>0.42</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0.223</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -864,7 +879,7 @@
         <v>1.04676418044599</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>7</v>
@@ -873,13 +888,16 @@
         <v>0.183</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>0.0151</v>
+        <v>0.019</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>12</v>
+        <v>0.13</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -890,7 +908,7 @@
         <v>2.21182387803038</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>8</v>
@@ -899,13 +917,16 @@
         <v>0.146</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>0.0151</v>
+        <v>0.015</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>12</v>
+        <v>0.08</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0.08</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -916,7 +937,7 @@
         <v>0.127485643480525</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>9</v>
@@ -925,13 +946,16 @@
         <v>0.108</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>0.0353</v>
+        <v>0.085</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>15</v>
+        <v>0.13</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0.154</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>0.13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -942,7 +966,7 @@
         <v>114.536998751119</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>10</v>
@@ -951,13 +975,16 @@
         <v>0.232</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>0.0151</v>
+        <v>0.015</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>12</v>
+        <v>0.17</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0.17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,7 +995,7 @@
         <v>0.00349680934648399</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>11</v>
@@ -977,13 +1004,16 @@
         <v>0.083</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>0.0894</v>
+        <v>0.145</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>15</v>
+        <v>0.13</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0.208</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>0.13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -994,7 +1024,7 @@
         <v>0.0407721285113296</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>12</v>
@@ -1003,13 +1033,16 @@
         <v>0.086</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>0.0367</v>
+        <v>0.015</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>0.003</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1020,7 +1053,7 @@
         <v>654.557000601105</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>13</v>
@@ -1029,13 +1062,16 @@
         <v>0.082</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>0.0151</v>
+        <v>0.015</v>
       </c>
       <c r="G16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="n">
         <v>0.03</v>
       </c>
-      <c r="H16" s="0" t="s">
-        <v>12</v>
+      <c r="I16" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,7 +1082,7 @@
         <v>0.18852187448211</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>14</v>
@@ -1055,13 +1091,16 @@
         <v>0.085</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>0.0151</v>
+        <v>0.015</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,7 +1111,7 @@
         <v>172.280303410619</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>15</v>
@@ -1081,13 +1120,16 @@
         <v>0.079</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>0.0151</v>
+        <v>0.015</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,7 +1140,7 @@
         <v>672.610866152973</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1</v>
@@ -1107,13 +1149,16 @@
         <v>0.079</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>0.0151</v>
+        <v>0.015</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>0.008</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1124,7 +1169,7 @@
         <v>0.00534800269057661</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>2</v>
@@ -1136,10 +1181,13 @@
         <v>0</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1150,7 +1198,7 @@
         <v>0.0135922640948401</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>3</v>
@@ -1162,10 +1210,13 @@
         <v>0</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1176,7 +1227,7 @@
         <v>24.3237350489964</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>4</v>
@@ -1185,13 +1236,16 @@
         <v>0.079</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>0.0151</v>
+        <v>0.015</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1202,7 +1256,7 @@
         <v>30.065592432435</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>5</v>
@@ -1211,13 +1265,16 @@
         <v>0.079</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>0.0151</v>
+        <v>0.015</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1228,7 +1285,7 @@
         <v>13.9224313158425</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>6</v>
@@ -1240,10 +1297,13 @@
         <v>0</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1254,7 +1314,7 @@
         <v>0.441615630387425</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>7</v>
@@ -1263,13 +1323,16 @@
         <v>200000000000</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>0.0019</v>
+        <v>0.001</v>
       </c>
       <c r="G25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="H25" s="0" t="s">
-        <v>30</v>
+      <c r="I25" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1280,7 +1343,7 @@
         <v>362.340173120484</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>8</v>
@@ -1289,13 +1352,16 @@
         <v>0.08</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>0.0151</v>
+        <v>0.015</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1306,7 +1372,7 @@
         <v>0.158705081874316</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>9</v>
@@ -1318,13 +1384,16 @@
         <v>0</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1335,7 +1404,7 @@
         <v>236.980250861124</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>10</v>
@@ -1347,13 +1416,16 @@
         <v>0</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,7 +1436,7 @@
         <v>0.316073030698462</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>11</v>
@@ -1373,13 +1445,19 @@
         <v>200000000000</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>0.0168</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>38</v>
+        <v>0.017</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1390,13 +1468,13 @@
         <v>9.63696692139679</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I30" s="0" t="s">
-        <v>38</v>
+      <c r="J30" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1407,13 +1485,13 @@
         <v>0.225266479037908</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="I31" s="0" t="s">
-        <v>38</v>
+      <c r="J31" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1424,13 +1502,13 @@
         <v>37.3747733037578</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="I32" s="0" t="s">
-        <v>38</v>
+      <c r="J32" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1441,32 +1519,32 @@
         <v>181.737298056476</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="I33" s="0" t="s">
-        <v>38</v>
+      <c r="J33" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,15 +1552,15 @@
         <v>3</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1492,6 +1570,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
@@ -1521,120 +1600,153 @@
       <c r="I42" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="J42" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="n">
-        <v>1.95353806753189E-005</v>
+        <v>1.03832710303222E-006</v>
       </c>
       <c r="B43" s="4" t="n">
-        <v>0.0329270563182907</v>
+        <v>0.00300829771122991</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>0.196</v>
+        <v>0.466</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>0.077</v>
+        <v>0.318</v>
       </c>
       <c r="G43" s="0" t="n">
-        <v>0.28</v>
+        <v>0.96</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <v>0.363</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>0.92</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="n">
-        <v>5.74635755817239E-005</v>
+        <v>1.10610306438123E-006</v>
       </c>
       <c r="B44" s="4" t="n">
-        <v>0.00443696160874432</v>
+        <v>0.000338909715960258</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E44" s="0" t="n">
-        <v>0.212</v>
+        <v>0.308</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>0.084</v>
+        <v>0.219</v>
       </c>
       <c r="G44" s="0" t="n">
-        <v>0.31</v>
+        <v>0.62</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>0.276</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>0.62</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="n">
-        <v>1.10610306438123E-006</v>
+        <v>1.4231564382078E-006</v>
       </c>
       <c r="B45" s="4" t="n">
-        <v>0.000338909715960258</v>
+        <v>0.00214765374049253</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E45" s="0" t="n">
-        <v>0.308</v>
+        <v>0.278</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>0.099</v>
+        <v>0.182</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>0.56</v>
+        <v>0.62</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>0.242</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>0.62</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="n">
-        <v>1.4231564382078E-006</v>
+        <v>1.54208600071874E-006</v>
       </c>
       <c r="B46" s="4" t="n">
-        <v>0.00214765374049253</v>
+        <v>0.00217747613620058</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>0.278</v>
+        <v>0.206</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>0.101</v>
+        <v>0.227</v>
       </c>
       <c r="G46" s="0" t="n">
-        <v>0.57</v>
+        <v>0.67</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>0.62</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="n">
-        <v>1.54208600071874E-006</v>
+        <v>1.82479140350789E-006</v>
       </c>
       <c r="B47" s="4" t="n">
-        <v>0.00217747613620058</v>
+        <v>0.0377388545111771</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E47" s="0" t="n">
-        <v>0.206</v>
+        <v>0.331</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>0.108</v>
+        <v>0.246</v>
       </c>
       <c r="G47" s="0" t="n">
-        <v>0.53</v>
+        <v>0.62</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <v>0.317</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>0.62</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1645,7 +1757,7 @@
         <v>0.0127298747056998</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>16</v>
@@ -1654,236 +1766,236 @@
         <v>0.226</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>0.114</v>
+        <v>0.262</v>
       </c>
       <c r="G48" s="0" t="n">
-        <v>0.63</v>
+        <v>0.75</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <v>0.301</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <v>0.71</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="n">
-        <v>7.01978251545733E-005</v>
+        <v>2.22305235306986E-006</v>
       </c>
       <c r="B49" s="4" t="n">
-        <v>1.16151961891159E-005</v>
+        <v>0.000542096462785538</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>0.08</v>
+        <v>0.334</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>0.115</v>
+        <v>0.292</v>
       </c>
       <c r="G49" s="0" t="n">
-        <v>0.28</v>
+        <v>0.79</v>
+      </c>
+      <c r="H49" s="0" t="n">
+        <v>0.362</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>0.79</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="n">
-        <v>1.82479140350789E-006</v>
+        <v>3.14614768104022E-006</v>
       </c>
       <c r="B50" s="4" t="n">
-        <v>0.0377388545111771</v>
+        <v>0.000431893750100302</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E50" s="0" t="n">
-        <v>0.331</v>
+        <v>0.313</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>0.117</v>
+        <v>0.275</v>
       </c>
       <c r="G50" s="0" t="n">
-        <v>0.59</v>
+        <v>0.71</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>0.71</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="n">
-        <v>1.03198644329961E-005</v>
+        <v>3.57454702108591E-006</v>
       </c>
       <c r="B51" s="4" t="n">
-        <v>7.40077844834827E-005</v>
+        <v>0.0388487377964991</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E51" s="0" t="n">
-        <v>0.242</v>
+        <v>0.355</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>0.117</v>
+        <v>0.266</v>
       </c>
       <c r="G51" s="0" t="n">
-        <v>0.5</v>
+        <v>0.71</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <v>0.351</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <v>0.71</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="n">
-        <v>1.2500112144408E-005</v>
+        <v>7.23258635944392E-006</v>
       </c>
       <c r="B52" s="4" t="n">
-        <v>1.81927676909693E-005</v>
+        <v>0.00500777479484594</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E52" s="0" t="n">
-        <v>0.209</v>
+        <v>0.294</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>0.117</v>
+        <v>0.283</v>
       </c>
       <c r="G52" s="0" t="n">
-        <v>0.54</v>
+        <v>0.62</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <v>0.343</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>0.62</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="n">
-        <v>7.23258635944392E-006</v>
+        <v>1.03198644329961E-005</v>
       </c>
       <c r="B53" s="4" t="n">
-        <v>0.00500777479484594</v>
+        <v>7.40077844834827E-005</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E53" s="0" t="n">
-        <v>0.294</v>
-      </c>
-      <c r="F53" s="0" t="n">
-        <v>0.118</v>
-      </c>
-      <c r="G53" s="0" t="n">
-        <v>0.58</v>
+        <v>0.242</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="n">
-        <v>3.14614768104022E-006</v>
+        <v>1.2500112144408E-005</v>
       </c>
       <c r="B54" s="4" t="n">
-        <v>0.000431893750100302</v>
+        <v>1.81927676909693E-005</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E54" s="0" t="n">
-        <v>0.313</v>
-      </c>
-      <c r="F54" s="0" t="n">
-        <v>0.119</v>
-      </c>
-      <c r="G54" s="0" t="n">
-        <v>0.63</v>
+        <v>0.209</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="n">
-        <v>3.57454702108591E-006</v>
+        <v>1.95353806753189E-005</v>
       </c>
       <c r="B55" s="4" t="n">
-        <v>0.0388487377964991</v>
+        <v>0.0329270563182907</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E55" s="0" t="n">
-        <v>0.355</v>
-      </c>
-      <c r="F55" s="0" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="G55" s="0" t="n">
-        <v>0.67</v>
+        <v>0.196</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="n">
-        <v>1.03832710303222E-006</v>
+        <v>5.74635755817239E-005</v>
       </c>
       <c r="B56" s="4" t="n">
-        <v>0.00300829771122991</v>
+        <v>0.00443696160874432</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E56" s="0" t="n">
-        <v>0.466</v>
-      </c>
-      <c r="F56" s="0" t="n">
-        <v>0.124</v>
-      </c>
-      <c r="G56" s="0" t="n">
-        <v>0.92</v>
+        <v>0.212</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="n">
-        <v>2.22305235306986E-006</v>
+        <v>7.01978251545733E-005</v>
       </c>
       <c r="B57" s="4" t="n">
-        <v>0.000542096462785538</v>
+        <v>1.16151961891159E-005</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>0.334</v>
-      </c>
-      <c r="F57" s="0" t="n">
-        <v>0.124</v>
-      </c>
-      <c r="G57" s="0" t="n">
-        <v>0.73</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1891,12 +2003,12 @@
         <v>3</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -1906,6 +2018,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
@@ -1935,6 +2048,9 @@
       <c r="I65" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="J65" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
@@ -1944,7 +2060,7 @@
         <v>0.01</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>3</v>
@@ -1958,8 +2074,8 @@
       <c r="G66" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I66" s="0" t="s">
-        <v>74</v>
+      <c r="J66" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1970,7 +2086,7 @@
         <v>0</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>1</v>
@@ -1993,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>1</v>
@@ -2016,7 +2132,7 @@
         <v>0</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>2</v>
@@ -2039,7 +2155,7 @@
         <v>0</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>1</v>
@@ -2062,7 +2178,7 @@
         <v>0</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>3</v>
@@ -2076,13 +2192,13 @@
       <c r="G71" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I71" s="0" t="s">
-        <v>80</v>
+      <c r="J71" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2092,6 +2208,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
@@ -2115,11 +2232,10 @@
       <c r="G74" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H74" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I74" s="3" t="s">
-        <v>10</v>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2130,7 +2246,7 @@
         <v>0.0008</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D75" s="0" t="n">
         <v>1</v>
@@ -2144,13 +2260,13 @@
       <c r="G75" s="0" t="n">
         <v>0.8</v>
       </c>
-      <c r="I75" s="0" t="s">
-        <v>83</v>
+      <c r="J75" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2160,10 +2276,11 @@
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2173,6 +2290,7 @@
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
@@ -2202,6 +2320,9 @@
       <c r="I81" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="J81" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="n">
@@ -2211,7 +2332,7 @@
         <v>0.000153030184042259</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>1</v>
@@ -2220,10 +2341,16 @@
         <v>0.047</v>
       </c>
       <c r="F82" s="0" t="n">
-        <v>0.119</v>
+        <v>0.262</v>
       </c>
       <c r="G82" s="0" t="n">
-        <v>0.84</v>
+        <v>0.92</v>
+      </c>
+      <c r="H82" s="0" t="n">
+        <v>0.338</v>
+      </c>
+      <c r="I82" s="0" t="n">
+        <v>0.87</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,7 +2361,7 @@
         <v>0.613281671174882</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>2</v>
@@ -2243,10 +2370,16 @@
         <v>0.06</v>
       </c>
       <c r="F83" s="0" t="n">
-        <v>0.111</v>
+        <v>0.25</v>
       </c>
       <c r="G83" s="0" t="n">
-        <v>0.78</v>
+        <v>0.83</v>
+      </c>
+      <c r="H83" s="0" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="I83" s="0" t="n">
+        <v>0.79</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2257,7 +2390,7 @@
         <v>0.00083424047044789</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>3</v>
@@ -2266,10 +2399,16 @@
         <v>0.043</v>
       </c>
       <c r="F84" s="0" t="n">
-        <v>0.119</v>
+        <v>0.266</v>
       </c>
       <c r="G84" s="0" t="n">
-        <v>0.74</v>
+        <v>0.79</v>
+      </c>
+      <c r="H84" s="0" t="n">
+        <v>0.343</v>
+      </c>
+      <c r="I84" s="0" t="n">
+        <v>0.79</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2280,7 +2419,7 @@
         <v>0.00145975149652255</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>4</v>
@@ -2289,9 +2428,15 @@
         <v>0.039</v>
       </c>
       <c r="F85" s="0" t="n">
-        <v>0.125</v>
+        <v>0.319</v>
       </c>
       <c r="G85" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H85" s="0" t="n">
+        <v>0.364</v>
+      </c>
+      <c r="I85" s="0" t="n">
         <v>0.71</v>
       </c>
     </row>
@@ -2303,7 +2448,7 @@
         <v>0.00214462479812596</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D86" s="0" t="n">
         <v>5</v>
@@ -2312,10 +2457,16 @@
         <v>0.043</v>
       </c>
       <c r="F86" s="0" t="n">
-        <v>0.125</v>
+        <v>0.296</v>
       </c>
       <c r="G86" s="0" t="n">
-        <v>0.68</v>
+        <v>0.75</v>
+      </c>
+      <c r="H86" s="0" t="n">
+        <v>0.362</v>
+      </c>
+      <c r="I86" s="0" t="n">
+        <v>0.71</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2326,7 +2477,7 @@
         <v>0.00204027518128024</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D87" s="0" t="n">
         <v>6</v>
@@ -2335,9 +2486,15 @@
         <v>0.043</v>
       </c>
       <c r="F87" s="0" t="n">
-        <v>0.133</v>
+        <v>0.312</v>
       </c>
       <c r="G87" s="0" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="H87" s="0" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="I87" s="0" t="n">
         <v>0.58</v>
       </c>
     </row>
@@ -2349,7 +2506,7 @@
         <v>2.2261234522861</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D88" s="0" t="n">
         <v>7</v>
@@ -2361,13 +2518,16 @@
         <v>0.015</v>
       </c>
       <c r="G88" s="0" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="H88" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I88" s="0" t="s">
-        <v>93</v>
+        <v>0.42</v>
+      </c>
+      <c r="H88" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I88" s="0" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="J88" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2378,7 +2538,7 @@
         <v>0.00363581666441528</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>8</v>
@@ -2387,9 +2547,15 @@
         <v>0.038</v>
       </c>
       <c r="F89" s="0" t="n">
-        <v>0.122</v>
+        <v>0.221</v>
       </c>
       <c r="G89" s="0" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="H89" s="0" t="n">
+        <v>0.309</v>
+      </c>
+      <c r="I89" s="0" t="n">
         <v>0.54</v>
       </c>
     </row>
@@ -2401,7 +2567,7 @@
         <v>0.385037978791714</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>9</v>
@@ -2413,13 +2579,16 @@
         <v>0.015</v>
       </c>
       <c r="G90" s="0" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="H90" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I90" s="0" t="s">
-        <v>93</v>
+        <v>0.21</v>
+      </c>
+      <c r="H90" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I90" s="0" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="J90" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2430,7 +2599,7 @@
         <v>0.046693736064734</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D91" s="0" t="n">
         <v>10</v>
@@ -2442,10 +2611,16 @@
         <v>0.015</v>
       </c>
       <c r="G91" s="0" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="I91" s="0" t="s">
-        <v>93</v>
+        <v>0.08</v>
+      </c>
+      <c r="H91" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I91" s="0" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="J91" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2456,7 +2631,7 @@
         <v>0.162706410105612</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D92" s="0" t="n">
         <v>11</v>
@@ -2470,8 +2645,14 @@
       <c r="G92" s="0" t="n">
         <v>0.25</v>
       </c>
-      <c r="I92" s="0" t="s">
-        <v>93</v>
+      <c r="H92" s="0" t="n">
+        <v>0.034</v>
+      </c>
+      <c r="I92" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="J92" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2482,7 +2663,7 @@
         <v>0.000189095715104318</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D93" s="0" t="n">
         <v>12</v>
@@ -2491,10 +2672,16 @@
         <v>0.022</v>
       </c>
       <c r="F93" s="0" t="n">
-        <v>0.124</v>
+        <v>0.285</v>
       </c>
       <c r="G93" s="0" t="n">
-        <v>0.66</v>
+        <v>0.79</v>
+      </c>
+      <c r="H93" s="0" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="I93" s="0" t="n">
+        <v>0.79</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2505,7 +2692,7 @@
         <v>1.13708526519229</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D94" s="0" t="n">
         <v>13</v>
@@ -2517,10 +2704,16 @@
         <v>0.015</v>
       </c>
       <c r="G94" s="0" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="I94" s="0" t="s">
-        <v>93</v>
+        <v>0.17</v>
+      </c>
+      <c r="H94" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I94" s="0" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="J94" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2531,7 +2724,7 @@
         <v>0.00657401455755455</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D95" s="0" t="n">
         <v>14</v>
@@ -2540,13 +2733,19 @@
         <v>0.049</v>
       </c>
       <c r="F95" s="0" t="n">
-        <v>0.018</v>
+        <v>0.116</v>
       </c>
       <c r="G95" s="0" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="I95" s="0" t="s">
-        <v>93</v>
+        <v>0.38</v>
+      </c>
+      <c r="H95" s="0" t="n">
+        <v>0.203</v>
+      </c>
+      <c r="I95" s="0" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="J95" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2557,7 +2756,7 @@
         <v>0.457935644905112</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D96" s="0" t="n">
         <v>15</v>
@@ -2569,10 +2768,16 @@
         <v>0.015</v>
       </c>
       <c r="G96" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="I96" s="0" t="s">
-        <v>93</v>
+        <v>0.17</v>
+      </c>
+      <c r="H96" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I96" s="0" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="J96" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2583,7 +2788,7 @@
         <v>0.0299086467558126</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D97" s="0" t="n">
         <v>1</v>
@@ -2595,10 +2800,16 @@
         <v>0.015</v>
       </c>
       <c r="G97" s="0" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="I97" s="0" t="s">
-        <v>93</v>
+        <v>0.25</v>
+      </c>
+      <c r="H97" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I97" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="J97" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2609,7 +2820,7 @@
         <v>1.35138015113964</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D98" s="0" t="n">
         <v>2</v>
@@ -2621,10 +2832,16 @@
         <v>0.015</v>
       </c>
       <c r="G98" s="0" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="I98" s="0" t="s">
-        <v>93</v>
+        <v>0.08</v>
+      </c>
+      <c r="H98" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I98" s="0" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="J98" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2635,7 +2852,7 @@
         <v>0.132421974305338</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D99" s="0" t="n">
         <v>3</v>
@@ -2644,16 +2861,19 @@
         <v>380000000</v>
       </c>
       <c r="F99" s="0" t="n">
-        <v>0.018</v>
+        <v>0.014</v>
       </c>
       <c r="G99" s="0" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H99" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I99" s="0" t="s">
-        <v>105</v>
+        <v>1</v>
+      </c>
+      <c r="H99" s="0" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="I99" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J99" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,7 +2884,7 @@
         <v>1.98269006319899</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D100" s="0" t="n">
         <v>4</v>
@@ -2673,13 +2893,19 @@
         <v>0.042</v>
       </c>
       <c r="F100" s="0" t="n">
-        <v>0.017</v>
+        <v>0.015</v>
       </c>
       <c r="G100" s="0" t="n">
         <v>0.13</v>
       </c>
-      <c r="I100" s="0" t="s">
-        <v>93</v>
+      <c r="H100" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I100" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="J100" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2690,7 +2916,7 @@
         <v>3.39161236924989</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D101" s="0" t="n">
         <v>5</v>
@@ -2702,10 +2928,16 @@
         <v>0.015</v>
       </c>
       <c r="G101" s="0" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="I101" s="0" t="s">
-        <v>93</v>
+        <v>0.08</v>
+      </c>
+      <c r="H101" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I101" s="0" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="J101" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2716,7 +2948,7 @@
         <v>0.0017523256961147</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D102" s="0" t="n">
         <v>6</v>
@@ -2725,13 +2957,19 @@
         <v>43400000000</v>
       </c>
       <c r="F102" s="0" t="n">
-        <v>0.015</v>
+        <v>0.005</v>
       </c>
       <c r="G102" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I102" s="0" t="s">
-        <v>105</v>
+        <v>1</v>
+      </c>
+      <c r="H102" s="0" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="I102" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J102" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,7 +2980,7 @@
         <v>0.448429759066528</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D103" s="0" t="n">
         <v>7</v>
@@ -2751,16 +2989,19 @@
         <v>1930000000</v>
       </c>
       <c r="F103" s="0" t="n">
-        <v>0.023</v>
+        <v>0.016</v>
       </c>
       <c r="G103" s="0" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H103" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I103" s="0" t="s">
-        <v>105</v>
+        <v>1</v>
+      </c>
+      <c r="H103" s="0" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="I103" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J103" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2771,7 +3012,7 @@
         <v>0.00467719681179643</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D104" s="0" t="n">
         <v>8</v>
@@ -2780,16 +3021,19 @@
         <v>636000000000</v>
       </c>
       <c r="F104" s="0" t="n">
-        <v>0.035</v>
+        <v>0.032</v>
       </c>
       <c r="G104" s="0" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H104" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I104" s="0" t="s">
-        <v>38</v>
+        <v>1</v>
+      </c>
+      <c r="H104" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="I104" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J104" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2800,7 +3044,7 @@
         <v>0.0496849799771728</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D105" s="0" t="n">
         <v>9</v>
@@ -2809,13 +3053,19 @@
         <v>18400000000000</v>
       </c>
       <c r="F105" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H105" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I105" s="0" t="s">
-        <v>38</v>
+        <v>0.015</v>
+      </c>
+      <c r="G105" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H105" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I105" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J105" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2826,7 +3076,7 @@
         <v>0.00730849961283516</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D106" s="0" t="n">
         <v>10</v>
@@ -2835,16 +3085,19 @@
         <v>1040000000000</v>
       </c>
       <c r="F106" s="0" t="n">
-        <v>0.074</v>
+        <v>0.097</v>
       </c>
       <c r="G106" s="0" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H106" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I106" s="0" t="s">
-        <v>38</v>
+        <v>1</v>
+      </c>
+      <c r="H106" s="0" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="I106" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J106" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2855,7 +3108,7 @@
         <v>0.357772344667488</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D107" s="0" t="n">
         <v>11</v>
@@ -2864,13 +3117,19 @@
         <v>454000000000000</v>
       </c>
       <c r="F107" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H107" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I107" s="0" t="s">
-        <v>38</v>
+        <v>0.015</v>
+      </c>
+      <c r="G107" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H107" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I107" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J107" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2881,7 +3140,7 @@
         <v>1.78066366225851</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D108" s="0" t="n">
         <v>12</v>
@@ -2890,13 +3149,19 @@
         <v>7.74</v>
       </c>
       <c r="F108" s="0" t="n">
-        <v>0.015</v>
+        <v>0</v>
       </c>
       <c r="G108" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="I108" s="0" t="s">
-        <v>38</v>
+      <c r="H108" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J108" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2907,7 +3172,7 @@
         <v>0.510827647752</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D109" s="0" t="n">
         <v>1</v>
@@ -2919,13 +3184,16 @@
         <v>0.015</v>
       </c>
       <c r="G109" s="0" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H109" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="I109" s="0" t="s">
-        <v>38</v>
+        <v>1</v>
+      </c>
+      <c r="H109" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I109" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J109" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2936,7 +3204,7 @@
         <v>0.00185294947891615</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D110" s="0" t="n">
         <v>2</v>
@@ -2945,13 +3213,19 @@
         <v>1700000000000000</v>
       </c>
       <c r="F110" s="0" t="n">
-        <v>0.015</v>
+        <v>0.007</v>
       </c>
       <c r="G110" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I110" s="0" t="s">
-        <v>38</v>
+        <v>1</v>
+      </c>
+      <c r="H110" s="0" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="I110" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J110" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2962,7 +3236,7 @@
         <v>2.84541673997607</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D111" s="0" t="n">
         <v>3</v>
@@ -2971,32 +3245,35 @@
         <v>68200000000000</v>
       </c>
       <c r="F111" s="0" t="n">
-        <v>0.015</v>
+        <v>0</v>
       </c>
       <c r="G111" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H111" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I111" s="0" t="s">
-        <v>38</v>
+      <c r="H111" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J111" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="0" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G114" s="0" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3004,15 +3281,15 @@
         <v>3</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G115" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3022,6 +3299,7 @@
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
+      <c r="J117" s="2"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
@@ -3051,6 +3329,9 @@
       <c r="I118" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="J118" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
@@ -3060,7 +3341,7 @@
         <v>0.002</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D119" s="0" t="n">
         <v>1</v>
@@ -3069,973 +3350,839 @@
         <v>0.026</v>
       </c>
       <c r="F119" s="0" t="n">
-        <v>0.133</v>
+        <v>0.37</v>
       </c>
       <c r="G119" s="0" t="n">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="2" t="s">
+        <v>0.71</v>
+      </c>
+      <c r="H119" s="0" t="n">
+        <v>0.419</v>
+      </c>
+      <c r="I119" s="0" t="n">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="n">
+        <v>2E-005</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D120" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B122" s="2"/>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
+      <c r="J122" s="2"/>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H123" s="3"/>
+      <c r="I123" s="3"/>
+      <c r="J123" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="n">
+        <v>3E-005</v>
+      </c>
+      <c r="B124" s="0" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D124" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E124" s="0" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="F124" s="0" t="n">
+        <v>0.328</v>
+      </c>
+      <c r="G124" s="0" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="H124" s="0" t="n">
+        <v>0.382</v>
+      </c>
+      <c r="I124" s="0" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="J124" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
-      <c r="E121" s="2"/>
-      <c r="F121" s="2"/>
-      <c r="G121" s="2"/>
-      <c r="H121" s="2"/>
-      <c r="I121" s="2"/>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="3" t="s">
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B127" s="1"/>
+      <c r="C127" s="1"/>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+      <c r="F127" s="1"/>
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
+      <c r="I127" s="1"/>
+      <c r="J127" s="1"/>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B128" s="2"/>
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+      <c r="H128" s="2"/>
+      <c r="I128" s="2"/>
+      <c r="J128" s="2"/>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B129" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C122" s="3" t="s">
+      <c r="C129" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D122" s="3" t="s">
+      <c r="D129" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E122" s="3" t="s">
+      <c r="E129" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F122" s="3" t="s">
+      <c r="F129" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G122" s="3" t="s">
+      <c r="G129" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H122" s="3" t="s">
+      <c r="H129" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I122" s="3" t="s">
+      <c r="I129" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="n">
-        <v>3E-005</v>
-      </c>
-      <c r="B123" s="0" t="n">
-        <v>0.003</v>
-      </c>
-      <c r="C123" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="D123" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="E123" s="0" t="n">
-        <v>0.017</v>
-      </c>
-      <c r="F123" s="0" t="n">
-        <v>0.131</v>
-      </c>
-      <c r="G123" s="0" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="I123" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B126" s="1"/>
-      <c r="C126" s="1"/>
-      <c r="D126" s="1"/>
-      <c r="E126" s="1"/>
-      <c r="F126" s="1"/>
-      <c r="G126" s="1"/>
-      <c r="H126" s="1"/>
-      <c r="I126" s="1"/>
-    </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="2"/>
-      <c r="E127" s="2"/>
-      <c r="F127" s="2"/>
-      <c r="G127" s="2"/>
-      <c r="H127" s="2"/>
-      <c r="I127" s="2"/>
-    </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D128" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E128" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F128" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G128" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H128" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I128" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="4" t="n">
-        <v>1.5654E-006</v>
-      </c>
-      <c r="B129" s="4" t="n">
-        <v>0.26921</v>
-      </c>
-      <c r="C129" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="D129" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E129" s="0" t="n">
-        <v>0.059</v>
-      </c>
-      <c r="F129" s="0" t="n">
-        <v>0.055</v>
-      </c>
-      <c r="G129" s="0" t="n">
-        <v>0.52</v>
+      <c r="J129" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="4" t="n">
-        <v>3.5554E-006</v>
+        <v>1.5654E-006</v>
       </c>
       <c r="B130" s="4" t="n">
-        <v>3.0387E-005</v>
+        <v>0.26921</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D130" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E130" s="0" t="n">
-        <v>0.036</v>
+        <v>0.059</v>
       </c>
       <c r="F130" s="0" t="n">
-        <v>0.122</v>
+        <v>0.092</v>
       </c>
       <c r="G130" s="0" t="n">
-        <v>0.89</v>
+        <v>0.54</v>
+      </c>
+      <c r="H130" s="0" t="n">
+        <v>0.127</v>
+      </c>
+      <c r="I130" s="0" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="4" t="n">
-        <v>1.1537E-005</v>
+        <v>3.5554E-006</v>
       </c>
       <c r="B131" s="4" t="n">
-        <v>0.2741</v>
+        <v>3.0387E-005</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D131" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E131" s="0" t="n">
-        <v>0.04</v>
+        <v>0.036</v>
       </c>
       <c r="F131" s="0" t="n">
-        <v>0.107</v>
+        <v>0.315</v>
       </c>
       <c r="G131" s="0" t="n">
-        <v>0.45</v>
+        <v>0.96</v>
+      </c>
+      <c r="H131" s="0" t="n">
+        <v>0.362</v>
+      </c>
+      <c r="I131" s="0" t="n">
+        <v>0.96</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="4" t="n">
-        <v>1.1713E-005</v>
+        <v>1.1537E-005</v>
       </c>
       <c r="B132" s="4" t="n">
-        <v>0.00073872</v>
+        <v>0.2741</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D132" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E132" s="0" t="n">
-        <v>0.031</v>
-      </c>
-      <c r="F132" s="0" t="n">
-        <v>0.128</v>
-      </c>
-      <c r="G132" s="0" t="n">
-        <v>0.85</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="4" t="n">
-        <v>1.3078E-005</v>
+        <v>1.1713E-005</v>
       </c>
       <c r="B133" s="4" t="n">
-        <v>5.5114E-005</v>
+        <v>0.00073872</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D133" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E133" s="0" t="n">
-        <v>0.044</v>
-      </c>
-      <c r="F133" s="0" t="n">
-        <v>0.129</v>
-      </c>
-      <c r="G133" s="0" t="n">
-        <v>0.9</v>
+        <v>0.031</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="4" t="n">
-        <v>1.6275E-005</v>
+        <v>1.3078E-005</v>
       </c>
       <c r="B134" s="4" t="n">
-        <v>7.581E-005</v>
+        <v>5.5114E-005</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D134" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E134" s="0" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="F134" s="0" t="n">
-        <v>0.129</v>
-      </c>
-      <c r="G134" s="0" t="n">
-        <v>0.88</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="4" t="n">
-        <v>1.8201E-005</v>
+        <v>1.6275E-005</v>
       </c>
       <c r="B135" s="4" t="n">
-        <v>5.0484E-005</v>
+        <v>7.581E-005</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D135" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E135" s="0" t="n">
-        <v>0.028</v>
-      </c>
-      <c r="F135" s="0" t="n">
-        <v>0.127</v>
-      </c>
-      <c r="G135" s="0" t="n">
-        <v>0.75</v>
+        <v>0.032</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="4" t="n">
-        <v>2.0148E-005</v>
+        <v>1.8201E-005</v>
       </c>
       <c r="B136" s="4" t="n">
-        <v>0.0012329</v>
+        <v>5.0484E-005</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D136" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E136" s="0" t="n">
-        <v>0.026</v>
-      </c>
-      <c r="F136" s="0" t="n">
-        <v>0.126</v>
-      </c>
-      <c r="G136" s="0" t="n">
-        <v>0.75</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="4" t="n">
-        <v>2.2684E-005</v>
+        <v>2.0148E-005</v>
       </c>
       <c r="B137" s="4" t="n">
-        <v>0.0007946</v>
+        <v>0.0012329</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D137" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E137" s="0" t="n">
         <v>0.026</v>
       </c>
-      <c r="F137" s="0" t="n">
-        <v>0.124</v>
-      </c>
-      <c r="G137" s="0" t="n">
-        <v>0.77</v>
-      </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="4" t="n">
-        <v>3.361E-005</v>
+        <v>2.2684E-005</v>
       </c>
       <c r="B138" s="4" t="n">
-        <v>0.00052887</v>
+        <v>0.0007946</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D138" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E138" s="0" t="n">
         <v>0.026</v>
       </c>
-      <c r="F138" s="0" t="n">
-        <v>0.125</v>
-      </c>
-      <c r="G138" s="0" t="n">
-        <v>0.71</v>
-      </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="4" t="n">
-        <v>3.8006E-005</v>
+        <v>3.361E-005</v>
       </c>
       <c r="B139" s="4" t="n">
-        <v>0.00048127</v>
+        <v>0.00052887</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D139" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E139" s="0" t="n">
-        <v>0.027</v>
-      </c>
-      <c r="F139" s="0" t="n">
-        <v>0.127</v>
-      </c>
-      <c r="G139" s="0" t="n">
-        <v>0.78</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="4" t="n">
-        <v>4.0787E-005</v>
+        <v>3.8006E-005</v>
       </c>
       <c r="B140" s="4" t="n">
-        <v>0.001023</v>
+        <v>0.00048127</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D140" s="0" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E140" s="0" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="F140" s="0" t="n">
-        <v>0.128</v>
-      </c>
-      <c r="G140" s="0" t="n">
-        <v>0.74</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="4" t="n">
-        <v>4.1844E-005</v>
+        <v>4.0787E-005</v>
       </c>
       <c r="B141" s="4" t="n">
-        <v>0.00084802</v>
+        <v>0.001023</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D141" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E141" s="0" t="n">
-        <v>0.024</v>
-      </c>
-      <c r="F141" s="0" t="n">
-        <v>0.123</v>
-      </c>
-      <c r="G141" s="0" t="n">
-        <v>0.63</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="4" t="n">
-        <v>6.5612E-005</v>
+        <v>4.1844E-005</v>
       </c>
       <c r="B142" s="4" t="n">
-        <v>0.003607</v>
+        <v>0.00084802</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D142" s="0" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E142" s="0" t="n">
-        <v>0.023</v>
-      </c>
-      <c r="F142" s="0" t="n">
-        <v>0.122</v>
-      </c>
-      <c r="G142" s="0" t="n">
-        <v>0.71</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="4" t="n">
-        <v>6.827E-005</v>
+        <v>6.5612E-005</v>
       </c>
       <c r="B143" s="4" t="n">
-        <v>0.18602</v>
+        <v>0.003607</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D143" s="0" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E143" s="0" t="n">
-        <v>0.043</v>
-      </c>
-      <c r="F143" s="0" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="G143" s="0" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="I143" s="0" t="s">
-        <v>93</v>
+        <v>0.023</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="4" t="n">
-        <v>0.00011998</v>
+        <v>6.827E-005</v>
       </c>
       <c r="B144" s="4" t="n">
-        <v>0.045356</v>
+        <v>0.18602</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D144" s="0" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E144" s="0" t="n">
         <v>0.043</v>
       </c>
-      <c r="F144" s="0" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="G144" s="0" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="I144" s="0" t="s">
-        <v>93</v>
+      <c r="J144" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="4" t="n">
-        <v>0.000143</v>
+        <v>0.00011998</v>
       </c>
       <c r="B145" s="4" t="n">
-        <v>0.00028769</v>
+        <v>0.045356</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D145" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E145" s="0" t="n">
-        <v>0.022</v>
-      </c>
-      <c r="F145" s="0" t="n">
-        <v>0.136</v>
-      </c>
-      <c r="G145" s="0" t="n">
-        <v>0.66</v>
+        <v>0.043</v>
+      </c>
+      <c r="J145" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="4" t="n">
-        <v>0.00025927</v>
+        <v>0.000143</v>
       </c>
       <c r="B146" s="4" t="n">
-        <v>0.00014377</v>
+        <v>0.00028769</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D146" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E146" s="0" t="n">
-        <v>0.036</v>
-      </c>
-      <c r="F146" s="0" t="n">
-        <v>0.061</v>
-      </c>
-      <c r="G146" s="0" t="n">
-        <v>0.2</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="4" t="n">
-        <v>0.00037919</v>
+        <v>0.00025927</v>
       </c>
       <c r="B147" s="4" t="n">
-        <v>0.0029846</v>
+        <v>0.00014377</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D147" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E147" s="0" t="n">
-        <v>0.028</v>
-      </c>
-      <c r="F147" s="0" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="G147" s="0" t="n">
-        <v>0.52</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="4" t="n">
-        <v>0.00039582</v>
+        <v>0.00037919</v>
       </c>
       <c r="B148" s="4" t="n">
-        <v>0.027861</v>
+        <v>0.0029846</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D148" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E148" s="0" t="n">
-        <v>0.043</v>
-      </c>
-      <c r="F148" s="0" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="G148" s="0" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="I148" s="0" t="s">
-        <v>93</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="4" t="n">
-        <v>0.00055286</v>
+        <v>0.00039582</v>
       </c>
       <c r="B149" s="4" t="n">
-        <v>0.13127</v>
+        <v>0.027861</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D149" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E149" s="0" t="n">
         <v>0.043</v>
       </c>
-      <c r="F149" s="0" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="G149" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="I149" s="0" t="s">
-        <v>93</v>
+      <c r="J149" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="4" t="n">
-        <v>0.0016262</v>
+        <v>0.00055286</v>
       </c>
       <c r="B150" s="4" t="n">
-        <v>2.8017E-005</v>
+        <v>0.13127</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D150" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E150" s="0" t="n">
-        <v>0.035</v>
-      </c>
-      <c r="F150" s="0" t="n">
-        <v>0.068</v>
-      </c>
-      <c r="G150" s="0" t="n">
-        <v>0.11</v>
+        <v>0.043</v>
+      </c>
+      <c r="J150" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="4" t="n">
-        <v>0.0016451</v>
+        <v>0.0016262</v>
       </c>
       <c r="B151" s="4" t="n">
-        <v>0.01021</v>
+        <v>2.8017E-005</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D151" s="0" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E151" s="0" t="n">
-        <v>0.042</v>
-      </c>
-      <c r="F151" s="0" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="G151" s="0" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="I151" s="0" t="s">
-        <v>93</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="4" t="n">
-        <v>0.0018396</v>
+        <v>0.0016451</v>
       </c>
       <c r="B152" s="4" t="n">
-        <v>0.004497</v>
+        <v>0.01021</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D152" s="0" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E152" s="0" t="n">
-        <v>0.024</v>
-      </c>
-      <c r="F152" s="0" t="n">
-        <v>0.127</v>
-      </c>
-      <c r="G152" s="0" t="n">
-        <v>0.44</v>
+        <v>0.042</v>
+      </c>
+      <c r="J152" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="4" t="n">
-        <v>0.0021531</v>
+        <v>0.0018396</v>
       </c>
       <c r="B153" s="4" t="n">
-        <v>0.0044713</v>
+        <v>0.004497</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D153" s="0" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E153" s="0" t="n">
-        <v>0.129</v>
-      </c>
-      <c r="F153" s="0" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="G153" s="0" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="I153" s="0" t="s">
-        <v>93</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="4" t="n">
-        <v>0.00378</v>
+        <v>0.0021531</v>
       </c>
       <c r="B154" s="4" t="n">
-        <v>0.19318</v>
+        <v>0.0044713</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D154" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E154" s="0" t="n">
-        <v>0.042</v>
-      </c>
-      <c r="F154" s="0" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="G154" s="0" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="I154" s="0" t="s">
-        <v>93</v>
+        <v>0.129</v>
+      </c>
+      <c r="J154" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="4" t="n">
-        <v>0.0037956</v>
+        <v>0.00378</v>
       </c>
       <c r="B155" s="4" t="n">
-        <v>0.0014238</v>
+        <v>0.19318</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D155" s="0" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E155" s="0" t="n">
-        <v>162.36</v>
-      </c>
-      <c r="F155" s="0" t="n">
-        <v>0.062</v>
-      </c>
-      <c r="G155" s="0" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H155" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="I155" s="0" t="s">
-        <v>38</v>
+        <v>0.042</v>
+      </c>
+      <c r="J155" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="4" t="n">
-        <v>0.0044606</v>
+        <v>0.0037956</v>
       </c>
       <c r="B156" s="4" t="n">
-        <v>0.11008</v>
+        <v>0.0014238</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D156" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E156" s="0" t="n">
-        <v>0.042</v>
-      </c>
-      <c r="F156" s="0" t="n">
-        <v>0.015</v>
-      </c>
-      <c r="G156" s="0" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="I156" s="0" t="s">
-        <v>93</v>
+        <v>162.36</v>
+      </c>
+      <c r="J156" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="4" t="n">
-        <v>0.0058469</v>
+        <v>0.0044606</v>
       </c>
       <c r="B157" s="4" t="n">
-        <v>9.3986E-005</v>
+        <v>0.11008</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D157" s="0" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E157" s="0" t="n">
-        <v>2443.44</v>
-      </c>
-      <c r="F157" s="0" t="n">
-        <v>0.085</v>
-      </c>
-      <c r="G157" s="0" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H157" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="I157" s="0" t="s">
-        <v>38</v>
+        <v>0.042</v>
+      </c>
+      <c r="J157" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="4" t="n">
+        <v>0.0058469</v>
+      </c>
+      <c r="B158" s="4" t="n">
+        <v>9.3986E-005</v>
+      </c>
+      <c r="C158" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="D158" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E158" s="0" t="n">
+        <v>2443.44</v>
+      </c>
+      <c r="J158" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="4" t="n">
         <v>0.0094124</v>
       </c>
-      <c r="B158" s="4" t="n">
+      <c r="B159" s="4" t="n">
         <v>4.3753E-005</v>
       </c>
-      <c r="C158" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="D158" s="0" t="n">
+      <c r="C159" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D159" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="E158" s="0" t="n">
+      <c r="E159" s="0" t="n">
         <v>174586</v>
       </c>
-      <c r="F158" s="0" t="n">
-        <v>0.058</v>
-      </c>
-      <c r="G158" s="0" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="H158" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="I158" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B160" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="G160" s="0" t="s">
-        <v>159</v>
+      <c r="J159" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="0" t="s">
-        <v>48</v>
-      </c>
       <c r="B161" s="0" t="s">
-        <v>160</v>
+        <v>43</v>
       </c>
       <c r="G161" s="0" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="G162" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B162" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
-      <c r="D164" s="2"/>
-      <c r="E164" s="2"/>
-      <c r="F164" s="2"/>
-      <c r="G164" s="2"/>
-      <c r="H164" s="2"/>
-      <c r="I164" s="2"/>
+      <c r="B163" s="0" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="3" t="s">
+      <c r="A165" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B165" s="2"/>
+      <c r="C165" s="2"/>
+      <c r="D165" s="2"/>
+      <c r="E165" s="2"/>
+      <c r="F165" s="2"/>
+      <c r="G165" s="2"/>
+      <c r="H165" s="2"/>
+      <c r="I165" s="2"/>
+      <c r="J165" s="2"/>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B165" s="3" t="s">
+      <c r="B166" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C165" s="3" t="s">
+      <c r="C166" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D165" s="3" t="s">
+      <c r="D166" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E165" s="3" t="s">
+      <c r="E166" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F165" s="3" t="s">
+      <c r="F166" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G165" s="3" t="s">
+      <c r="G166" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H165" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="I165" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="0" t="n">
+      <c r="H166" s="3"/>
+      <c r="I166" s="3"/>
+      <c r="J166" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="n">
         <v>4E-005</v>
       </c>
-      <c r="B166" s="0" t="n">
+      <c r="B167" s="0" t="n">
         <v>7E-005</v>
       </c>
-      <c r="C166" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="D166" s="0" t="n">
+      <c r="C167" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="D167" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E166" s="0" t="n">
+      <c r="E167" s="0" t="n">
         <v>0.017</v>
       </c>
-      <c r="F166" s="0" t="n">
+      <c r="F167" s="0" t="n">
         <v>0.149</v>
       </c>
-      <c r="G166" s="0" t="n">
+      <c r="G167" s="0" t="n">
         <v>0.58</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A41:I41"/>
-    <mergeCell ref="A64:I64"/>
-    <mergeCell ref="A73:I73"/>
-    <mergeCell ref="A79:I79"/>
-    <mergeCell ref="A80:I80"/>
-    <mergeCell ref="A117:I117"/>
-    <mergeCell ref="A121:I121"/>
-    <mergeCell ref="A126:I126"/>
-    <mergeCell ref="A127:I127"/>
-    <mergeCell ref="A164:I164"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A41:J41"/>
+    <mergeCell ref="A64:J64"/>
+    <mergeCell ref="A73:J73"/>
+    <mergeCell ref="A79:J79"/>
+    <mergeCell ref="A80:J80"/>
+    <mergeCell ref="A117:J117"/>
+    <mergeCell ref="A122:J122"/>
+    <mergeCell ref="A127:J127"/>
+    <mergeCell ref="A128:J128"/>
+    <mergeCell ref="A165:J165"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
More hyperparamter updated results
</commit_message>
<xml_diff>
--- a/experiments/hyperparameters/hyperparemeter_search.xlsx
+++ b/experiments/hyperparameters/hyperparemeter_search.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="348" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="174" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="162">
   <si>
     <t>EXPERIMENT 1</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Alpha divided by 10 at epoch 30, and again at epoch 40</t>
+  </si>
+  <si>
+    <t>run117</t>
   </si>
   <si>
     <t>EXPERIMENT 2</t>
@@ -619,8 +622,8 @@
   </sheetPr>
   <dimension ref="A1:J167"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I53" activeCellId="0" sqref="I53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A125" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F134" activeCellId="0" sqref="F134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1910,6 +1913,18 @@
       <c r="E53" s="0" t="n">
         <v>0.242</v>
       </c>
+      <c r="F53" s="0" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="G53" s="0" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>0.54</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="n">
@@ -1927,6 +1942,18 @@
       <c r="E54" s="0" t="n">
         <v>0.209</v>
       </c>
+      <c r="F54" s="0" t="n">
+        <v>0.259</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>0.298</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>0.58</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="n">
@@ -1944,6 +1971,18 @@
       <c r="E55" s="0" t="n">
         <v>0.196</v>
       </c>
+      <c r="F55" s="0" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="G55" s="0" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>0.176</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>0.29</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="n">
@@ -1961,6 +2000,18 @@
       <c r="E56" s="0" t="n">
         <v>0.212</v>
       </c>
+      <c r="F56" s="0" t="n">
+        <v>0.148</v>
+      </c>
+      <c r="G56" s="0" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <v>0.202</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <v>0.38</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="n">
@@ -1977,6 +2028,18 @@
       </c>
       <c r="E57" s="0" t="n">
         <v>0.08</v>
+      </c>
+      <c r="F57" s="0" t="n">
+        <v>0.253</v>
+      </c>
+      <c r="G57" s="0" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <v>0.307</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <v>0.38</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2069,9 +2132,15 @@
         <v>0.453</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>0.004</v>
+        <v>0</v>
       </c>
       <c r="G66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J66" s="0" t="s">
@@ -2095,10 +2164,16 @@
         <v>95.248</v>
       </c>
       <c r="F67" s="0" t="n">
-        <v>0.039</v>
+        <v>0.038</v>
       </c>
       <c r="G67" s="0" t="n">
-        <v>0.99999</v>
+        <v>1</v>
+      </c>
+      <c r="H67" s="0" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="I67" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2118,9 +2193,15 @@
         <v>0.075</v>
       </c>
       <c r="F68" s="0" t="n">
-        <v>0.12</v>
+        <v>0.211</v>
       </c>
       <c r="G68" s="0" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="H68" s="0" t="n">
+        <v>0.256</v>
+      </c>
+      <c r="I68" s="0" t="n">
         <v>0.29</v>
       </c>
     </row>
@@ -2141,10 +2222,16 @@
         <v>0.209</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>0.121</v>
+        <v>0.266</v>
       </c>
       <c r="G69" s="0" t="n">
-        <v>0.51</v>
+        <v>0.58</v>
+      </c>
+      <c r="H69" s="0" t="n">
+        <v>0.292</v>
+      </c>
+      <c r="I69" s="0" t="n">
+        <v>0.58</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2164,10 +2251,16 @@
         <v>0.335</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>0.104</v>
+        <v>0.235</v>
       </c>
       <c r="G70" s="0" t="n">
-        <v>0.77</v>
+        <v>0.83</v>
+      </c>
+      <c r="H70" s="0" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="I70" s="0" t="n">
+        <v>0.83</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2187,9 +2280,15 @@
         <v>0.611</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>0.015</v>
+        <v>0.01</v>
       </c>
       <c r="G71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I71" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J71" s="0" t="s">
@@ -2232,8 +2331,12 @@
       <c r="G74" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
+      <c r="H74" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="J74" s="3" t="s">
         <v>11</v>
       </c>
@@ -2255,18 +2358,38 @@
         <v>0.1805</v>
       </c>
       <c r="F75" s="0" t="n">
-        <v>0.133</v>
+        <v>0.368</v>
       </c>
       <c r="G75" s="0" t="n">
-        <v>0.8</v>
+        <v>0.83</v>
+      </c>
+      <c r="H75" s="0" t="n">
+        <v>0.406</v>
+      </c>
+      <c r="I75" s="0" t="n">
+        <v>0.83</v>
       </c>
       <c r="J75" s="0" t="s">
         <v>80</v>
       </c>
     </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>3E-006</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2280,7 +2403,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2332,7 +2455,7 @@
         <v>0.000153030184042259</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>1</v>
@@ -2361,7 +2484,7 @@
         <v>0.613281671174882</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>2</v>
@@ -2390,7 +2513,7 @@
         <v>0.00083424047044789</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>3</v>
@@ -2419,7 +2542,7 @@
         <v>0.00145975149652255</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D85" s="0" t="n">
         <v>4</v>
@@ -2448,7 +2571,7 @@
         <v>0.00214462479812596</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D86" s="0" t="n">
         <v>5</v>
@@ -2477,7 +2600,7 @@
         <v>0.00204027518128024</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D87" s="0" t="n">
         <v>6</v>
@@ -2506,7 +2629,7 @@
         <v>2.2261234522861</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D88" s="0" t="n">
         <v>7</v>
@@ -2527,7 +2650,7 @@
         <v>0.42</v>
       </c>
       <c r="J88" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2538,7 +2661,7 @@
         <v>0.00363581666441528</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D89" s="0" t="n">
         <v>8</v>
@@ -2567,7 +2690,7 @@
         <v>0.385037978791714</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D90" s="0" t="n">
         <v>9</v>
@@ -2588,7 +2711,7 @@
         <v>0.21</v>
       </c>
       <c r="J90" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2599,7 +2722,7 @@
         <v>0.046693736064734</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D91" s="0" t="n">
         <v>10</v>
@@ -2620,7 +2743,7 @@
         <v>0.08</v>
       </c>
       <c r="J91" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2631,7 +2754,7 @@
         <v>0.162706410105612</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D92" s="0" t="n">
         <v>11</v>
@@ -2652,7 +2775,7 @@
         <v>0.25</v>
       </c>
       <c r="J92" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2663,7 +2786,7 @@
         <v>0.000189095715104318</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D93" s="0" t="n">
         <v>12</v>
@@ -2692,7 +2815,7 @@
         <v>1.13708526519229</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D94" s="0" t="n">
         <v>13</v>
@@ -2713,7 +2836,7 @@
         <v>0.17</v>
       </c>
       <c r="J94" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2724,7 +2847,7 @@
         <v>0.00657401455755455</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D95" s="0" t="n">
         <v>14</v>
@@ -2745,7 +2868,7 @@
         <v>0.38</v>
       </c>
       <c r="J95" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2756,7 +2879,7 @@
         <v>0.457935644905112</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D96" s="0" t="n">
         <v>15</v>
@@ -2777,7 +2900,7 @@
         <v>0.17</v>
       </c>
       <c r="J96" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2788,7 +2911,7 @@
         <v>0.0299086467558126</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D97" s="0" t="n">
         <v>1</v>
@@ -2809,7 +2932,7 @@
         <v>0.25</v>
       </c>
       <c r="J97" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2820,7 +2943,7 @@
         <v>1.35138015113964</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D98" s="0" t="n">
         <v>2</v>
@@ -2841,7 +2964,7 @@
         <v>0.08</v>
       </c>
       <c r="J98" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2852,7 +2975,7 @@
         <v>0.132421974305338</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D99" s="0" t="n">
         <v>3</v>
@@ -2873,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="J99" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2884,7 +3007,7 @@
         <v>1.98269006319899</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D100" s="0" t="n">
         <v>4</v>
@@ -2905,7 +3028,7 @@
         <v>0.13</v>
       </c>
       <c r="J100" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2916,7 +3039,7 @@
         <v>3.39161236924989</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D101" s="0" t="n">
         <v>5</v>
@@ -2937,7 +3060,7 @@
         <v>0.08</v>
       </c>
       <c r="J101" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2948,7 +3071,7 @@
         <v>0.0017523256961147</v>
       </c>
       <c r="C102" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D102" s="0" t="n">
         <v>6</v>
@@ -2969,7 +3092,7 @@
         <v>1</v>
       </c>
       <c r="J102" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2980,7 +3103,7 @@
         <v>0.448429759066528</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D103" s="0" t="n">
         <v>7</v>
@@ -3001,7 +3124,7 @@
         <v>1</v>
       </c>
       <c r="J103" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3012,7 +3135,7 @@
         <v>0.00467719681179643</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D104" s="0" t="n">
         <v>8</v>
@@ -3044,7 +3167,7 @@
         <v>0.0496849799771728</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D105" s="0" t="n">
         <v>9</v>
@@ -3076,7 +3199,7 @@
         <v>0.00730849961283516</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D106" s="0" t="n">
         <v>10</v>
@@ -3108,7 +3231,7 @@
         <v>0.357772344667488</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D107" s="0" t="n">
         <v>11</v>
@@ -3140,7 +3263,7 @@
         <v>1.78066366225851</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D108" s="0" t="n">
         <v>12</v>
@@ -3172,7 +3295,7 @@
         <v>0.510827647752</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D109" s="0" t="n">
         <v>1</v>
@@ -3204,7 +3327,7 @@
         <v>0.00185294947891615</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D110" s="0" t="n">
         <v>2</v>
@@ -3236,7 +3359,7 @@
         <v>2.84541673997607</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D111" s="0" t="n">
         <v>3</v>
@@ -3270,10 +3393,10 @@
         <v>45</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G114" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3281,10 +3404,10 @@
         <v>3</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G115" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3341,7 +3464,7 @@
         <v>0.002</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D119" s="0" t="n">
         <v>1</v>
@@ -3370,7 +3493,7 @@
         <v>0.002</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D120" s="0" t="n">
         <v>2</v>
@@ -3378,7 +3501,7 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -3426,7 +3549,7 @@
         <v>0.003</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D124" s="0" t="n">
         <v>2</v>
@@ -3447,12 +3570,12 @@
         <v>0.71</v>
       </c>
       <c r="J124" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3466,7 +3589,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -3518,7 +3641,7 @@
         <v>0.26921</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D130" s="0" t="n">
         <v>1</v>
@@ -3547,7 +3670,7 @@
         <v>3.0387E-005</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D131" s="0" t="n">
         <v>2</v>
@@ -3576,13 +3699,25 @@
         <v>0.2741</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D132" s="0" t="n">
         <v>3</v>
       </c>
       <c r="E132" s="0" t="n">
         <v>0.04</v>
+      </c>
+      <c r="F132" s="0" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="G132" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H132" s="0" t="n">
+        <v>0.255</v>
+      </c>
+      <c r="I132" s="0" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3593,13 +3728,25 @@
         <v>0.00073872</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D133" s="0" t="n">
         <v>4</v>
       </c>
       <c r="E133" s="0" t="n">
         <v>0.031</v>
+      </c>
+      <c r="F133" s="0" t="n">
+        <v>0.311</v>
+      </c>
+      <c r="G133" s="0" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="H133" s="0" t="n">
+        <v>0.368</v>
+      </c>
+      <c r="I133" s="0" t="n">
+        <v>0.92</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3610,7 +3757,7 @@
         <v>5.5114E-005</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D134" s="0" t="n">
         <v>5</v>
@@ -3627,7 +3774,7 @@
         <v>7.581E-005</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D135" s="0" t="n">
         <v>6</v>
@@ -3644,7 +3791,7 @@
         <v>5.0484E-005</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D136" s="0" t="n">
         <v>7</v>
@@ -3661,7 +3808,7 @@
         <v>0.0012329</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D137" s="0" t="n">
         <v>8</v>
@@ -3678,7 +3825,7 @@
         <v>0.0007946</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D138" s="0" t="n">
         <v>9</v>
@@ -3695,7 +3842,7 @@
         <v>0.00052887</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D139" s="0" t="n">
         <v>10</v>
@@ -3712,7 +3859,7 @@
         <v>0.00048127</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D140" s="0" t="n">
         <v>11</v>
@@ -3729,7 +3876,7 @@
         <v>0.001023</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D141" s="0" t="n">
         <v>12</v>
@@ -3746,7 +3893,7 @@
         <v>0.00084802</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D142" s="0" t="n">
         <v>13</v>
@@ -3763,7 +3910,7 @@
         <v>0.003607</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D143" s="0" t="n">
         <v>14</v>
@@ -3780,7 +3927,7 @@
         <v>0.18602</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D144" s="0" t="n">
         <v>15</v>
@@ -3789,7 +3936,7 @@
         <v>0.043</v>
       </c>
       <c r="J144" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3800,7 +3947,7 @@
         <v>0.045356</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D145" s="0" t="n">
         <v>1</v>
@@ -3809,7 +3956,7 @@
         <v>0.043</v>
       </c>
       <c r="J145" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3820,7 +3967,7 @@
         <v>0.00028769</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D146" s="0" t="n">
         <v>2</v>
@@ -3837,7 +3984,7 @@
         <v>0.00014377</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D147" s="0" t="n">
         <v>3</v>
@@ -3854,7 +4001,7 @@
         <v>0.0029846</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D148" s="0" t="n">
         <v>4</v>
@@ -3871,7 +4018,7 @@
         <v>0.027861</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D149" s="0" t="n">
         <v>5</v>
@@ -3880,7 +4027,7 @@
         <v>0.043</v>
       </c>
       <c r="J149" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3891,7 +4038,7 @@
         <v>0.13127</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D150" s="0" t="n">
         <v>6</v>
@@ -3900,7 +4047,7 @@
         <v>0.043</v>
       </c>
       <c r="J150" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3911,7 +4058,7 @@
         <v>2.8017E-005</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D151" s="0" t="n">
         <v>7</v>
@@ -3928,7 +4075,7 @@
         <v>0.01021</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D152" s="0" t="n">
         <v>8</v>
@@ -3937,7 +4084,7 @@
         <v>0.042</v>
       </c>
       <c r="J152" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3948,7 +4095,7 @@
         <v>0.004497</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D153" s="0" t="n">
         <v>9</v>
@@ -3965,7 +4112,7 @@
         <v>0.0044713</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D154" s="0" t="n">
         <v>10</v>
@@ -3974,7 +4121,7 @@
         <v>0.129</v>
       </c>
       <c r="J154" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3985,7 +4132,7 @@
         <v>0.19318</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D155" s="0" t="n">
         <v>11</v>
@@ -3994,7 +4141,7 @@
         <v>0.042</v>
       </c>
       <c r="J155" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4005,7 +4152,7 @@
         <v>0.0014238</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D156" s="0" t="n">
         <v>12</v>
@@ -4025,7 +4172,7 @@
         <v>0.11008</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D157" s="0" t="n">
         <v>13</v>
@@ -4034,7 +4181,7 @@
         <v>0.042</v>
       </c>
       <c r="J157" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4045,7 +4192,7 @@
         <v>9.3986E-005</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D158" s="0" t="n">
         <v>14</v>
@@ -4065,7 +4212,7 @@
         <v>4.3753E-005</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D159" s="0" t="n">
         <v>15</v>
@@ -4082,7 +4229,7 @@
         <v>43</v>
       </c>
       <c r="G161" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4090,10 +4237,10 @@
         <v>45</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G162" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4101,7 +4248,7 @@
         <v>3</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4154,7 +4301,7 @@
         <v>7E-005</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D167" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
bit more hs results, tomorrow they'll be complete
</commit_message>
<xml_diff>
--- a/experiments/hyperparameters/hyperparemeter_search.xlsx
+++ b/experiments/hyperparameters/hyperparemeter_search.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="163">
   <si>
     <t>EXPERIMENT 1</t>
   </si>
@@ -494,13 +494,16 @@
     <t>10 .^ unifrnd(-6,-2,30,1)</t>
   </si>
   <si>
-    <t>For plots deleted points with 6 highest alphas or 6 highest lambdas (if repreated)</t>
+    <t>For plots deleted points with 6 highest alphas or 6 highest lambdas (if repeated)</t>
   </si>
   <si>
     <t>10 .^ unifrnd(-5, 0, 30, 1)</t>
   </si>
   <si>
     <t>run115</t>
+  </si>
+  <si>
+    <t>run118</t>
   </si>
 </sst>
 </file>
@@ -620,10 +623,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J167"/>
+  <dimension ref="A1:J168"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A125" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F134" activeCellId="0" sqref="F134"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A135" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B168" activeCellId="0" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3765,6 +3768,18 @@
       <c r="E134" s="0" t="n">
         <v>0.044</v>
       </c>
+      <c r="F134" s="0" t="n">
+        <v>0.308</v>
+      </c>
+      <c r="G134" s="0" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="H134" s="0" t="n">
+        <v>0.366</v>
+      </c>
+      <c r="I134" s="0" t="n">
+        <v>0.92</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="4" t="n">
@@ -3782,6 +3797,18 @@
       <c r="E135" s="0" t="n">
         <v>0.032</v>
       </c>
+      <c r="F135" s="0" t="n">
+        <v>0.317</v>
+      </c>
+      <c r="G135" s="0" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="H135" s="0" t="n">
+        <v>0.376</v>
+      </c>
+      <c r="I135" s="0" t="n">
+        <v>0.92</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="4" t="n">
@@ -3799,6 +3826,18 @@
       <c r="E136" s="0" t="n">
         <v>0.028</v>
       </c>
+      <c r="F136" s="0" t="n">
+        <v>0.307</v>
+      </c>
+      <c r="G136" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="H136" s="0" t="n">
+        <v>0.364</v>
+      </c>
+      <c r="I136" s="0" t="n">
+        <v>0.79</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="4" t="n">
@@ -3816,6 +3855,18 @@
       <c r="E137" s="0" t="n">
         <v>0.026</v>
       </c>
+      <c r="F137" s="0" t="n">
+        <v>0.309</v>
+      </c>
+      <c r="G137" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="H137" s="0" t="n">
+        <v>0.364</v>
+      </c>
+      <c r="I137" s="0" t="n">
+        <v>0.79</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="4" t="n">
@@ -3833,6 +3884,18 @@
       <c r="E138" s="0" t="n">
         <v>0.026</v>
       </c>
+      <c r="F138" s="0" t="n">
+        <v>0.321</v>
+      </c>
+      <c r="G138" s="0" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="H138" s="0" t="n">
+        <v>0.368</v>
+      </c>
+      <c r="I138" s="0" t="n">
+        <v>0.83</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="4" t="n">
@@ -3850,6 +3913,18 @@
       <c r="E139" s="0" t="n">
         <v>0.026</v>
       </c>
+      <c r="F139" s="0" t="n">
+        <v>0.323</v>
+      </c>
+      <c r="G139" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="H139" s="0" t="n">
+        <v>0.378</v>
+      </c>
+      <c r="I139" s="0" t="n">
+        <v>0.79</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="4" t="n">
@@ -3867,6 +3942,18 @@
       <c r="E140" s="0" t="n">
         <v>0.027</v>
       </c>
+      <c r="F140" s="0" t="n">
+        <v>0.334</v>
+      </c>
+      <c r="G140" s="0" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="H140" s="0" t="n">
+        <v>0.387</v>
+      </c>
+      <c r="I140" s="0" t="n">
+        <v>0.83</v>
+      </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="4" t="n">
@@ -3884,6 +3971,18 @@
       <c r="E141" s="0" t="n">
         <v>0.025</v>
       </c>
+      <c r="F141" s="0" t="n">
+        <v>0.321</v>
+      </c>
+      <c r="G141" s="0" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="H141" s="0" t="n">
+        <v>0.374</v>
+      </c>
+      <c r="I141" s="0" t="n">
+        <v>0.79</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="4" t="n">
@@ -3901,6 +4000,18 @@
       <c r="E142" s="0" t="n">
         <v>0.024</v>
       </c>
+      <c r="F142" s="0" t="n">
+        <v>0.315</v>
+      </c>
+      <c r="G142" s="0" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="H142" s="0" t="n">
+        <v>0.369</v>
+      </c>
+      <c r="I142" s="0" t="n">
+        <v>0.66</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="4" t="n">
@@ -3918,6 +4029,18 @@
       <c r="E143" s="0" t="n">
         <v>0.023</v>
       </c>
+      <c r="F143" s="0" t="n">
+        <v>0.303</v>
+      </c>
+      <c r="G143" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H143" s="0" t="n">
+        <v>0.368</v>
+      </c>
+      <c r="I143" s="0" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="4" t="n">
@@ -3935,6 +4058,18 @@
       <c r="E144" s="0" t="n">
         <v>0.043</v>
       </c>
+      <c r="F144" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G144" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="H144" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I144" s="0" t="n">
+        <v>0.13</v>
+      </c>
       <c r="J144" s="0" t="s">
         <v>91</v>
       </c>
@@ -3955,6 +4090,18 @@
       <c r="E145" s="0" t="n">
         <v>0.043</v>
       </c>
+      <c r="F145" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G145" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="H145" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I145" s="0" t="n">
+        <v>0.13</v>
+      </c>
       <c r="J145" s="0" t="s">
         <v>91</v>
       </c>
@@ -3975,6 +4122,18 @@
       <c r="E146" s="0" t="n">
         <v>0.022</v>
       </c>
+      <c r="F146" s="0" t="n">
+        <v>0.314</v>
+      </c>
+      <c r="G146" s="0" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="H146" s="0" t="n">
+        <v>0.373</v>
+      </c>
+      <c r="I146" s="0" t="n">
+        <v>0.67</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="4" t="n">
@@ -3992,6 +4151,18 @@
       <c r="E147" s="0" t="n">
         <v>0.036</v>
       </c>
+      <c r="F147" s="0" t="n">
+        <v>0.105</v>
+      </c>
+      <c r="G147" s="0" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="H147" s="0" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="I147" s="0" t="n">
+        <v>0.21</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="4" t="n">
@@ -4008,6 +4179,18 @@
       </c>
       <c r="E148" s="0" t="n">
         <v>0.028</v>
+      </c>
+      <c r="F148" s="0" t="n">
+        <v>0.305</v>
+      </c>
+      <c r="G148" s="0" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="H148" s="0" t="n">
+        <v>0.355</v>
+      </c>
+      <c r="I148" s="0" t="n">
+        <v>0.54</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4314,6 +4497,17 @@
       </c>
       <c r="G167" s="0" t="n">
         <v>0.58</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="n">
+        <v>4E-005</v>
+      </c>
+      <c r="B168" s="0" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="C168" s="0" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all hyperparameter search results
</commit_message>
<xml_diff>
--- a/experiments/hyperparameters/hyperparemeter_search.xlsx
+++ b/experiments/hyperparameters/hyperparemeter_search.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="174" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="87" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="163">
   <si>
     <t>EXPERIMENT 1</t>
   </si>
@@ -494,7 +494,7 @@
     <t>10 .^ unifrnd(-6,-2,30,1)</t>
   </si>
   <si>
-    <t>For plots deleted points with 6 highest alphas or 6 highest lambdas (if repeated)</t>
+    <t>For plots deleted points with 10 highest alphas or 10 highest lambdas (if repeated)</t>
   </si>
   <si>
     <t>10 .^ unifrnd(-5, 0, 30, 1)</t>
@@ -625,8 +625,8 @@
   </sheetPr>
   <dimension ref="A1:J168"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A135" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B168" activeCellId="0" sqref="B168"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A141" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G162" activeCellId="0" sqref="G162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4209,6 +4209,18 @@
       <c r="E149" s="0" t="n">
         <v>0.043</v>
       </c>
+      <c r="F149" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G149" s="0" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="H149" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I149" s="0" t="n">
+        <v>0.08</v>
+      </c>
       <c r="J149" s="0" t="s">
         <v>91</v>
       </c>
@@ -4229,6 +4241,18 @@
       <c r="E150" s="0" t="n">
         <v>0.043</v>
       </c>
+      <c r="F150" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G150" s="0" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="H150" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I150" s="0" t="n">
+        <v>0.04</v>
+      </c>
       <c r="J150" s="0" t="s">
         <v>91</v>
       </c>
@@ -4249,6 +4273,18 @@
       <c r="E151" s="0" t="n">
         <v>0.035</v>
       </c>
+      <c r="F151" s="0" t="n">
+        <v>0.111</v>
+      </c>
+      <c r="G151" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="H151" s="0" t="n">
+        <v>0.168</v>
+      </c>
+      <c r="I151" s="0" t="n">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="4" t="n">
@@ -4266,6 +4302,18 @@
       <c r="E152" s="0" t="n">
         <v>0.042</v>
       </c>
+      <c r="F152" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G152" s="0" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="H152" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I152" s="0" t="n">
+        <v>0.08</v>
+      </c>
       <c r="J152" s="0" t="s">
         <v>91</v>
       </c>
@@ -4286,6 +4334,18 @@
       <c r="E153" s="0" t="n">
         <v>0.024</v>
       </c>
+      <c r="F153" s="0" t="n">
+        <v>0.289</v>
+      </c>
+      <c r="G153" s="0" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="H153" s="0" t="n">
+        <v>0.366</v>
+      </c>
+      <c r="I153" s="0" t="n">
+        <v>0.54</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="4" t="n">
@@ -4303,8 +4363,17 @@
       <c r="E154" s="0" t="n">
         <v>0.129</v>
       </c>
-      <c r="J154" s="0" t="s">
-        <v>91</v>
+      <c r="F154" s="0" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="G154" s="0" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="H154" s="0" t="n">
+        <v>0.038</v>
+      </c>
+      <c r="I154" s="0" t="n">
+        <v>0.04</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4323,6 +4392,18 @@
       <c r="E155" s="0" t="n">
         <v>0.042</v>
       </c>
+      <c r="F155" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G155" s="0" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="H155" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I155" s="0" t="n">
+        <v>0.08</v>
+      </c>
       <c r="J155" s="0" t="s">
         <v>91</v>
       </c>
@@ -4343,6 +4424,18 @@
       <c r="E156" s="0" t="n">
         <v>162.36</v>
       </c>
+      <c r="F156" s="0" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="G156" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H156" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="I156" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="J156" s="0" t="s">
         <v>36</v>
       </c>
@@ -4363,6 +4456,18 @@
       <c r="E157" s="0" t="n">
         <v>0.042</v>
       </c>
+      <c r="F157" s="0" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="G157" s="0" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="H157" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I157" s="0" t="n">
+        <v>0.13</v>
+      </c>
       <c r="J157" s="0" t="s">
         <v>91</v>
       </c>
@@ -4383,6 +4488,18 @@
       <c r="E158" s="0" t="n">
         <v>2443.44</v>
       </c>
+      <c r="F158" s="0" t="n">
+        <v>0.098</v>
+      </c>
+      <c r="G158" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H158" s="0" t="n">
+        <v>0.171</v>
+      </c>
+      <c r="I158" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="J158" s="0" t="s">
         <v>36</v>
       </c>
@@ -4402,6 +4519,18 @@
       </c>
       <c r="E159" s="0" t="n">
         <v>174586</v>
+      </c>
+      <c r="F159" s="0" t="n">
+        <v>0.066</v>
+      </c>
+      <c r="G159" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H159" s="0" t="n">
+        <v>0.129</v>
+      </c>
+      <c r="I159" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="J159" s="0" t="s">
         <v>36</v>
@@ -4470,8 +4599,12 @@
       <c r="G166" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H166" s="3"/>
-      <c r="I166" s="3"/>
+      <c r="H166" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I166" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="J166" s="3" t="s">
         <v>11</v>
       </c>
@@ -4493,10 +4626,16 @@
         <v>0.017</v>
       </c>
       <c r="F167" s="0" t="n">
-        <v>0.149</v>
+        <v>0.329</v>
       </c>
       <c r="G167" s="0" t="n">
-        <v>0.58</v>
+        <v>0.83</v>
+      </c>
+      <c r="H167" s="0" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="I167" s="0" t="n">
+        <v>0.83</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4508,6 +4647,9 @@
       </c>
       <c r="C168" s="0" t="s">
         <v>162</v>
+      </c>
+      <c r="D168" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated report: results from experiment 3
</commit_message>
<xml_diff>
--- a/experiments/hyperparameters/hyperparemeter_search.xlsx
+++ b/experiments/hyperparameters/hyperparemeter_search.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="89" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="90" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -655,8 +655,8 @@
   </sheetPr>
   <dimension ref="A1:J174"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A157" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D176" activeCellId="0" sqref="D176"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A149" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D168" activeCellId="0" sqref="D168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4716,6 +4716,21 @@
       </c>
       <c r="D168" s="0" t="n">
         <v>16</v>
+      </c>
+      <c r="E168" s="0" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="F168" s="0" t="n">
+        <v>0.313</v>
+      </c>
+      <c r="G168" s="0" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="H168" s="0" t="n">
+        <v>0.348</v>
+      </c>
+      <c r="I168" s="0" t="n">
+        <v>0.87</v>
       </c>
       <c r="J168" s="0" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
Hyperaparameter search results for experiment 1
</commit_message>
<xml_diff>
--- a/experiments/hyperparameters/hyperparemeter_search.xlsx
+++ b/experiments/hyperparameters/hyperparemeter_search.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="44" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="88" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="534">
   <si>
     <t>EXPERIMENT 2</t>
   </si>
@@ -893,6 +893,9 @@
     <t>fold5</t>
   </si>
   <si>
+    <t>EXPERIMENT 1</t>
+  </si>
+  <si>
     <t>10 .^ unifrnd(-5,-1,25,1)</t>
   </si>
   <si>
@@ -1079,40 +1082,40 @@
     <t>run279</t>
   </si>
   <si>
-    <t>low predictions</t>
-  </si>
-  <si>
     <t>run280</t>
   </si>
   <si>
     <t>run281</t>
   </si>
   <si>
+    <t>run289</t>
+  </si>
+  <si>
+    <t>kinda big jump</t>
+  </si>
+  <si>
     <t>run282</t>
   </si>
   <si>
+    <t>run286</t>
+  </si>
+  <si>
+    <t>run287</t>
+  </si>
+  <si>
+    <t>run285</t>
+  </si>
+  <si>
     <t>run283</t>
   </si>
   <si>
+    <t>run288</t>
+  </si>
+  <si>
     <t>run284</t>
   </si>
   <si>
-    <t>run285</t>
-  </si>
-  <si>
-    <t>run286</t>
-  </si>
-  <si>
-    <t>run287</t>
-  </si>
-  <si>
-    <t>run288</t>
-  </si>
-  <si>
-    <t>run289</t>
-  </si>
-  <si>
-    <t>kinda big jump</t>
+    <t>big jump in FP</t>
   </si>
   <si>
     <t>run290</t>
@@ -1157,36 +1160,36 @@
     <t>run303</t>
   </si>
   <si>
+    <t>run312</t>
+  </si>
+  <si>
+    <t>run308</t>
+  </si>
+  <si>
+    <t>run305</t>
+  </si>
+  <si>
+    <t>run309</t>
+  </si>
+  <si>
+    <t>run310</t>
+  </si>
+  <si>
+    <t>run311</t>
+  </si>
+  <si>
+    <t>run307</t>
+  </si>
+  <si>
+    <t>run313</t>
+  </si>
+  <si>
+    <t>run306</t>
+  </si>
+  <si>
     <t>run304</t>
   </si>
   <si>
-    <t>run305</t>
-  </si>
-  <si>
-    <t>run306</t>
-  </si>
-  <si>
-    <t>run307</t>
-  </si>
-  <si>
-    <t>run308</t>
-  </si>
-  <si>
-    <t>run309</t>
-  </si>
-  <si>
-    <t>run310</t>
-  </si>
-  <si>
-    <t>run311</t>
-  </si>
-  <si>
-    <t>run312</t>
-  </si>
-  <si>
-    <t>run313</t>
-  </si>
-  <si>
     <t>run314</t>
   </si>
   <si>
@@ -1229,27 +1232,27 @@
     <t>run327</t>
   </si>
   <si>
+    <t>run334</t>
+  </si>
+  <si>
+    <t>run333</t>
+  </si>
+  <si>
+    <t>run331</t>
+  </si>
+  <si>
+    <t>run332</t>
+  </si>
+  <si>
+    <t>run330</t>
+  </si>
+  <si>
     <t>run328</t>
   </si>
   <si>
     <t>run329</t>
   </si>
   <si>
-    <t>run330</t>
-  </si>
-  <si>
-    <t>run331</t>
-  </si>
-  <si>
-    <t>run332</t>
-  </si>
-  <si>
-    <t>run333</t>
-  </si>
-  <si>
-    <t>run334</t>
-  </si>
-  <si>
     <t>run335</t>
   </si>
   <si>
@@ -1307,13 +1310,313 @@
     <t>run353</t>
   </si>
   <si>
-    <t>EXPERIMENT 3_2</t>
-  </si>
-  <si>
-    <t>10 .^ unifrnd(-5,-4,20,1)</t>
+    <t>EXPERIMENT 1_2</t>
+  </si>
+  <si>
+    <t>10 .^ unifrnd(-5,-2,20,1)</t>
   </si>
   <si>
     <t>10 .^ unifrnd(-3, 0, 20, 1)</t>
+  </si>
+  <si>
+    <t>run354</t>
+  </si>
+  <si>
+    <t>run355</t>
+  </si>
+  <si>
+    <t>run356</t>
+  </si>
+  <si>
+    <t>run357</t>
+  </si>
+  <si>
+    <t>run358</t>
+  </si>
+  <si>
+    <t>run359</t>
+  </si>
+  <si>
+    <t>run360</t>
+  </si>
+  <si>
+    <t>run361</t>
+  </si>
+  <si>
+    <t>run362</t>
+  </si>
+  <si>
+    <t>run363</t>
+  </si>
+  <si>
+    <t>run364</t>
+  </si>
+  <si>
+    <t>run365</t>
+  </si>
+  <si>
+    <t>run366</t>
+  </si>
+  <si>
+    <t>run367</t>
+  </si>
+  <si>
+    <t>run368</t>
+  </si>
+  <si>
+    <t>run369</t>
+  </si>
+  <si>
+    <t>run370</t>
+  </si>
+  <si>
+    <t>run371</t>
+  </si>
+  <si>
+    <t>run372</t>
+  </si>
+  <si>
+    <t>run373</t>
+  </si>
+  <si>
+    <t>run374</t>
+  </si>
+  <si>
+    <t>run375</t>
+  </si>
+  <si>
+    <t>run376</t>
+  </si>
+  <si>
+    <t>run377</t>
+  </si>
+  <si>
+    <t>run378</t>
+  </si>
+  <si>
+    <t>run379</t>
+  </si>
+  <si>
+    <t>run380</t>
+  </si>
+  <si>
+    <t>run381</t>
+  </si>
+  <si>
+    <t>run382</t>
+  </si>
+  <si>
+    <t>run383</t>
+  </si>
+  <si>
+    <t>run384</t>
+  </si>
+  <si>
+    <t>run385</t>
+  </si>
+  <si>
+    <t>run386</t>
+  </si>
+  <si>
+    <t>run387</t>
+  </si>
+  <si>
+    <t>run388</t>
+  </si>
+  <si>
+    <t>run389</t>
+  </si>
+  <si>
+    <t>run390</t>
+  </si>
+  <si>
+    <t>run391</t>
+  </si>
+  <si>
+    <t>run392</t>
+  </si>
+  <si>
+    <t>run393</t>
+  </si>
+  <si>
+    <t>run394</t>
+  </si>
+  <si>
+    <t>run395</t>
+  </si>
+  <si>
+    <t>run396</t>
+  </si>
+  <si>
+    <t>run397</t>
+  </si>
+  <si>
+    <t>run398</t>
+  </si>
+  <si>
+    <t>run399</t>
+  </si>
+  <si>
+    <t>run400</t>
+  </si>
+  <si>
+    <t>run401</t>
+  </si>
+  <si>
+    <t>run402</t>
+  </si>
+  <si>
+    <t>run403</t>
+  </si>
+  <si>
+    <t>run404</t>
+  </si>
+  <si>
+    <t>run405</t>
+  </si>
+  <si>
+    <t>run406</t>
+  </si>
+  <si>
+    <t>run407</t>
+  </si>
+  <si>
+    <t>run408</t>
+  </si>
+  <si>
+    <t>run409</t>
+  </si>
+  <si>
+    <t>run410</t>
+  </si>
+  <si>
+    <t>run411</t>
+  </si>
+  <si>
+    <t>run412</t>
+  </si>
+  <si>
+    <t>run413</t>
+  </si>
+  <si>
+    <t>run414</t>
+  </si>
+  <si>
+    <t>run415</t>
+  </si>
+  <si>
+    <t>run416</t>
+  </si>
+  <si>
+    <t>run417</t>
+  </si>
+  <si>
+    <t>run418</t>
+  </si>
+  <si>
+    <t>run419</t>
+  </si>
+  <si>
+    <t>run420</t>
+  </si>
+  <si>
+    <t>run421</t>
+  </si>
+  <si>
+    <t>run422</t>
+  </si>
+  <si>
+    <t>run423</t>
+  </si>
+  <si>
+    <t>run424</t>
+  </si>
+  <si>
+    <t>run425</t>
+  </si>
+  <si>
+    <t>run426</t>
+  </si>
+  <si>
+    <t>run427</t>
+  </si>
+  <si>
+    <t>run428</t>
+  </si>
+  <si>
+    <t>run429</t>
+  </si>
+  <si>
+    <t>run430</t>
+  </si>
+  <si>
+    <t>run431</t>
+  </si>
+  <si>
+    <t>run432</t>
+  </si>
+  <si>
+    <t>run433</t>
+  </si>
+  <si>
+    <t>run434</t>
+  </si>
+  <si>
+    <t>run435</t>
+  </si>
+  <si>
+    <t>run436</t>
+  </si>
+  <si>
+    <t>run437</t>
+  </si>
+  <si>
+    <t>run438</t>
+  </si>
+  <si>
+    <t>run439</t>
+  </si>
+  <si>
+    <t>run440</t>
+  </si>
+  <si>
+    <t>run441</t>
+  </si>
+  <si>
+    <t>run442</t>
+  </si>
+  <si>
+    <t>run443</t>
+  </si>
+  <si>
+    <t>run444</t>
+  </si>
+  <si>
+    <t>run445</t>
+  </si>
+  <si>
+    <t>run446</t>
+  </si>
+  <si>
+    <t>run447</t>
+  </si>
+  <si>
+    <t>run448</t>
+  </si>
+  <si>
+    <t>run449</t>
+  </si>
+  <si>
+    <t>run450</t>
+  </si>
+  <si>
+    <t>run451</t>
+  </si>
+  <si>
+    <t>run452</t>
+  </si>
+  <si>
+    <t>run453</t>
   </si>
 </sst>
 </file>
@@ -1481,16 +1784,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K469"/>
+  <dimension ref="A1:K581"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A451" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A463" activeCellId="0" sqref="A463"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A560" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F582" activeCellId="0" sqref="F582"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6071428571429"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.91836734693878"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.02551020408163"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1071428571429"/>
@@ -8358,7 +8661,7 @@
     </row>
     <row r="310" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="12" t="s">
-        <v>173</v>
+        <v>292</v>
       </c>
       <c r="B310" s="12"/>
       <c r="C310" s="12"/>
@@ -8377,7 +8680,7 @@
         <v>48</v>
       </c>
       <c r="B312" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G312" s="0" t="s">
         <v>175</v>
@@ -8388,7 +8691,7 @@
         <v>3</v>
       </c>
       <c r="B313" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8431,7 +8734,7 @@
         <v>0.038571</v>
       </c>
       <c r="C317" s="6" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D317" s="6" t="n">
         <v>6</v>
@@ -8448,7 +8751,7 @@
         <v>0.0010015</v>
       </c>
       <c r="C318" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D318" s="0" t="n">
         <v>7</v>
@@ -8465,7 +8768,7 @@
         <v>0.0036454</v>
       </c>
       <c r="C319" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D319" s="0" t="n">
         <v>8</v>
@@ -8482,7 +8785,7 @@
         <v>0.00010918</v>
       </c>
       <c r="C320" s="6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D320" s="6" t="n">
         <v>9</v>
@@ -8499,7 +8802,7 @@
         <v>0.00019646</v>
       </c>
       <c r="C321" s="6" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="D321" s="6" t="n">
         <v>10</v>
@@ -8516,7 +8819,7 @@
         <v>0.00021838</v>
       </c>
       <c r="C322" s="6" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D322" s="6" t="n">
         <v>11</v>
@@ -8533,7 +8836,7 @@
         <v>0.0011012</v>
       </c>
       <c r="C323" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D323" s="0" t="n">
         <v>12</v>
@@ -8550,7 +8853,7 @@
         <v>0.0023038</v>
       </c>
       <c r="C324" s="8" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D324" s="8" t="n">
         <v>13</v>
@@ -8559,7 +8862,7 @@
         <v>0.618</v>
       </c>
       <c r="F324" s="8" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="325" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8570,7 +8873,7 @@
         <v>0.047091</v>
       </c>
       <c r="C325" s="8" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D325" s="8" t="n">
         <v>14</v>
@@ -8579,7 +8882,7 @@
         <v>0.621</v>
       </c>
       <c r="F325" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="326" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8590,7 +8893,7 @@
         <v>0.00051262</v>
       </c>
       <c r="C326" s="6" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D326" s="6" t="n">
         <v>15</v>
@@ -8607,7 +8910,7 @@
         <v>0.00012501</v>
       </c>
       <c r="C327" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D327" s="0" t="n">
         <v>16</v>
@@ -8624,7 +8927,7 @@
         <v>0.054703</v>
       </c>
       <c r="C328" s="8" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D328" s="8" t="n">
         <v>17</v>
@@ -8633,7 +8936,7 @@
         <v>0.421</v>
       </c>
       <c r="F328" s="8" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8644,7 +8947,7 @@
         <v>0.040168</v>
       </c>
       <c r="C329" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D329" s="0" t="n">
         <v>18</v>
@@ -8661,7 +8964,7 @@
         <v>0.018404</v>
       </c>
       <c r="C330" s="8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D330" s="8" t="n">
         <v>19</v>
@@ -8678,7 +8981,7 @@
         <v>0.00079363</v>
       </c>
       <c r="C331" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D331" s="0" t="n">
         <v>20</v>
@@ -8687,7 +8990,7 @@
         <v>0.297</v>
       </c>
       <c r="F331" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="332" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8698,7 +9001,7 @@
         <v>0.00016243</v>
       </c>
       <c r="C332" s="6" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D332" s="6" t="n">
         <v>21</v>
@@ -8718,7 +9021,7 @@
         <v>0.00016268</v>
       </c>
       <c r="C333" s="6" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D333" s="6" t="n">
         <v>22</v>
@@ -8738,7 +9041,7 @@
         <v>0.075067</v>
       </c>
       <c r="C334" s="6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D334" s="6" t="n">
         <v>23</v>
@@ -8758,7 +9061,7 @@
         <v>0.011392</v>
       </c>
       <c r="C335" s="6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D335" s="6" t="n">
         <v>24</v>
@@ -8778,7 +9081,7 @@
         <v>0.00057281</v>
       </c>
       <c r="C336" s="6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D336" s="6" t="n">
         <v>25</v>
@@ -8798,7 +9101,7 @@
         <v>0.00012086</v>
       </c>
       <c r="C337" s="6" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D337" s="6" t="n">
         <v>26</v>
@@ -8818,7 +9121,7 @@
         <v>0.00011615</v>
       </c>
       <c r="C338" s="6" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D338" s="6" t="n">
         <v>27</v>
@@ -8838,7 +9141,7 @@
         <v>0.00042194</v>
       </c>
       <c r="C339" s="6" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D339" s="6" t="n">
         <v>28</v>
@@ -8858,7 +9161,7 @@
         <v>0.00010217</v>
       </c>
       <c r="C340" s="6" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D340" s="6" t="n">
         <v>29</v>
@@ -8878,7 +9181,7 @@
         <v>0.025484</v>
       </c>
       <c r="C341" s="6" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D341" s="6" t="n">
         <v>30</v>
@@ -8930,7 +9233,7 @@
         <v>0.0036712</v>
       </c>
       <c r="C345" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D345" s="0" t="n">
         <v>6</v>
@@ -8947,7 +9250,7 @@
         <v>0.0077482</v>
       </c>
       <c r="C346" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D346" s="0" t="n">
         <v>7</v>
@@ -8956,20 +9259,20 @@
         <v>0.211</v>
       </c>
     </row>
-    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A347" s="11" t="n">
+    <row r="347" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="7" t="n">
         <v>2.1528E-005</v>
       </c>
-      <c r="B347" s="11" t="n">
+      <c r="B347" s="7" t="n">
         <v>0.052655</v>
       </c>
-      <c r="C347" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="D347" s="0" t="n">
+      <c r="C347" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="D347" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="E347" s="0" t="n">
+      <c r="E347" s="8" t="n">
         <v>0.55</v>
       </c>
     </row>
@@ -8981,7 +9284,7 @@
         <v>0.07084</v>
       </c>
       <c r="C348" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D348" s="0" t="n">
         <v>9</v>
@@ -8998,7 +9301,7 @@
         <v>0.072016</v>
       </c>
       <c r="C349" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D349" s="0" t="n">
         <v>10</v>
@@ -9015,7 +9318,7 @@
         <v>0.0079555</v>
       </c>
       <c r="C350" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D350" s="0" t="n">
         <v>11</v>
@@ -9024,20 +9327,20 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A351" s="11" t="n">
+    <row r="351" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="7" t="n">
         <v>0.00010264</v>
       </c>
-      <c r="B351" s="11" t="n">
+      <c r="B351" s="7" t="n">
         <v>0.049627</v>
       </c>
-      <c r="C351" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="D351" s="0" t="n">
+      <c r="C351" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="D351" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="E351" s="0" t="n">
+      <c r="E351" s="8" t="n">
         <v>0.386</v>
       </c>
     </row>
@@ -9049,7 +9352,7 @@
         <v>0.00011182</v>
       </c>
       <c r="C352" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D352" s="0" t="n">
         <v>13</v>
@@ -9066,77 +9369,80 @@
         <v>0.013387</v>
       </c>
       <c r="C353" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D353" s="0" t="n">
         <v>14</v>
       </c>
-    </row>
-    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A354" s="11" t="n">
+      <c r="E353" s="0" t="n">
+        <v>0.286</v>
+      </c>
+    </row>
+    <row r="354" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A354" s="5" t="n">
         <v>0.00016629</v>
       </c>
-      <c r="B354" s="11" t="n">
+      <c r="B354" s="5" t="n">
         <v>0.015967</v>
       </c>
-      <c r="C354" s="0" t="s">
-        <v>332</v>
-      </c>
-      <c r="D354" s="0" t="n">
+      <c r="C354" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="D354" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="E354" s="0" t="n">
+      <c r="E354" s="6" t="n">
         <v>0.071</v>
       </c>
     </row>
-    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A355" s="11" t="n">
+    <row r="355" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="5" t="n">
         <v>0.00038917</v>
       </c>
-      <c r="B355" s="11" t="n">
+      <c r="B355" s="5" t="n">
         <v>0.0018935</v>
       </c>
-      <c r="C355" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="D355" s="0" t="n">
+      <c r="C355" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="D355" s="6" t="n">
         <v>16</v>
       </c>
-      <c r="E355" s="0" t="n">
+      <c r="E355" s="6" t="n">
         <v>0.063</v>
       </c>
     </row>
-    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A356" s="11" t="n">
+    <row r="356" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A356" s="7" t="n">
         <v>0.00099599</v>
       </c>
-      <c r="B356" s="11" t="n">
+      <c r="B356" s="7" t="n">
         <v>0.0047879</v>
       </c>
-      <c r="C356" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D356" s="0" t="n">
+      <c r="C356" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="D356" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="E356" s="0" t="n">
+      <c r="E356" s="8" t="n">
         <v>0.308</v>
       </c>
     </row>
-    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A357" s="11" t="n">
+    <row r="357" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="5" t="n">
         <v>0.0013434</v>
       </c>
-      <c r="B357" s="11" t="n">
+      <c r="B357" s="5" t="n">
         <v>0.00026081</v>
       </c>
-      <c r="C357" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="D357" s="0" t="n">
+      <c r="C357" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="D357" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="E357" s="0" t="n">
+      <c r="E357" s="6" t="n">
         <v>0.135</v>
       </c>
     </row>
@@ -9148,7 +9454,7 @@
         <v>0.00014644</v>
       </c>
       <c r="C358" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D358" s="0" t="n">
         <v>19</v>
@@ -9157,20 +9463,20 @@
         <v>0.28</v>
       </c>
     </row>
-    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A359" s="11" t="n">
+    <row r="359" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="7" t="n">
         <v>0.0015186</v>
       </c>
-      <c r="B359" s="11" t="n">
+      <c r="B359" s="7" t="n">
         <v>0.017673</v>
       </c>
-      <c r="C359" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="D359" s="0" t="n">
+      <c r="C359" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="D359" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="E359" s="0" t="n">
+      <c r="E359" s="8" t="n">
         <v>0.364</v>
       </c>
     </row>
@@ -9182,7 +9488,7 @@
         <v>0.0018069</v>
       </c>
       <c r="C360" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D360" s="0" t="n">
         <v>21</v>
@@ -9199,7 +9505,7 @@
         <v>0.019084</v>
       </c>
       <c r="C361" s="6" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D361" s="6" t="n">
         <v>22</v>
@@ -9219,7 +9525,7 @@
         <v>0.0052615</v>
       </c>
       <c r="C362" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D362" s="6" t="n">
         <v>23</v>
@@ -9239,7 +9545,7 @@
         <v>0.016879</v>
       </c>
       <c r="C363" s="6" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D363" s="6" t="n">
         <v>24</v>
@@ -9259,7 +9565,7 @@
         <v>0.0010247</v>
       </c>
       <c r="C364" s="6" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="D364" s="6" t="n">
         <v>25</v>
@@ -9279,7 +9585,7 @@
         <v>0.00011077</v>
       </c>
       <c r="C365" s="6" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D365" s="6" t="n">
         <v>26</v>
@@ -9299,7 +9605,7 @@
         <v>0.0028669</v>
       </c>
       <c r="C366" s="6" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D366" s="6" t="n">
         <v>27</v>
@@ -9319,7 +9625,7 @@
         <v>0.0004377</v>
       </c>
       <c r="C367" s="6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D367" s="6" t="n">
         <v>28</v>
@@ -9339,7 +9645,7 @@
         <v>0.004911</v>
       </c>
       <c r="C368" s="6" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D368" s="6" t="n">
         <v>29</v>
@@ -9359,7 +9665,7 @@
         <v>0.00020247</v>
       </c>
       <c r="C369" s="6" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D369" s="6" t="n">
         <v>30</v>
@@ -9403,37 +9709,37 @@
       </c>
       <c r="G372" s="4"/>
     </row>
-    <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A373" s="11" t="n">
+    <row r="373" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A373" s="5" t="n">
         <v>1.4258E-005</v>
       </c>
-      <c r="B373" s="11" t="n">
+      <c r="B373" s="5" t="n">
         <v>0.0087449</v>
       </c>
-      <c r="C373" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="D373" s="0" t="n">
+      <c r="C373" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="D373" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="E373" s="0" t="n">
+      <c r="E373" s="6" t="n">
         <v>0.033</v>
       </c>
     </row>
-    <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A374" s="11" t="n">
+    <row r="374" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A374" s="5" t="n">
         <v>1.4903E-005</v>
       </c>
-      <c r="B374" s="11" t="n">
+      <c r="B374" s="5" t="n">
         <v>0.022824</v>
       </c>
-      <c r="C374" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="D374" s="0" t="n">
+      <c r="C374" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="D374" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="E374" s="0" t="n">
+      <c r="E374" s="6" t="n">
         <v>0.077</v>
       </c>
     </row>
@@ -9445,7 +9751,7 @@
         <v>0.0003705</v>
       </c>
       <c r="C375" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D375" s="0" t="n">
         <v>8</v>
@@ -9462,7 +9768,7 @@
         <v>0.00079597</v>
       </c>
       <c r="C376" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D376" s="0" t="n">
         <v>9</v>
@@ -9479,10 +9785,13 @@
         <v>0.052861</v>
       </c>
       <c r="C377" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D377" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="E377" s="0" t="n">
+        <v>0.247</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9493,7 +9802,7 @@
         <v>0.0042871</v>
       </c>
       <c r="C378" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D378" s="0" t="n">
         <v>11</v>
@@ -9501,177 +9810,204 @@
       <c r="E378" s="0" t="n">
         <v>0.185</v>
       </c>
-      <c r="F378" s="0" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A379" s="11" t="n">
+    </row>
+    <row r="379" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A379" s="7" t="n">
         <v>6.4091E-005</v>
       </c>
-      <c r="B379" s="11" t="n">
+      <c r="B379" s="7" t="n">
         <v>0.034916</v>
       </c>
-      <c r="C379" s="0" t="s">
+      <c r="C379" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="D379" s="0" t="n">
+      <c r="D379" s="8" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A380" s="11" t="n">
+      <c r="E379" s="8" t="n">
+        <v>0.266</v>
+      </c>
+    </row>
+    <row r="380" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A380" s="5" t="n">
         <v>7.0073E-005</v>
       </c>
-      <c r="B380" s="11" t="n">
+      <c r="B380" s="5" t="n">
         <v>0.025851</v>
       </c>
-      <c r="C380" s="0" t="s">
+      <c r="C380" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="D380" s="0" t="n">
+      <c r="D380" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="E380" s="0" t="n">
+      <c r="E380" s="6" t="n">
         <v>0.091</v>
       </c>
     </row>
-    <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A381" s="11" t="n">
+    <row r="381" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A381" s="7" t="n">
+        <v>0.00079145</v>
+      </c>
+      <c r="B381" s="7" t="n">
+        <v>0.00048157</v>
+      </c>
+      <c r="C381" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="D381" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="E381" s="8" t="n">
+        <v>0.488</v>
+      </c>
+      <c r="F381" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="382" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A382" s="5" t="n">
         <v>8.5191E-005</v>
       </c>
-      <c r="B381" s="11" t="n">
+      <c r="B382" s="5" t="n">
         <v>0.0012959</v>
       </c>
-      <c r="C381" s="0" t="s">
-        <v>357</v>
-      </c>
-      <c r="D381" s="0" t="n">
+      <c r="C382" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="D382" s="6" t="n">
         <v>14</v>
       </c>
-    </row>
-    <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A382" s="11" t="n">
-        <v>0.00010569</v>
-      </c>
-      <c r="B382" s="11" t="n">
-        <v>0.030448</v>
-      </c>
-      <c r="C382" s="0" t="s">
+      <c r="E382" s="6" t="n">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="383" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A383" s="7" t="n">
+        <v>0.00041831</v>
+      </c>
+      <c r="B383" s="7" t="n">
+        <v>0.0025948</v>
+      </c>
+      <c r="C383" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="D383" s="8" t="n">
+        <v>18</v>
+      </c>
+      <c r="E383" s="8" t="n">
+        <v>0.286</v>
+      </c>
+      <c r="F383" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="D382" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A383" s="11" t="n">
-        <v>0.00013934</v>
-      </c>
-      <c r="B383" s="11" t="n">
-        <v>0.094741</v>
-      </c>
-      <c r="C383" s="0" t="s">
-        <v>359</v>
-      </c>
-      <c r="D383" s="0" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A384" s="11" t="n">
-        <v>0.00029152</v>
-      </c>
-      <c r="B384" s="11" t="n">
-        <v>0.0050044</v>
-      </c>
-      <c r="C384" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="D384" s="0" t="n">
-        <v>17</v>
+    </row>
+    <row r="384" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A384" s="7" t="n">
+        <v>0.00043116</v>
+      </c>
+      <c r="B384" s="7" t="n">
+        <v>0.0033583</v>
+      </c>
+      <c r="C384" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="D384" s="8" t="n">
+        <v>19</v>
+      </c>
+      <c r="E384" s="8" t="n">
+        <v>0.399</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="11" t="n">
-        <v>0.00041831</v>
+        <v>0.00029152</v>
       </c>
       <c r="B385" s="11" t="n">
-        <v>0.0025948</v>
+        <v>0.0050044</v>
       </c>
       <c r="C385" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D385" s="0" t="n">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="E385" s="0" t="n">
+        <v>0.122</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="11" t="n">
-        <v>0.00043116</v>
+        <v>0.00010569</v>
       </c>
       <c r="B386" s="11" t="n">
-        <v>0.0033583</v>
+        <v>0.030448</v>
       </c>
       <c r="C386" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D386" s="0" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A387" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="E386" s="0" t="n">
+        <v>0.138</v>
+      </c>
+    </row>
+    <row r="387" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A387" s="7" t="n">
         <v>0.00044228</v>
       </c>
-      <c r="B387" s="11" t="n">
+      <c r="B387" s="7" t="n">
         <v>0.039525</v>
       </c>
-      <c r="C387" s="0" t="s">
-        <v>363</v>
-      </c>
-      <c r="D387" s="0" t="n">
+      <c r="C387" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="D387" s="8" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A388" s="11" t="n">
-        <v>0.00079145</v>
-      </c>
-      <c r="B388" s="11" t="n">
-        <v>0.00048157</v>
-      </c>
-      <c r="C388" s="0" t="s">
-        <v>364</v>
-      </c>
-      <c r="D388" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="E388" s="0" t="n">
-        <v>0.488</v>
-      </c>
-      <c r="F388" s="0" t="s">
+      <c r="E387" s="8" t="n">
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="388" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A388" s="5" t="n">
+        <v>0.00013934</v>
+      </c>
+      <c r="B388" s="5" t="n">
+        <v>0.094741</v>
+      </c>
+      <c r="C388" s="6" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A389" s="11" t="n">
+      <c r="D388" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="E388" s="6" t="n">
+        <v>0.103</v>
+      </c>
+      <c r="F388" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="389" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A389" s="5" t="n">
         <v>0.0010816</v>
       </c>
-      <c r="B389" s="11" t="n">
+      <c r="B389" s="5" t="n">
         <v>0.00022451</v>
       </c>
-      <c r="C389" s="0" t="s">
-        <v>366</v>
-      </c>
-      <c r="D389" s="0" t="n">
+      <c r="C389" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="D389" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="E389" s="0" t="n">
+      <c r="E389" s="6" t="n">
         <v>0.102</v>
       </c>
-      <c r="F389" s="0" t="s">
-        <v>365</v>
+      <c r="F389" s="6" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="390" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9682,7 +10018,7 @@
         <v>0.020617</v>
       </c>
       <c r="C390" s="6" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="D390" s="6" t="n">
         <v>23</v>
@@ -9702,7 +10038,7 @@
         <v>0.0010824</v>
       </c>
       <c r="C391" s="6" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D391" s="6" t="n">
         <v>24</v>
@@ -9722,7 +10058,7 @@
         <v>0.0085214</v>
       </c>
       <c r="C392" s="6" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D392" s="6" t="n">
         <v>25</v>
@@ -9742,7 +10078,7 @@
         <v>0.084653</v>
       </c>
       <c r="C393" s="6" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D393" s="6" t="n">
         <v>26</v>
@@ -9762,7 +10098,7 @@
         <v>0.013976</v>
       </c>
       <c r="C394" s="6" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D394" s="6" t="n">
         <v>27</v>
@@ -9782,7 +10118,7 @@
         <v>0.0086208</v>
       </c>
       <c r="C395" s="6" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D395" s="6" t="n">
         <v>28</v>
@@ -9802,7 +10138,7 @@
         <v>0.001198</v>
       </c>
       <c r="C396" s="6" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D396" s="6" t="n">
         <v>29</v>
@@ -9822,7 +10158,7 @@
         <v>0.0016733</v>
       </c>
       <c r="C397" s="6" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D397" s="6" t="n">
         <v>30</v>
@@ -9866,54 +10202,54 @@
       </c>
       <c r="G400" s="4"/>
     </row>
-    <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A401" s="11" t="n">
+    <row r="401" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A401" s="5" t="n">
         <v>1.0028E-005</v>
       </c>
-      <c r="B401" s="11" t="n">
+      <c r="B401" s="5" t="n">
         <v>0.081537</v>
       </c>
-      <c r="C401" s="0" t="s">
-        <v>375</v>
-      </c>
-      <c r="D401" s="0" t="n">
+      <c r="C401" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="D401" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="E401" s="0" t="n">
+      <c r="E401" s="6" t="n">
         <v>0.125</v>
       </c>
     </row>
-    <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A402" s="11" t="n">
+    <row r="402" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A402" s="5" t="n">
         <v>2.154E-005</v>
       </c>
-      <c r="B402" s="11" t="n">
+      <c r="B402" s="5" t="n">
         <v>0.00026455</v>
       </c>
-      <c r="C402" s="0" t="s">
-        <v>376</v>
-      </c>
-      <c r="D402" s="0" t="n">
+      <c r="C402" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="D402" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="E402" s="0" t="n">
+      <c r="E402" s="6" t="n">
         <v>0.033</v>
       </c>
     </row>
-    <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A403" s="11" t="n">
+    <row r="403" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A403" s="5" t="n">
         <v>5.5079E-005</v>
       </c>
-      <c r="B403" s="11" t="n">
+      <c r="B403" s="5" t="n">
         <v>0.036404</v>
       </c>
-      <c r="C403" s="0" t="s">
-        <v>377</v>
-      </c>
-      <c r="D403" s="0" t="n">
+      <c r="C403" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="D403" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="E403" s="0" t="n">
+      <c r="E403" s="6" t="n">
         <v>0.12</v>
       </c>
     </row>
@@ -9925,7 +10261,7 @@
         <v>0.0080256</v>
       </c>
       <c r="C404" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D404" s="0" t="n">
         <v>9</v>
@@ -9934,158 +10270,194 @@
         <v>0.174</v>
       </c>
     </row>
-    <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A405" s="11" t="n">
+    <row r="405" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A405" s="5" t="n">
         <v>0.00010212</v>
       </c>
-      <c r="B405" s="11" t="n">
+      <c r="B405" s="5" t="n">
         <v>0.00015942</v>
       </c>
-      <c r="C405" s="0" t="s">
-        <v>379</v>
-      </c>
-      <c r="D405" s="0" t="n">
+      <c r="C405" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="D405" s="6" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A406" s="11" t="n">
-        <v>0.0001585</v>
-      </c>
-      <c r="B406" s="11" t="n">
-        <v>0.045676</v>
-      </c>
-      <c r="C406" s="0" t="s">
-        <v>380</v>
-      </c>
-      <c r="D406" s="0" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A407" s="11" t="n">
-        <v>0.00016235</v>
-      </c>
-      <c r="B407" s="11" t="n">
-        <v>0.00034318</v>
-      </c>
-      <c r="C407" s="0" t="s">
+      <c r="E405" s="6" t="n">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="406" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A406" s="5" t="n">
+        <v>0.0026695</v>
+      </c>
+      <c r="B406" s="5" t="n">
+        <v>0.00018241</v>
+      </c>
+      <c r="C406" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="D407" s="0" t="n">
-        <v>12</v>
+      <c r="D406" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="E406" s="6" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="F406" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="407" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A407" s="7" t="n">
+        <v>0.00061616</v>
+      </c>
+      <c r="B407" s="7" t="n">
+        <v>0.00027012</v>
+      </c>
+      <c r="C407" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="D407" s="8" t="n">
+        <v>15</v>
+      </c>
+      <c r="E407" s="8" t="n">
+        <v>0.278</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="11" t="n">
-        <v>0.00038783</v>
+        <v>0.00016235</v>
       </c>
       <c r="B408" s="11" t="n">
-        <v>0.013443</v>
+        <v>0.00034318</v>
       </c>
       <c r="C408" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D408" s="0" t="n">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="E408" s="0" t="n">
+        <v>0.222</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="11" t="n">
-        <v>0.00057614</v>
+        <v>0.000815</v>
       </c>
       <c r="B409" s="11" t="n">
-        <v>0.0075124</v>
+        <v>0.00036079</v>
       </c>
       <c r="C409" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D409" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A410" s="11" t="n">
-        <v>0.00061616</v>
-      </c>
-      <c r="B410" s="11" t="n">
-        <v>0.00027012</v>
-      </c>
-      <c r="C410" s="0" t="s">
-        <v>384</v>
-      </c>
-      <c r="D410" s="0" t="n">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="E409" s="0" t="n">
+        <v>0.147</v>
+      </c>
+    </row>
+    <row r="410" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A410" s="7" t="n">
+        <v>0.00092065</v>
+      </c>
+      <c r="B410" s="7" t="n">
+        <v>0.00072963</v>
+      </c>
+      <c r="C410" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="D410" s="8" t="n">
+        <v>17</v>
+      </c>
+      <c r="E410" s="8" t="n">
+        <v>0.312</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="11" t="n">
-        <v>0.000815</v>
+        <v>0.0020659</v>
       </c>
       <c r="B411" s="11" t="n">
-        <v>0.00036079</v>
+        <v>0.0010293</v>
       </c>
       <c r="C411" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="D411" s="0" t="n">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="E411" s="0" t="n">
+        <v>0.216</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="11" t="n">
-        <v>0.00092065</v>
+        <v>0.00057614</v>
       </c>
       <c r="B412" s="11" t="n">
-        <v>0.00072963</v>
+        <v>0.0075124</v>
       </c>
       <c r="C412" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D412" s="0" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A413" s="11" t="n">
-        <v>0.0020659</v>
-      </c>
-      <c r="B413" s="11" t="n">
-        <v>0.0010293</v>
-      </c>
-      <c r="C413" s="0" t="s">
-        <v>387</v>
-      </c>
-      <c r="D413" s="0" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A414" s="11" t="n">
-        <v>0.0026695</v>
-      </c>
-      <c r="B414" s="11" t="n">
-        <v>0.00018241</v>
-      </c>
-      <c r="C414" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E412" s="0" t="n">
+        <v>0.236</v>
+      </c>
+    </row>
+    <row r="413" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A413" s="7" t="n">
+        <v>0.0027193</v>
+      </c>
+      <c r="B413" s="7" t="n">
+        <v>0.0088273</v>
+      </c>
+      <c r="C413" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="D414" s="0" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A415" s="11" t="n">
-        <v>0.0027193</v>
-      </c>
-      <c r="B415" s="11" t="n">
-        <v>0.0088273</v>
-      </c>
-      <c r="C415" s="0" t="s">
+      <c r="D413" s="8" t="n">
+        <v>20</v>
+      </c>
+      <c r="E413" s="8" t="n">
+        <v>0.247</v>
+      </c>
+    </row>
+    <row r="414" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A414" s="7" t="n">
+        <v>0.00038783</v>
+      </c>
+      <c r="B414" s="7" t="n">
+        <v>0.013443</v>
+      </c>
+      <c r="C414" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="D415" s="0" t="n">
-        <v>20</v>
+      <c r="D414" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="E414" s="8" t="n">
+        <v>0.247</v>
+      </c>
+    </row>
+    <row r="415" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A415" s="7" t="n">
+        <v>0.0001585</v>
+      </c>
+      <c r="B415" s="7" t="n">
+        <v>0.045676</v>
+      </c>
+      <c r="C415" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="D415" s="8" t="n">
+        <v>11</v>
+      </c>
+      <c r="E415" s="8" t="n">
+        <v>0.296</v>
       </c>
     </row>
     <row r="416" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10096,7 +10468,7 @@
         <v>0.084736</v>
       </c>
       <c r="C416" s="6" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D416" s="6" t="n">
         <v>21</v>
@@ -10116,7 +10488,7 @@
         <v>0.053103</v>
       </c>
       <c r="C417" s="6" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D417" s="6" t="n">
         <v>22</v>
@@ -10136,7 +10508,7 @@
         <v>0.0021064</v>
       </c>
       <c r="C418" s="6" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D418" s="6" t="n">
         <v>23</v>
@@ -10156,7 +10528,7 @@
         <v>0.038518</v>
       </c>
       <c r="C419" s="6" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D419" s="6" t="n">
         <v>24</v>
@@ -10176,7 +10548,7 @@
         <v>0.0017141</v>
       </c>
       <c r="C420" s="6" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D420" s="6" t="n">
         <v>25</v>
@@ -10196,7 +10568,7 @@
         <v>0.0020659</v>
       </c>
       <c r="C421" s="6" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="D421" s="6" t="n">
         <v>26</v>
@@ -10216,7 +10588,7 @@
         <v>0.0026181</v>
       </c>
       <c r="C422" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D422" s="6" t="n">
         <v>27</v>
@@ -10236,7 +10608,7 @@
         <v>0.00048946</v>
       </c>
       <c r="C423" s="6" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D423" s="6" t="n">
         <v>28</v>
@@ -10256,7 +10628,7 @@
         <v>0.0038405</v>
       </c>
       <c r="C424" s="6" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D424" s="6" t="n">
         <v>29</v>
@@ -10276,7 +10648,7 @@
         <v>0.00055617</v>
       </c>
       <c r="C425" s="6" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D425" s="6" t="n">
         <v>30</v>
@@ -10320,37 +10692,37 @@
       </c>
       <c r="G428" s="4"/>
     </row>
-    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A429" s="11" t="n">
+    <row r="429" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A429" s="5" t="n">
         <v>4.4833E-005</v>
       </c>
-      <c r="B429" s="11" t="n">
+      <c r="B429" s="5" t="n">
         <v>0.00035603</v>
       </c>
-      <c r="C429" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="D429" s="0" t="n">
+      <c r="C429" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="D429" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="E429" s="0" t="n">
+      <c r="E429" s="6" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A430" s="11" t="n">
+    <row r="430" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A430" s="5" t="n">
         <v>4.8588E-005</v>
       </c>
-      <c r="B430" s="11" t="n">
+      <c r="B430" s="5" t="n">
         <v>0.00022552</v>
       </c>
-      <c r="C430" s="0" t="s">
-        <v>401</v>
-      </c>
-      <c r="D430" s="0" t="n">
+      <c r="C430" s="6" t="s">
+        <v>402</v>
+      </c>
+      <c r="D430" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="E430" s="0" t="n">
+      <c r="E430" s="6" t="n">
         <v>0.12</v>
       </c>
     </row>
@@ -10362,178 +10734,229 @@
         <v>0.019546</v>
       </c>
       <c r="C431" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D431" s="0" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A432" s="11" t="n">
+      <c r="E431" s="0" t="n">
+        <v>0.161</v>
+      </c>
+    </row>
+    <row r="432" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A432" s="5" t="n">
         <v>0.00012792</v>
       </c>
-      <c r="B432" s="11" t="n">
+      <c r="B432" s="5" t="n">
         <v>0.00013883</v>
       </c>
-      <c r="C432" s="0" t="s">
-        <v>403</v>
-      </c>
-      <c r="D432" s="0" t="n">
+      <c r="C432" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="D432" s="6" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A433" s="11" t="n">
-        <v>0.00018996</v>
-      </c>
-      <c r="B433" s="11" t="n">
-        <v>0.02095</v>
-      </c>
-      <c r="C433" s="0" t="s">
-        <v>404</v>
-      </c>
-      <c r="D433" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="11" t="n">
-        <v>0.00052525</v>
-      </c>
-      <c r="B434" s="11" t="n">
-        <v>0.062916</v>
-      </c>
-      <c r="C434" s="0" t="s">
+      <c r="E432" s="6" t="n">
+        <v>0.042</v>
+      </c>
+    </row>
+    <row r="433" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A433" s="7" t="n">
+        <v>0.0023426</v>
+      </c>
+      <c r="B433" s="7" t="n">
+        <v>0.00048386</v>
+      </c>
+      <c r="C433" s="8" t="s">
         <v>405</v>
       </c>
-      <c r="D434" s="0" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="11" t="n">
+      <c r="D433" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="E433" s="8" t="n">
+        <v>0.276</v>
+      </c>
+    </row>
+    <row r="434" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A434" s="5" t="n">
+        <v>0.0023119</v>
+      </c>
+      <c r="B434" s="5" t="n">
+        <v>0.0031136</v>
+      </c>
+      <c r="C434" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="D434" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="E434" s="6" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="435" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A435" s="7" t="n">
+        <v>0.0013616</v>
+      </c>
+      <c r="B435" s="7" t="n">
+        <v>0.0045854</v>
+      </c>
+      <c r="C435" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="D435" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="E435" s="8" t="n">
+        <v>0.339</v>
+      </c>
+      <c r="F435" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="436" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A436" s="7" t="n">
+        <v>0.0014138</v>
+      </c>
+      <c r="B436" s="7" t="n">
+        <v>0.01921</v>
+      </c>
+      <c r="C436" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="D436" s="8" t="n">
+        <v>14</v>
+      </c>
+      <c r="E436" s="8" t="n">
+        <v>0.289</v>
+      </c>
+    </row>
+    <row r="437" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A437" s="7" t="n">
         <v>0.0010185</v>
       </c>
-      <c r="B435" s="11" t="n">
+      <c r="B437" s="7" t="n">
         <v>0.02068</v>
       </c>
-      <c r="C435" s="0" t="s">
-        <v>406</v>
-      </c>
-      <c r="D435" s="0" t="n">
+      <c r="C437" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="D437" s="8" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A436" s="11" t="n">
-        <v>0.0013616</v>
-      </c>
-      <c r="B436" s="11" t="n">
-        <v>0.0045854</v>
-      </c>
-      <c r="C436" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="D436" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A437" s="11" t="n">
-        <v>0.0014138</v>
-      </c>
-      <c r="B437" s="11" t="n">
-        <v>0.01921</v>
-      </c>
-      <c r="C437" s="0" t="s">
-        <v>408</v>
-      </c>
-      <c r="D437" s="0" t="n">
-        <v>14</v>
+      <c r="E437" s="8" t="n">
+        <v>0.286</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="11" t="n">
-        <v>0.0023119</v>
+        <v>0.00018996</v>
       </c>
       <c r="B438" s="11" t="n">
-        <v>0.0031136</v>
+        <v>0.02095</v>
       </c>
       <c r="C438" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D438" s="0" t="n">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="E438" s="0" t="n">
+        <v>0.204</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="11" t="n">
-        <v>0.0023426</v>
+        <v>0.00052525</v>
       </c>
       <c r="B439" s="11" t="n">
-        <v>0.00048386</v>
+        <v>0.062916</v>
       </c>
       <c r="C439" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D439" s="0" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A440" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="E439" s="0" t="n">
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="440" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A440" s="5" t="n">
         <v>0.002477</v>
       </c>
-      <c r="B440" s="11" t="n">
+      <c r="B440" s="5" t="n">
         <v>0.04752</v>
       </c>
-      <c r="C440" s="0" t="s">
-        <v>411</v>
-      </c>
-      <c r="D440" s="0" t="n">
+      <c r="C440" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="D440" s="6" t="n">
         <v>17</v>
       </c>
-    </row>
-    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A441" s="11" t="n">
+      <c r="E440" s="6" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="F440" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="441" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A441" s="5" t="n">
         <v>0.0029472</v>
       </c>
-      <c r="B441" s="11" t="n">
+      <c r="B441" s="5" t="n">
         <v>0.0062512</v>
       </c>
-      <c r="C441" s="0" t="s">
-        <v>412</v>
-      </c>
-      <c r="D441" s="0" t="n">
+      <c r="C441" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="D441" s="6" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A442" s="11" t="n">
+      <c r="E441" s="6" t="n">
+        <v>0.054</v>
+      </c>
+    </row>
+    <row r="442" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A442" s="5" t="n">
         <v>0.0033207</v>
       </c>
-      <c r="B442" s="11" t="n">
+      <c r="B442" s="5" t="n">
         <v>0.00062416</v>
       </c>
-      <c r="C442" s="0" t="s">
-        <v>413</v>
-      </c>
-      <c r="D442" s="0" t="n">
+      <c r="C442" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="D442" s="6" t="n">
         <v>19</v>
       </c>
-    </row>
-    <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A443" s="11" t="n">
+      <c r="E442" s="6" t="n">
+        <v>0.435</v>
+      </c>
+      <c r="F442" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="443" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A443" s="5" t="n">
         <v>0.0060778</v>
       </c>
-      <c r="B443" s="11" t="n">
+      <c r="B443" s="5" t="n">
         <v>0.0088268</v>
       </c>
-      <c r="C443" s="0" t="s">
-        <v>414</v>
-      </c>
-      <c r="D443" s="0" t="n">
+      <c r="C443" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="D443" s="6" t="n">
         <v>20</v>
+      </c>
+      <c r="E443" s="6" t="n">
+        <v>0.579</v>
+      </c>
+      <c r="F443" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="444" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10544,7 +10967,7 @@
         <v>0.00011799</v>
       </c>
       <c r="C444" s="6" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D444" s="6" t="n">
         <v>21</v>
@@ -10564,7 +10987,7 @@
         <v>0.00087168</v>
       </c>
       <c r="C445" s="6" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D445" s="6" t="n">
         <v>22</v>
@@ -10584,7 +11007,7 @@
         <v>0.0090079</v>
       </c>
       <c r="C446" s="6" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="D446" s="6" t="n">
         <v>23</v>
@@ -10604,7 +11027,7 @@
         <v>0.0040595</v>
       </c>
       <c r="C447" s="6" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D447" s="6" t="n">
         <v>24</v>
@@ -10624,7 +11047,7 @@
         <v>0.0082223</v>
       </c>
       <c r="C448" s="6" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D448" s="6" t="n">
         <v>25</v>
@@ -10644,7 +11067,7 @@
         <v>0.0075781</v>
       </c>
       <c r="C449" s="6" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D449" s="6" t="n">
         <v>26</v>
@@ -10664,7 +11087,7 @@
         <v>0.027969</v>
       </c>
       <c r="C450" s="6" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D450" s="6" t="n">
         <v>27</v>
@@ -10684,7 +11107,7 @@
         <v>0.041283</v>
       </c>
       <c r="C451" s="6" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D451" s="6" t="n">
         <v>28</v>
@@ -10704,7 +11127,7 @@
         <v>0.00032859</v>
       </c>
       <c r="C452" s="6" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="D452" s="6" t="n">
         <v>29</v>
@@ -10724,7 +11147,7 @@
         <v>0.029059</v>
       </c>
       <c r="C453" s="6" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D453" s="6" t="n">
         <v>30</v>
@@ -10775,7 +11198,7 @@
         <v>0.03</v>
       </c>
       <c r="C457" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D457" s="0" t="n">
         <v>6</v>
@@ -10785,40 +11208,68 @@
       </c>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A458" s="11"/>
-      <c r="B458" s="11"/>
+      <c r="A458" s="11" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="B458" s="11" t="n">
+        <v>0.04</v>
+      </c>
       <c r="C458" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
+      </c>
+      <c r="D458" s="0" t="n">
+        <v>7</v>
       </c>
       <c r="F458" s="0" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A459" s="11"/>
-      <c r="B459" s="11"/>
+      <c r="A459" s="11" t="n">
+        <v>9E-005</v>
+      </c>
+      <c r="B459" s="11" t="n">
+        <v>0.005</v>
+      </c>
       <c r="C459" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
+      </c>
+      <c r="D459" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="F459" s="0" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A460" s="11"/>
-      <c r="B460" s="11"/>
+      <c r="A460" s="11" t="n">
+        <v>0.0006</v>
+      </c>
+      <c r="B460" s="11" t="n">
+        <v>0.008</v>
+      </c>
       <c r="C460" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
+      </c>
+      <c r="D460" s="0" t="n">
+        <v>9</v>
       </c>
       <c r="F460" s="0" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A461" s="11"/>
-      <c r="B461" s="11"/>
+      <c r="A461" s="11" t="n">
+        <v>0.0006</v>
+      </c>
+      <c r="B461" s="11" t="n">
+        <v>0.01</v>
+      </c>
       <c r="C461" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
+      </c>
+      <c r="D461" s="0" t="n">
+        <v>10</v>
       </c>
       <c r="F461" s="0" t="s">
         <v>291</v>
@@ -10826,7 +11277,7 @@
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="12" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B463" s="12"/>
       <c r="C463" s="12"/>
@@ -10845,7 +11296,7 @@
         <v>48</v>
       </c>
       <c r="B465" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="G465" s="0" t="s">
         <v>175</v>
@@ -10856,7 +11307,7 @@
         <v>3</v>
       </c>
       <c r="B466" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10891,8 +11342,1622 @@
       </c>
       <c r="G469" s="4"/>
     </row>
+    <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A470" s="11" t="n">
+        <v>1.6546E-005</v>
+      </c>
+      <c r="B470" s="11" t="n">
+        <v>0.3364606</v>
+      </c>
+      <c r="C470" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="D470" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A471" s="11" t="n">
+        <v>2.1434E-005</v>
+      </c>
+      <c r="B471" s="11" t="n">
+        <v>0.0554675</v>
+      </c>
+      <c r="C471" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="D471" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A472" s="11" t="n">
+        <v>3.324E-005</v>
+      </c>
+      <c r="B472" s="11" t="n">
+        <v>0.0036334</v>
+      </c>
+      <c r="C472" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="D472" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A473" s="11" t="n">
+        <v>5.1531E-005</v>
+      </c>
+      <c r="B473" s="11" t="n">
+        <v>0.6906702</v>
+      </c>
+      <c r="C473" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="D473" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="11" t="n">
+        <v>6.4539E-005</v>
+      </c>
+      <c r="B474" s="11" t="n">
+        <v>0.0874128</v>
+      </c>
+      <c r="C474" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="D474" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A475" s="11" t="n">
+        <v>0.00010521</v>
+      </c>
+      <c r="B475" s="11" t="n">
+        <v>0.0066661</v>
+      </c>
+      <c r="C475" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="D475" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A476" s="11" t="n">
+        <v>0.00011148</v>
+      </c>
+      <c r="B476" s="11" t="n">
+        <v>0.3805353</v>
+      </c>
+      <c r="C476" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="D476" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A477" s="11" t="n">
+        <v>0.00016302</v>
+      </c>
+      <c r="B477" s="11" t="n">
+        <v>0.0937002</v>
+      </c>
+      <c r="C477" s="0" t="s">
+        <v>441</v>
+      </c>
+      <c r="D477" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A478" s="11" t="n">
+        <v>0.00040381</v>
+      </c>
+      <c r="B478" s="11" t="n">
+        <v>0.0021062</v>
+      </c>
+      <c r="C478" s="0" t="s">
+        <v>442</v>
+      </c>
+      <c r="D478" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A479" s="11" t="n">
+        <v>0.00047202</v>
+      </c>
+      <c r="B479" s="11" t="n">
+        <v>0.0056217</v>
+      </c>
+      <c r="C479" s="0" t="s">
+        <v>443</v>
+      </c>
+      <c r="D479" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A480" s="11" t="n">
+        <v>0.00072969</v>
+      </c>
+      <c r="B480" s="11" t="n">
+        <v>0.150206</v>
+      </c>
+      <c r="C480" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="D480" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A481" s="11" t="n">
+        <v>0.00078044</v>
+      </c>
+      <c r="B481" s="11" t="n">
+        <v>0.4237876</v>
+      </c>
+      <c r="C481" s="0" t="s">
+        <v>445</v>
+      </c>
+      <c r="D481" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A482" s="11" t="n">
+        <v>0.0010278</v>
+      </c>
+      <c r="B482" s="11" t="n">
+        <v>0.0097653</v>
+      </c>
+      <c r="C482" s="0" t="s">
+        <v>446</v>
+      </c>
+      <c r="D482" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A483" s="11" t="n">
+        <v>0.0016154</v>
+      </c>
+      <c r="B483" s="11" t="n">
+        <v>0.0042225</v>
+      </c>
+      <c r="C483" s="0" t="s">
+        <v>447</v>
+      </c>
+      <c r="D483" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A484" s="11" t="n">
+        <v>0.0019026</v>
+      </c>
+      <c r="B484" s="11" t="n">
+        <v>0.0010762</v>
+      </c>
+      <c r="C484" s="0" t="s">
+        <v>448</v>
+      </c>
+      <c r="D484" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A485" s="11" t="n">
+        <v>0.0034332</v>
+      </c>
+      <c r="B485" s="11" t="n">
+        <v>0.7402161</v>
+      </c>
+      <c r="C485" s="0" t="s">
+        <v>449</v>
+      </c>
+      <c r="D485" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A486" s="11" t="n">
+        <v>0.0053245</v>
+      </c>
+      <c r="B486" s="11" t="n">
+        <v>0.0172276</v>
+      </c>
+      <c r="C486" s="0" t="s">
+        <v>450</v>
+      </c>
+      <c r="D486" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A487" s="11" t="n">
+        <v>0.0065557</v>
+      </c>
+      <c r="B487" s="11" t="n">
+        <v>0.0026726</v>
+      </c>
+      <c r="C487" s="0" t="s">
+        <v>451</v>
+      </c>
+      <c r="D487" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E487" s="0" t="n">
+        <v>0.124</v>
+      </c>
+      <c r="F487" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A488" s="11" t="n">
+        <v>0.0079053</v>
+      </c>
+      <c r="B488" s="11" t="n">
+        <v>0.003742</v>
+      </c>
+      <c r="C488" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="D488" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="E488" s="0" t="n">
+        <v>0.142</v>
+      </c>
+      <c r="F488" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A489" s="11" t="n">
+        <v>0.008589</v>
+      </c>
+      <c r="B489" s="11" t="n">
+        <v>0.6753151</v>
+      </c>
+      <c r="C489" s="0" t="s">
+        <v>453</v>
+      </c>
+      <c r="D489" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E489" s="0" t="n">
+        <v>0.424</v>
+      </c>
+      <c r="F489" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A491" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="B491" s="13"/>
+      <c r="C491" s="13"/>
+      <c r="D491" s="13"/>
+      <c r="E491" s="13"/>
+      <c r="F491" s="13"/>
+      <c r="G491" s="13"/>
+    </row>
+    <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A492" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B492" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C492" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D492" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E492" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F492" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G492" s="4"/>
+    </row>
+    <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A493" s="11" t="n">
+        <v>1.5675E-005</v>
+      </c>
+      <c r="B493" s="11" t="n">
+        <v>0.0028178</v>
+      </c>
+      <c r="C493" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="D493" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A494" s="11" t="n">
+        <v>2.5329E-005</v>
+      </c>
+      <c r="B494" s="11" t="n">
+        <v>0.0018946</v>
+      </c>
+      <c r="C494" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="D494" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A495" s="11" t="n">
+        <v>2.7433E-005</v>
+      </c>
+      <c r="B495" s="11" t="n">
+        <v>0.0966219</v>
+      </c>
+      <c r="C495" s="0" t="s">
+        <v>456</v>
+      </c>
+      <c r="D495" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A496" s="11" t="n">
+        <v>3.2859E-005</v>
+      </c>
+      <c r="B496" s="11" t="n">
+        <v>0.0051958</v>
+      </c>
+      <c r="C496" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="D496" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A497" s="11" t="n">
+        <v>3.7739E-005</v>
+      </c>
+      <c r="B497" s="11" t="n">
+        <v>0.0043637</v>
+      </c>
+      <c r="C497" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="D497" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A498" s="11" t="n">
+        <v>3.9702E-005</v>
+      </c>
+      <c r="B498" s="11" t="n">
+        <v>0.0312187</v>
+      </c>
+      <c r="C498" s="0" t="s">
+        <v>459</v>
+      </c>
+      <c r="D498" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A499" s="11" t="n">
+        <v>4.589E-005</v>
+      </c>
+      <c r="B499" s="11" t="n">
+        <v>0.1905453</v>
+      </c>
+      <c r="C499" s="0" t="s">
+        <v>460</v>
+      </c>
+      <c r="D499" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A500" s="11" t="n">
+        <v>5.0586E-005</v>
+      </c>
+      <c r="B500" s="11" t="n">
+        <v>0.3139434</v>
+      </c>
+      <c r="C500" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="D500" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A501" s="11" t="n">
+        <v>5.232E-005</v>
+      </c>
+      <c r="B501" s="11" t="n">
+        <v>0.1373997</v>
+      </c>
+      <c r="C501" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="D501" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A502" s="11" t="n">
+        <v>5.8133E-005</v>
+      </c>
+      <c r="B502" s="11" t="n">
+        <v>0.314184</v>
+      </c>
+      <c r="C502" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="D502" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A503" s="11" t="n">
+        <v>7.2325E-005</v>
+      </c>
+      <c r="B503" s="11" t="n">
+        <v>0.0737628</v>
+      </c>
+      <c r="C503" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="D503" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A504" s="11" t="n">
+        <v>0.00012154</v>
+      </c>
+      <c r="B504" s="11" t="n">
+        <v>0.0101554</v>
+      </c>
+      <c r="C504" s="0" t="s">
+        <v>465</v>
+      </c>
+      <c r="D504" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A505" s="11" t="n">
+        <v>0.0001574</v>
+      </c>
+      <c r="B505" s="11" t="n">
+        <v>0.3136236</v>
+      </c>
+      <c r="C505" s="0" t="s">
+        <v>466</v>
+      </c>
+      <c r="D505" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A506" s="11" t="n">
+        <v>0.00018285</v>
+      </c>
+      <c r="B506" s="11" t="n">
+        <v>0.0011338</v>
+      </c>
+      <c r="C506" s="0" t="s">
+        <v>467</v>
+      </c>
+      <c r="D506" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A507" s="11" t="n">
+        <v>0.00019898</v>
+      </c>
+      <c r="B507" s="11" t="n">
+        <v>0.6018989</v>
+      </c>
+      <c r="C507" s="0" t="s">
+        <v>468</v>
+      </c>
+      <c r="D507" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A508" s="11" t="n">
+        <v>0.00073229</v>
+      </c>
+      <c r="B508" s="11" t="n">
+        <v>0.0913831</v>
+      </c>
+      <c r="C508" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="D508" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A509" s="11" t="n">
+        <v>0.0011529</v>
+      </c>
+      <c r="B509" s="11" t="n">
+        <v>0.0825684</v>
+      </c>
+      <c r="C509" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="D509" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A510" s="11" t="n">
+        <v>0.0029386</v>
+      </c>
+      <c r="B510" s="11" t="n">
+        <v>0.146197</v>
+      </c>
+      <c r="C510" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="D510" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E510" s="0" t="n">
+        <v>0.263</v>
+      </c>
+    </row>
+    <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A511" s="11" t="n">
+        <v>0.0034427</v>
+      </c>
+      <c r="B511" s="11" t="n">
+        <v>0.0017839</v>
+      </c>
+      <c r="C511" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="D511" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="E511" s="0" t="n">
+        <v>0.062</v>
+      </c>
+      <c r="F511" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A512" s="11" t="n">
+        <v>0.0046946</v>
+      </c>
+      <c r="B512" s="11" t="n">
+        <v>0.0240136</v>
+      </c>
+      <c r="C512" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="D512" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E512" s="0" t="n">
+        <v>0.474</v>
+      </c>
+      <c r="F512" s="0" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A514" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B514" s="13"/>
+      <c r="C514" s="13"/>
+      <c r="D514" s="13"/>
+      <c r="E514" s="13"/>
+      <c r="F514" s="13"/>
+      <c r="G514" s="13"/>
+    </row>
+    <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A515" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B515" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C515" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D515" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E515" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F515" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A516" s="11" t="n">
+        <v>1.169E-005</v>
+      </c>
+      <c r="B516" s="11" t="n">
+        <v>0.0089262</v>
+      </c>
+      <c r="C516" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="D516" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A517" s="11" t="n">
+        <v>1.4089E-005</v>
+      </c>
+      <c r="B517" s="11" t="n">
+        <v>0.0015234</v>
+      </c>
+      <c r="C517" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="D517" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A518" s="11" t="n">
+        <v>1.8107E-005</v>
+      </c>
+      <c r="B518" s="11" t="n">
+        <v>0.5553683</v>
+      </c>
+      <c r="C518" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="D518" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A519" s="11" t="n">
+        <v>2.363E-005</v>
+      </c>
+      <c r="B519" s="11" t="n">
+        <v>0.0520492</v>
+      </c>
+      <c r="C519" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="D519" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A520" s="11" t="n">
+        <v>0.0001042</v>
+      </c>
+      <c r="B520" s="11" t="n">
+        <v>0.0697921</v>
+      </c>
+      <c r="C520" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="D520" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A521" s="11" t="n">
+        <v>0.00015067</v>
+      </c>
+      <c r="B521" s="11" t="n">
+        <v>0.0623434</v>
+      </c>
+      <c r="C521" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="D521" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A522" s="11" t="n">
+        <v>0.00020506</v>
+      </c>
+      <c r="B522" s="11" t="n">
+        <v>0.7336958</v>
+      </c>
+      <c r="C522" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="D522" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A523" s="11" t="n">
+        <v>0.00034951</v>
+      </c>
+      <c r="B523" s="11" t="n">
+        <v>0.3123063</v>
+      </c>
+      <c r="C523" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="D523" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A524" s="11" t="n">
+        <v>0.0003727</v>
+      </c>
+      <c r="B524" s="11" t="n">
+        <v>0.1619842</v>
+      </c>
+      <c r="C524" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="D524" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A525" s="11" t="n">
+        <v>0.00044525</v>
+      </c>
+      <c r="B525" s="11" t="n">
+        <v>0.0106163</v>
+      </c>
+      <c r="C525" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="D525" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A526" s="11" t="n">
+        <v>0.00054573</v>
+      </c>
+      <c r="B526" s="11" t="n">
+        <v>0.0043901</v>
+      </c>
+      <c r="C526" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="D526" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A527" s="11" t="n">
+        <v>0.00092296</v>
+      </c>
+      <c r="B527" s="11" t="n">
+        <v>0.5681399</v>
+      </c>
+      <c r="C527" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="D527" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A528" s="11" t="n">
+        <v>0.00099429</v>
+      </c>
+      <c r="B528" s="11" t="n">
+        <v>0.0030212</v>
+      </c>
+      <c r="C528" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="D528" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A529" s="11" t="n">
+        <v>0.0011866</v>
+      </c>
+      <c r="B529" s="11" t="n">
+        <v>0.1269318</v>
+      </c>
+      <c r="C529" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="D529" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A530" s="11" t="n">
+        <v>0.0014278</v>
+      </c>
+      <c r="B530" s="11" t="n">
+        <v>0.0553141</v>
+      </c>
+      <c r="C530" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="D530" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A531" s="11" t="n">
+        <v>0.0020741</v>
+      </c>
+      <c r="B531" s="11" t="n">
+        <v>0.0445031</v>
+      </c>
+      <c r="C531" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="D531" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A532" s="11" t="n">
+        <v>0.0029028</v>
+      </c>
+      <c r="B532" s="11" t="n">
+        <v>0.0127251</v>
+      </c>
+      <c r="C532" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="D532" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A533" s="11" t="n">
+        <v>0.0040751</v>
+      </c>
+      <c r="B533" s="11" t="n">
+        <v>0.0019656</v>
+      </c>
+      <c r="C533" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="D533" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E533" s="0" t="n">
+        <v>0.386</v>
+      </c>
+      <c r="F533" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A534" s="11" t="n">
+        <v>0.0052367</v>
+      </c>
+      <c r="B534" s="11" t="n">
+        <v>0.0011963</v>
+      </c>
+      <c r="C534" s="0" t="s">
+        <v>492</v>
+      </c>
+      <c r="D534" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="E534" s="0" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F534" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A535" s="11" t="n">
+        <v>0.00822</v>
+      </c>
+      <c r="B535" s="11" t="n">
+        <v>0.0017011</v>
+      </c>
+      <c r="C535" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="D535" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E535" s="0" t="n">
+        <v>0.066</v>
+      </c>
+      <c r="F535" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A537" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="B537" s="13"/>
+      <c r="C537" s="13"/>
+      <c r="D537" s="13"/>
+      <c r="E537" s="13"/>
+      <c r="F537" s="13"/>
+      <c r="G537" s="13"/>
+    </row>
+    <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A538" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B538" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C538" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D538" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E538" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F538" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G538" s="4"/>
+    </row>
+    <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A539" s="11" t="n">
+        <v>2.022E-005</v>
+      </c>
+      <c r="B539" s="11" t="n">
+        <v>0.1550242</v>
+      </c>
+      <c r="C539" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="D539" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A540" s="11" t="n">
+        <v>2.2628E-005</v>
+      </c>
+      <c r="B540" s="11" t="n">
+        <v>0.001751</v>
+      </c>
+      <c r="C540" s="0" t="s">
+        <v>495</v>
+      </c>
+      <c r="D540" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A541" s="11" t="n">
+        <v>2.5671E-005</v>
+      </c>
+      <c r="B541" s="11" t="n">
+        <v>0.0016059</v>
+      </c>
+      <c r="C541" s="0" t="s">
+        <v>496</v>
+      </c>
+      <c r="D541" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A542" s="11" t="n">
+        <v>4.1009E-005</v>
+      </c>
+      <c r="B542" s="11" t="n">
+        <v>0.0079769</v>
+      </c>
+      <c r="C542" s="0" t="s">
+        <v>497</v>
+      </c>
+      <c r="D542" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A543" s="11" t="n">
+        <v>5.1362E-005</v>
+      </c>
+      <c r="B543" s="11" t="n">
+        <v>0.2642545</v>
+      </c>
+      <c r="C543" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="D543" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A544" s="11" t="n">
+        <v>5.204E-005</v>
+      </c>
+      <c r="B544" s="11" t="n">
+        <v>0.8091169</v>
+      </c>
+      <c r="C544" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="D544" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A545" s="11" t="n">
+        <v>5.3496E-005</v>
+      </c>
+      <c r="B545" s="11" t="n">
+        <v>0.0633867</v>
+      </c>
+      <c r="C545" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="D545" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A546" s="11" t="n">
+        <v>9.3627E-005</v>
+      </c>
+      <c r="B546" s="11" t="n">
+        <v>0.0032802</v>
+      </c>
+      <c r="C546" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="D546" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A547" s="11" t="n">
+        <v>0.00019114</v>
+      </c>
+      <c r="B547" s="11" t="n">
+        <v>0.008914</v>
+      </c>
+      <c r="C547" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="D547" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A548" s="11" t="n">
+        <v>0.00036622</v>
+      </c>
+      <c r="B548" s="11" t="n">
+        <v>0.0052602</v>
+      </c>
+      <c r="C548" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="D548" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A549" s="11" t="n">
+        <v>0.00061699</v>
+      </c>
+      <c r="B549" s="11" t="n">
+        <v>0.6316548</v>
+      </c>
+      <c r="C549" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="D549" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A550" s="11" t="n">
+        <v>0.00068092</v>
+      </c>
+      <c r="B550" s="11" t="n">
+        <v>0.0193573</v>
+      </c>
+      <c r="C550" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="D550" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A551" s="11" t="n">
+        <v>0.00068623</v>
+      </c>
+      <c r="B551" s="11" t="n">
+        <v>0.0015879</v>
+      </c>
+      <c r="C551" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="D551" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A552" s="11" t="n">
+        <v>0.00081216</v>
+      </c>
+      <c r="B552" s="11" t="n">
+        <v>0.0437004</v>
+      </c>
+      <c r="C552" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="D552" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A553" s="11" t="n">
+        <v>0.001062</v>
+      </c>
+      <c r="B553" s="11" t="n">
+        <v>0.0033356</v>
+      </c>
+      <c r="C553" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="D553" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A554" s="11" t="n">
+        <v>0.0017452</v>
+      </c>
+      <c r="B554" s="11" t="n">
+        <v>0.0028573</v>
+      </c>
+      <c r="C554" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="D554" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A555" s="11" t="n">
+        <v>0.0029918</v>
+      </c>
+      <c r="B555" s="11" t="n">
+        <v>0.0570815</v>
+      </c>
+      <c r="C555" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="D555" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A556" s="11" t="n">
+        <v>0.0033841</v>
+      </c>
+      <c r="B556" s="11" t="n">
+        <v>0.0256605</v>
+      </c>
+      <c r="C556" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="D556" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E556" s="0" t="n">
+        <v>0.116</v>
+      </c>
+      <c r="F556" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A557" s="11" t="n">
+        <v>0.0049189</v>
+      </c>
+      <c r="B557" s="11" t="n">
+        <v>0.0066357</v>
+      </c>
+      <c r="C557" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="D557" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="E557" s="0" t="n">
+        <v>0.072</v>
+      </c>
+      <c r="F557" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A558" s="11" t="n">
+        <v>0.008357</v>
+      </c>
+      <c r="B558" s="11" t="n">
+        <v>0.0626824</v>
+      </c>
+      <c r="C558" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="D558" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E558" s="0" t="n">
+        <v>0.071</v>
+      </c>
+      <c r="F558" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A560" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="B560" s="13"/>
+      <c r="C560" s="13"/>
+      <c r="D560" s="13"/>
+      <c r="E560" s="13"/>
+      <c r="F560" s="13"/>
+      <c r="G560" s="13"/>
+    </row>
+    <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A561" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B561" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C561" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D561" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E561" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F561" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G561" s="4"/>
+    </row>
+    <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A562" s="11" t="n">
+        <v>1.1974E-005</v>
+      </c>
+      <c r="B562" s="11" t="n">
+        <v>0.8034868</v>
+      </c>
+      <c r="C562" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="D562" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A563" s="11" t="n">
+        <v>1.3593E-005</v>
+      </c>
+      <c r="B563" s="11" t="n">
+        <v>0.0631875</v>
+      </c>
+      <c r="C563" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="D563" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A564" s="11" t="n">
+        <v>2.4974E-005</v>
+      </c>
+      <c r="B564" s="11" t="n">
+        <v>0.0832902</v>
+      </c>
+      <c r="C564" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="D564" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A565" s="11" t="n">
+        <v>3.6482E-005</v>
+      </c>
+      <c r="B565" s="11" t="n">
+        <v>0.0013965</v>
+      </c>
+      <c r="C565" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="D565" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A566" s="11" t="n">
+        <v>6.1263E-005</v>
+      </c>
+      <c r="B566" s="11" t="n">
+        <v>0.7930285</v>
+      </c>
+      <c r="C566" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="D566" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A567" s="11" t="n">
+        <v>9.0421E-005</v>
+      </c>
+      <c r="B567" s="11" t="n">
+        <v>0.8374195</v>
+      </c>
+      <c r="C567" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="D567" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A568" s="11" t="n">
+        <v>9.7136E-005</v>
+      </c>
+      <c r="B568" s="11" t="n">
+        <v>0.3480775</v>
+      </c>
+      <c r="C568" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="D568" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A569" s="11" t="n">
+        <v>0.00012183</v>
+      </c>
+      <c r="B569" s="11" t="n">
+        <v>0.0086159</v>
+      </c>
+      <c r="C569" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="D569" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A570" s="11" t="n">
+        <v>0.0001276</v>
+      </c>
+      <c r="B570" s="11" t="n">
+        <v>0.0252616</v>
+      </c>
+      <c r="C570" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="D570" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A571" s="11" t="n">
+        <v>0.00013644</v>
+      </c>
+      <c r="B571" s="11" t="n">
+        <v>0.1866638</v>
+      </c>
+      <c r="C571" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="D571" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A572" s="11" t="n">
+        <v>0.00026674</v>
+      </c>
+      <c r="B572" s="11" t="n">
+        <v>0.0056232</v>
+      </c>
+      <c r="C572" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="D572" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A573" s="11" t="n">
+        <v>0.00029883</v>
+      </c>
+      <c r="B573" s="11" t="n">
+        <v>0.0288742</v>
+      </c>
+      <c r="C573" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="D573" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A574" s="11" t="n">
+        <v>0.0004866</v>
+      </c>
+      <c r="B574" s="11" t="n">
+        <v>0.1482461</v>
+      </c>
+      <c r="C574" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="D574" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A575" s="11" t="n">
+        <v>0.00051564</v>
+      </c>
+      <c r="B575" s="11" t="n">
+        <v>0.0964185</v>
+      </c>
+      <c r="C575" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="D575" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A576" s="11" t="n">
+        <v>0.00069454</v>
+      </c>
+      <c r="B576" s="11" t="n">
+        <v>0.0056318</v>
+      </c>
+      <c r="C576" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="D576" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A577" s="11" t="n">
+        <v>0.0011851</v>
+      </c>
+      <c r="B577" s="11" t="n">
+        <v>0.0295227</v>
+      </c>
+      <c r="C577" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="D577" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="578" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A578" s="11" t="n">
+        <v>0.0012842</v>
+      </c>
+      <c r="B578" s="11" t="n">
+        <v>0.1085323</v>
+      </c>
+      <c r="C578" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="D578" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A579" s="11" t="n">
+        <v>0.0027521</v>
+      </c>
+      <c r="B579" s="11" t="n">
+        <v>0.0084986</v>
+      </c>
+      <c r="C579" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="D579" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E579" s="0" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="F579" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A580" s="11" t="n">
+        <v>0.009611</v>
+      </c>
+      <c r="B580" s="11" t="n">
+        <v>0.0384803</v>
+      </c>
+      <c r="C580" s="0" t="s">
+        <v>532</v>
+      </c>
+      <c r="D580" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="E580" s="0" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="F580" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A581" s="11" t="n">
+        <v>0.0098824</v>
+      </c>
+      <c r="B581" s="11" t="n">
+        <v>0.0174164</v>
+      </c>
+      <c r="C581" s="0" t="s">
+        <v>533</v>
+      </c>
+      <c r="D581" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E581" s="0" t="n">
+        <v>0.083</v>
+      </c>
+      <c r="F581" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="32">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A41:K41"/>
@@ -10921,6 +12986,10 @@
     <mergeCell ref="A455:G455"/>
     <mergeCell ref="A463:G463"/>
     <mergeCell ref="A468:G468"/>
+    <mergeCell ref="A491:G491"/>
+    <mergeCell ref="A514:G514"/>
+    <mergeCell ref="A537:G537"/>
+    <mergeCell ref="A560:G560"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
hyperparameter results for the very last experiment :)
</commit_message>
<xml_diff>
--- a/experiments/hyperparameters/hyperparemeter_search.xlsx
+++ b/experiments/hyperparameters/hyperparemeter_search.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="22" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="11" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="755">
   <si>
     <t>EXPERIMENT 2_old</t>
   </si>
@@ -1970,54 +1970,54 @@
     <t>run565</t>
   </si>
   <si>
+    <t>run576</t>
+  </si>
+  <si>
+    <t>run578</t>
+  </si>
+  <si>
+    <t>run575</t>
+  </si>
+  <si>
+    <t>run568</t>
+  </si>
+  <si>
+    <t>run579</t>
+  </si>
+  <si>
+    <t>run572</t>
+  </si>
+  <si>
+    <t>run581</t>
+  </si>
+  <si>
+    <t>run571</t>
+  </si>
+  <si>
+    <t>run574</t>
+  </si>
+  <si>
+    <t>run567</t>
+  </si>
+  <si>
+    <t>run570</t>
+  </si>
+  <si>
+    <t>run573</t>
+  </si>
+  <si>
+    <t>run569</t>
+  </si>
+  <si>
     <t>run566</t>
   </si>
   <si>
-    <t>run567</t>
-  </si>
-  <si>
-    <t>run568</t>
-  </si>
-  <si>
-    <t>run569</t>
-  </si>
-  <si>
-    <t>run570</t>
-  </si>
-  <si>
-    <t>run571</t>
-  </si>
-  <si>
-    <t>run572</t>
-  </si>
-  <si>
-    <t>run573</t>
-  </si>
-  <si>
-    <t>run574</t>
-  </si>
-  <si>
-    <t>run575</t>
-  </si>
-  <si>
-    <t>run576</t>
-  </si>
-  <si>
     <t>run577</t>
   </si>
   <si>
-    <t>run578</t>
-  </si>
-  <si>
-    <t>run579</t>
-  </si>
-  <si>
     <t>run580</t>
   </si>
   <si>
-    <t>run581</t>
-  </si>
-  <si>
     <t>run582</t>
   </si>
   <si>
@@ -2027,33 +2027,33 @@
     <t>run584</t>
   </si>
   <si>
+    <t>run588</t>
+  </si>
+  <si>
+    <t>run589</t>
+  </si>
+  <si>
+    <t>run590</t>
+  </si>
+  <si>
     <t>run585</t>
   </si>
   <si>
+    <t>run592</t>
+  </si>
+  <si>
+    <t>run593</t>
+  </si>
+  <si>
+    <t>run587</t>
+  </si>
+  <si>
     <t>run586</t>
   </si>
   <si>
-    <t>run587</t>
-  </si>
-  <si>
-    <t>run588</t>
-  </si>
-  <si>
-    <t>run589</t>
-  </si>
-  <si>
-    <t>run590</t>
-  </si>
-  <si>
     <t>run591</t>
   </si>
   <si>
-    <t>run592</t>
-  </si>
-  <si>
-    <t>run593</t>
-  </si>
-  <si>
     <t>run594</t>
   </si>
   <si>
@@ -2084,48 +2084,48 @@
     <t>run603</t>
   </si>
   <si>
+    <t>run610</t>
+  </si>
+  <si>
+    <t>run613</t>
+  </si>
+  <si>
+    <t>run607</t>
+  </si>
+  <si>
+    <t>run609</t>
+  </si>
+  <si>
+    <t>run612</t>
+  </si>
+  <si>
+    <t>run614</t>
+  </si>
+  <si>
     <t>run604</t>
   </si>
   <si>
+    <t>run617</t>
+  </si>
+  <si>
     <t>run605</t>
   </si>
   <si>
+    <t>run615</t>
+  </si>
+  <si>
+    <t>run616</t>
+  </si>
+  <si>
     <t>run606</t>
   </si>
   <si>
-    <t>run607</t>
+    <t>run611</t>
   </si>
   <si>
     <t>run608</t>
   </si>
   <si>
-    <t>run609</t>
-  </si>
-  <si>
-    <t>run610</t>
-  </si>
-  <si>
-    <t>run611</t>
-  </si>
-  <si>
-    <t>run612</t>
-  </si>
-  <si>
-    <t>run613</t>
-  </si>
-  <si>
-    <t>run614</t>
-  </si>
-  <si>
-    <t>run615</t>
-  </si>
-  <si>
-    <t>run616</t>
-  </si>
-  <si>
-    <t>run617</t>
-  </si>
-  <si>
     <t>run618</t>
   </si>
   <si>
@@ -2147,6 +2147,9 @@
     <t>run624</t>
   </si>
   <si>
+    <t>not converged</t>
+  </si>
+  <si>
     <t>run625</t>
   </si>
   <si>
@@ -2159,6 +2162,9 @@
     <t>run628</t>
   </si>
   <si>
+    <t>invalid</t>
+  </si>
+  <si>
     <t>run629</t>
   </si>
   <si>
@@ -2259,6 +2265,21 @@
   </si>
   <si>
     <t>run662</t>
+  </si>
+  <si>
+    <t>run663</t>
+  </si>
+  <si>
+    <t>run664</t>
+  </si>
+  <si>
+    <t>run665</t>
+  </si>
+  <si>
+    <t>run666</t>
+  </si>
+  <si>
+    <t>run667</t>
   </si>
 </sst>
 </file>
@@ -2269,7 +2290,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2290,6 +2311,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF800000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2352,7 +2380,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2401,11 +2429,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2426,10 +2470,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K838"/>
+  <dimension ref="A1:K847"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A707" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B718" activeCellId="0" sqref="B718"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A817" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E829" activeCellId="0" sqref="E829"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -14564,8 +14608,9 @@
       <c r="E626" s="6" t="n">
         <v>0.084</v>
       </c>
-    </row>
-    <row r="627" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F626" s="0"/>
+    </row>
+    <row r="627" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A627" s="5" t="n">
         <v>2.0331E-006</v>
       </c>
@@ -14582,7 +14627,7 @@
         <v>0.112</v>
       </c>
     </row>
-    <row r="628" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="628" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A628" s="5" t="n">
         <v>2.8808E-006</v>
       </c>
@@ -14806,7 +14851,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="641" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A641" s="7" t="n">
         <v>0.00010406</v>
       </c>
@@ -15437,7 +15482,7 @@
         <v>0.173</v>
       </c>
     </row>
-    <row r="680" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="680" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="5" t="n">
         <v>0.00033445</v>
       </c>
@@ -15855,7 +15900,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="705" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="705" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A705" s="7" t="n">
         <v>0.00019583</v>
       </c>
@@ -15923,20 +15968,20 @@
         <v>0.318</v>
       </c>
     </row>
-    <row r="709" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A709" s="12" t="n">
+    <row r="709" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A709" s="9" t="n">
         <v>0.00033831</v>
       </c>
-      <c r="B709" s="12" t="n">
+      <c r="B709" s="9" t="n">
         <v>0.0029797</v>
       </c>
-      <c r="C709" s="13" t="s">
+      <c r="C709" s="12" t="s">
         <v>641</v>
       </c>
-      <c r="D709" s="13" t="n">
+      <c r="D709" s="12" t="n">
         <v>18</v>
       </c>
-      <c r="E709" s="13" t="n">
+      <c r="E709" s="12" t="n">
         <v>0.364</v>
       </c>
     </row>
@@ -16140,18 +16185,21 @@
       </c>
       <c r="G726" s="4"/>
     </row>
-    <row r="727" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A727" s="9" t="n">
+    <row r="727" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A727" s="5" t="n">
         <v>1.8666E-005</v>
       </c>
-      <c r="B727" s="9" t="n">
+      <c r="B727" s="5" t="n">
         <v>0.0070719</v>
       </c>
-      <c r="C727" s="0" t="s">
+      <c r="C727" s="6" t="s">
         <v>648</v>
       </c>
-      <c r="D727" s="0" t="n">
+      <c r="D727" s="6" t="n">
         <v>21</v>
+      </c>
+      <c r="E727" s="6" t="n">
+        <v>0.08</v>
       </c>
     </row>
     <row r="728" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16167,131 +16215,161 @@
       <c r="D728" s="0" t="n">
         <v>22</v>
       </c>
-    </row>
-    <row r="729" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A729" s="9" t="n">
+      <c r="E728" s="0" t="n">
+        <v>0.278</v>
+      </c>
+    </row>
+    <row r="729" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A729" s="5" t="n">
         <v>5.2376E-005</v>
       </c>
-      <c r="B729" s="9" t="n">
+      <c r="B729" s="5" t="n">
         <v>0.0418053</v>
       </c>
-      <c r="C729" s="0" t="s">
+      <c r="C729" s="6" t="s">
         <v>650</v>
       </c>
-      <c r="D729" s="0" t="n">
+      <c r="D729" s="6" t="n">
         <v>23</v>
       </c>
-    </row>
-    <row r="730" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A730" s="9" t="n">
-        <v>6.7318E-005</v>
-      </c>
-      <c r="B730" s="9" t="n">
-        <v>0.3159105</v>
-      </c>
-      <c r="C730" s="0" t="s">
+      <c r="E729" s="6" t="n">
+        <v>0.213</v>
+      </c>
+    </row>
+    <row r="730" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A730" s="5" t="n">
+        <v>0.00055539</v>
+      </c>
+      <c r="B730" s="5" t="n">
+        <v>0.0018864</v>
+      </c>
+      <c r="C730" s="6" t="s">
         <v>651</v>
       </c>
-      <c r="D730" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="731" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A731" s="9" t="n">
-        <v>7.427E-005</v>
-      </c>
-      <c r="B731" s="9" t="n">
-        <v>0.0754769</v>
-      </c>
-      <c r="C731" s="0" t="s">
+      <c r="D730" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="E730" s="6" t="n">
+        <v>0.227</v>
+      </c>
+    </row>
+    <row r="731" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A731" s="5" t="n">
+        <v>0.00098877</v>
+      </c>
+      <c r="B731" s="5" t="n">
+        <v>0.0024774</v>
+      </c>
+      <c r="C731" s="6" t="s">
         <v>652</v>
       </c>
-      <c r="D731" s="0" t="n">
-        <v>25</v>
+      <c r="D731" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="E731" s="6" t="n">
+        <v>0.133</v>
       </c>
     </row>
     <row r="732" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A732" s="9" t="n">
-        <v>7.531E-005</v>
+        <v>0.00039029</v>
       </c>
       <c r="B732" s="9" t="n">
-        <v>0.00747</v>
+        <v>0.0028429</v>
       </c>
       <c r="C732" s="0" t="s">
         <v>653</v>
       </c>
       <c r="D732" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E732" s="0" t="n">
+        <v>0.242</v>
+      </c>
+    </row>
+    <row r="733" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A733" s="5" t="n">
+        <v>7.531E-005</v>
+      </c>
+      <c r="B733" s="5" t="n">
+        <v>0.00747</v>
+      </c>
+      <c r="C733" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="D733" s="6" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="733" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A733" s="9" t="n">
-        <v>9.8843E-005</v>
-      </c>
-      <c r="B733" s="9" t="n">
-        <v>0.2547246</v>
-      </c>
-      <c r="C733" s="0" t="s">
-        <v>654</v>
-      </c>
-      <c r="D733" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="734" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A734" s="9" t="n">
-        <v>0.00011354</v>
-      </c>
-      <c r="B734" s="9" t="n">
-        <v>0.1858051</v>
-      </c>
-      <c r="C734" s="0" t="s">
+      <c r="E733" s="6" t="n">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="734" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A734" s="5" t="n">
+        <v>0.0011034</v>
+      </c>
+      <c r="B734" s="5" t="n">
+        <v>0.0116369</v>
+      </c>
+      <c r="C734" s="6" t="s">
         <v>655</v>
       </c>
-      <c r="D734" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="735" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A735" s="9" t="n">
-        <v>0.00013785</v>
-      </c>
-      <c r="B735" s="9" t="n">
-        <v>0.0432537</v>
-      </c>
-      <c r="C735" s="0" t="s">
+      <c r="D734" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="E734" s="6" t="n">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="735" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A735" s="7" t="n">
+        <v>0.00016602</v>
+      </c>
+      <c r="B735" s="7" t="n">
+        <v>0.0231793</v>
+      </c>
+      <c r="C735" s="8" t="s">
         <v>656</v>
       </c>
-      <c r="D735" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="736" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A736" s="9" t="n">
-        <v>0.00016602</v>
-      </c>
-      <c r="B736" s="9" t="n">
-        <v>0.0231793</v>
-      </c>
-      <c r="C736" s="0" t="s">
+      <c r="D735" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E735" s="8" t="n">
+        <v>0.403</v>
+      </c>
+    </row>
+    <row r="736" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A736" s="7" t="n">
+        <v>0.0018385</v>
+      </c>
+      <c r="B736" s="7" t="n">
+        <v>0.0245581</v>
+      </c>
+      <c r="C736" s="8" t="s">
         <v>657</v>
       </c>
-      <c r="D736" s="0" t="n">
-        <v>5</v>
+      <c r="D736" s="8" t="n">
+        <v>19</v>
+      </c>
+      <c r="E736" s="8" t="n">
+        <v>0.486</v>
       </c>
     </row>
     <row r="737" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A737" s="9" t="n">
-        <v>0.00019056</v>
+        <v>0.00013785</v>
       </c>
       <c r="B737" s="9" t="n">
-        <v>0.2528158</v>
+        <v>0.0432537</v>
       </c>
       <c r="C737" s="0" t="s">
         <v>658</v>
       </c>
       <c r="D737" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="E737" s="0" t="n">
+        <v>0.3</v>
       </c>
     </row>
     <row r="738" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16307,117 +16385,144 @@
       <c r="D738" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="739" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A739" s="9" t="n">
-        <v>0.00039029</v>
-      </c>
-      <c r="B739" s="9" t="n">
-        <v>0.0028429</v>
-      </c>
-      <c r="C739" s="0" t="s">
+      <c r="E738" s="0" t="n">
+        <v>0.278</v>
+      </c>
+    </row>
+    <row r="739" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A739" s="7" t="n">
+        <v>7.427E-005</v>
+      </c>
+      <c r="B739" s="7" t="n">
+        <v>0.0754769</v>
+      </c>
+      <c r="C739" s="8" t="s">
         <v>660</v>
       </c>
-      <c r="D739" s="0" t="n">
-        <v>10</v>
+      <c r="D739" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="E739" s="8" t="n">
+        <v>0.467</v>
       </c>
     </row>
     <row r="740" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A740" s="9" t="n">
-        <v>0.00055539</v>
+        <v>0.00011354</v>
       </c>
       <c r="B740" s="9" t="n">
-        <v>0.0018864</v>
+        <v>0.1858051</v>
       </c>
       <c r="C740" s="0" t="s">
         <v>661</v>
       </c>
       <c r="D740" s="0" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="741" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A741" s="9" t="n">
-        <v>0.00090118</v>
-      </c>
-      <c r="B741" s="9" t="n">
-        <v>0.4039587</v>
-      </c>
-      <c r="C741" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E740" s="0" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="741" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A741" s="5" t="n">
+        <v>0.00019056</v>
+      </c>
+      <c r="B741" s="5" t="n">
+        <v>0.2528158</v>
+      </c>
+      <c r="C741" s="6" t="s">
         <v>662</v>
       </c>
-      <c r="D741" s="0" t="n">
-        <v>13</v>
+      <c r="D741" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="E741" s="6" t="n">
+        <v>0.189</v>
       </c>
     </row>
     <row r="742" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A742" s="9" t="n">
-        <v>0.00098877</v>
+        <v>9.8843E-005</v>
       </c>
       <c r="B742" s="9" t="n">
-        <v>0.0024774</v>
+        <v>0.2547246</v>
       </c>
       <c r="C742" s="0" t="s">
         <v>663</v>
       </c>
       <c r="D742" s="0" t="n">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="E742" s="0" t="n">
+        <v>0.272</v>
       </c>
     </row>
     <row r="743" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A743" s="9" t="n">
-        <v>0.0011034</v>
+        <v>6.7318E-005</v>
       </c>
       <c r="B743" s="9" t="n">
-        <v>0.0116369</v>
+        <v>0.3159105</v>
       </c>
       <c r="C743" s="0" t="s">
         <v>664</v>
       </c>
       <c r="D743" s="0" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="744" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A744" s="9" t="n">
+        <v>24</v>
+      </c>
+      <c r="E743" s="0" t="n">
+        <v>0.292</v>
+      </c>
+    </row>
+    <row r="744" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A744" s="5" t="n">
+        <v>0.00090118</v>
+      </c>
+      <c r="B744" s="5" t="n">
+        <v>0.4039587</v>
+      </c>
+      <c r="C744" s="6" t="s">
+        <v>665</v>
+      </c>
+      <c r="D744" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="E744" s="6" t="n">
+        <v>0.208</v>
+      </c>
+    </row>
+    <row r="745" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A745" s="7" t="n">
         <v>0.0013155</v>
       </c>
-      <c r="B744" s="9" t="n">
+      <c r="B745" s="7" t="n">
         <v>0.480748</v>
       </c>
-      <c r="C744" s="0" t="s">
-        <v>665</v>
-      </c>
-      <c r="D744" s="0" t="n">
+      <c r="C745" s="8" t="s">
+        <v>666</v>
+      </c>
+      <c r="D745" s="8" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="745" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A745" s="9" t="n">
-        <v>0.0018385</v>
-      </c>
-      <c r="B745" s="9" t="n">
-        <v>0.0245581</v>
-      </c>
-      <c r="C745" s="0" t="s">
-        <v>666</v>
-      </c>
-      <c r="D745" s="0" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="746" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A746" s="9" t="n">
+      <c r="E745" s="8" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="746" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A746" s="13" t="n">
         <v>0.0041912</v>
       </c>
-      <c r="B746" s="9" t="n">
+      <c r="B746" s="13" t="n">
         <v>0.0295907</v>
       </c>
-      <c r="C746" s="0" t="s">
+      <c r="C746" s="14" t="s">
         <v>667</v>
       </c>
-      <c r="D746" s="0" t="n">
+      <c r="D746" s="14" t="n">
         <v>20</v>
+      </c>
+      <c r="E746" s="14" t="n">
+        <v>0.171</v>
       </c>
     </row>
     <row r="748" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16452,158 +16557,194 @@
       </c>
       <c r="G749" s="4"/>
     </row>
-    <row r="750" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A750" s="9" t="n">
+    <row r="750" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A750" s="5" t="n">
         <v>1.4057E-005</v>
       </c>
-      <c r="B750" s="9" t="n">
+      <c r="B750" s="5" t="n">
         <v>0.0033753</v>
       </c>
-      <c r="C750" s="0" t="s">
+      <c r="C750" s="6" t="s">
         <v>668</v>
       </c>
-      <c r="D750" s="0" t="n">
+      <c r="D750" s="6" t="n">
         <v>21</v>
       </c>
-    </row>
-    <row r="751" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A751" s="9" t="n">
+      <c r="E750" s="6" t="n">
+        <v>0.011</v>
+      </c>
+    </row>
+    <row r="751" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A751" s="5" t="n">
         <v>2.4498E-005</v>
       </c>
-      <c r="B751" s="9" t="n">
+      <c r="B751" s="5" t="n">
         <v>0.0163899</v>
       </c>
-      <c r="C751" s="0" t="s">
+      <c r="C751" s="6" t="s">
         <v>669</v>
       </c>
-      <c r="D751" s="0" t="n">
+      <c r="D751" s="6" t="n">
         <v>22</v>
       </c>
-    </row>
-    <row r="752" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A752" s="9" t="n">
+      <c r="E751" s="6" t="n">
+        <v>0.074</v>
+      </c>
+    </row>
+    <row r="752" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A752" s="7" t="n">
+        <v>0.0001066</v>
+      </c>
+      <c r="B752" s="7" t="n">
+        <v>0.0025984</v>
+      </c>
+      <c r="C752" s="8" t="s">
+        <v>670</v>
+      </c>
+      <c r="D752" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E752" s="8" t="n">
+        <v>0.222</v>
+      </c>
+    </row>
+    <row r="753" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A753" s="7" t="n">
+        <v>0.00027365</v>
+      </c>
+      <c r="B753" s="7" t="n">
+        <v>0.015192</v>
+      </c>
+      <c r="C753" s="8" t="s">
+        <v>671</v>
+      </c>
+      <c r="D753" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E753" s="8" t="n">
+        <v>0.214</v>
+      </c>
+    </row>
+    <row r="754" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A754" s="7" t="n">
+        <v>0.00058323</v>
+      </c>
+      <c r="B754" s="7" t="n">
+        <v>0.0173452</v>
+      </c>
+      <c r="C754" s="8" t="s">
+        <v>672</v>
+      </c>
+      <c r="D754" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E754" s="8" t="n">
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="755" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A755" s="7" t="n">
         <v>4.2452E-005</v>
       </c>
-      <c r="B752" s="9" t="n">
+      <c r="B755" s="7" t="n">
         <v>0.0737432</v>
       </c>
-      <c r="C752" s="0" t="s">
-        <v>670</v>
-      </c>
-      <c r="D752" s="0" t="n">
+      <c r="C755" s="8" t="s">
+        <v>673</v>
+      </c>
+      <c r="D755" s="8" t="n">
         <v>23</v>
       </c>
-    </row>
-    <row r="753" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A753" s="9" t="n">
-        <v>4.8186E-005</v>
-      </c>
-      <c r="B753" s="9" t="n">
-        <v>0.163018</v>
-      </c>
-      <c r="C753" s="0" t="s">
-        <v>671</v>
-      </c>
-      <c r="D753" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="754" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A754" s="9" t="n">
-        <v>7.5177E-005</v>
-      </c>
-      <c r="B754" s="9" t="n">
-        <v>0.1113902</v>
-      </c>
-      <c r="C754" s="0" t="s">
-        <v>672</v>
-      </c>
-      <c r="D754" s="0" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="755" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A755" s="9" t="n">
-        <v>0.0001066</v>
-      </c>
-      <c r="B755" s="9" t="n">
-        <v>0.0025984</v>
-      </c>
-      <c r="C755" s="0" t="s">
-        <v>673</v>
-      </c>
-      <c r="D755" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="756" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A756" s="9" t="n">
-        <v>0.00027365</v>
-      </c>
-      <c r="B756" s="9" t="n">
-        <v>0.015192</v>
-      </c>
-      <c r="C756" s="0" t="s">
+      <c r="E755" s="8" t="n">
+        <v>0.211</v>
+      </c>
+    </row>
+    <row r="756" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A756" s="7" t="n">
+        <v>0.00072716</v>
+      </c>
+      <c r="B756" s="7" t="n">
+        <v>0.0793741</v>
+      </c>
+      <c r="C756" s="8" t="s">
         <v>674</v>
       </c>
-      <c r="D756" s="0" t="n">
-        <v>2</v>
+      <c r="D756" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E756" s="8" t="n">
+        <v>0.206</v>
       </c>
     </row>
     <row r="757" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A757" s="9" t="n">
-        <v>0.00058323</v>
+        <v>0.0011466</v>
       </c>
       <c r="B757" s="9" t="n">
-        <v>0.0173452</v>
+        <v>0.0817089</v>
       </c>
       <c r="C757" s="0" t="s">
         <v>675</v>
       </c>
       <c r="D757" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="E757" s="0" t="n">
+        <v>0.154</v>
       </c>
     </row>
     <row r="758" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A758" s="9" t="n">
-        <v>0.00060707</v>
+        <v>7.5177E-005</v>
       </c>
       <c r="B758" s="9" t="n">
-        <v>0.4357645</v>
+        <v>0.1113902</v>
       </c>
       <c r="C758" s="0" t="s">
         <v>676</v>
       </c>
       <c r="D758" s="0" t="n">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="E758" s="0" t="n">
+        <v>0.138</v>
       </c>
     </row>
     <row r="759" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A759" s="9" t="n">
-        <v>0.00072716</v>
+        <v>4.8186E-005</v>
       </c>
       <c r="B759" s="9" t="n">
-        <v>0.0793741</v>
+        <v>0.163018</v>
       </c>
       <c r="C759" s="0" t="s">
         <v>677</v>
       </c>
       <c r="D759" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="760" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A760" s="9" t="n">
-        <v>0.0011466</v>
-      </c>
-      <c r="B760" s="9" t="n">
-        <v>0.0817089</v>
-      </c>
-      <c r="C760" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E759" s="0" t="n">
+        <v>0.129</v>
+      </c>
+    </row>
+    <row r="760" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A760" s="5" t="n">
+        <v>0.00060707</v>
+      </c>
+      <c r="B760" s="5" t="n">
+        <v>0.4357645</v>
+      </c>
+      <c r="C760" s="6" t="s">
         <v>678</v>
       </c>
-      <c r="D760" s="0" t="n">
-        <v>6</v>
+      <c r="D760" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E760" s="6" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="F760" s="6" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="761" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16619,19 +16760,28 @@
       <c r="D761" s="0" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="762" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A762" s="9" t="n">
+      <c r="E761" s="0" t="n">
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="762" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A762" s="5" t="n">
         <v>0.0016064</v>
       </c>
-      <c r="B762" s="9" t="n">
+      <c r="B762" s="5" t="n">
         <v>0.655014</v>
       </c>
-      <c r="C762" s="0" t="s">
+      <c r="C762" s="6" t="s">
         <v>680</v>
       </c>
-      <c r="D762" s="0" t="n">
+      <c r="D762" s="6" t="n">
         <v>10</v>
+      </c>
+      <c r="E762" s="6" t="n">
+        <v>0.066</v>
+      </c>
+      <c r="F762" s="6" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="763" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16647,47 +16797,65 @@
       <c r="D763" s="0" t="n">
         <v>11</v>
       </c>
-    </row>
-    <row r="764" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A764" s="9" t="n">
+      <c r="E763" s="0" t="n">
+        <v>0.103</v>
+      </c>
+    </row>
+    <row r="764" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A764" s="5" t="n">
         <v>0.0022187</v>
       </c>
-      <c r="B764" s="9" t="n">
+      <c r="B764" s="5" t="n">
         <v>0.5065797</v>
       </c>
-      <c r="C764" s="0" t="s">
+      <c r="C764" s="6" t="s">
         <v>682</v>
       </c>
-      <c r="D764" s="0" t="n">
+      <c r="D764" s="6" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="765" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A765" s="9" t="n">
+      <c r="E764" s="6" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="F764" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="765" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A765" s="5" t="n">
         <v>0.0027533</v>
       </c>
-      <c r="B765" s="9" t="n">
+      <c r="B765" s="5" t="n">
         <v>0.0023478</v>
       </c>
-      <c r="C765" s="0" t="s">
+      <c r="C765" s="6" t="s">
         <v>683</v>
       </c>
-      <c r="D765" s="0" t="n">
+      <c r="D765" s="6" t="n">
         <v>16</v>
       </c>
-    </row>
-    <row r="766" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A766" s="9" t="n">
+      <c r="E765" s="6" t="n">
+        <v>0.007</v>
+      </c>
+    </row>
+    <row r="766" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A766" s="5" t="n">
         <v>0.0038317</v>
       </c>
-      <c r="B766" s="9" t="n">
+      <c r="B766" s="5" t="n">
         <v>0.2289818</v>
       </c>
-      <c r="C766" s="0" t="s">
+      <c r="C766" s="6" t="s">
         <v>684</v>
       </c>
-      <c r="D766" s="0" t="n">
+      <c r="D766" s="6" t="n">
         <v>17</v>
+      </c>
+      <c r="E766" s="6" t="n">
+        <v>0.278</v>
+      </c>
+      <c r="F766" s="6" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="767" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16703,33 +16871,48 @@
       <c r="D767" s="0" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="768" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A768" s="9" t="n">
+      <c r="E767" s="0" t="n">
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="768" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A768" s="5" t="n">
         <v>0.004114</v>
       </c>
-      <c r="B768" s="9" t="n">
+      <c r="B768" s="5" t="n">
         <v>0.1371036</v>
       </c>
-      <c r="C768" s="0" t="s">
+      <c r="C768" s="6" t="s">
         <v>686</v>
       </c>
-      <c r="D768" s="0" t="n">
+      <c r="D768" s="6" t="n">
         <v>19</v>
       </c>
-    </row>
-    <row r="769" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A769" s="9" t="n">
+      <c r="E768" s="6" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="F768" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="769" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A769" s="5" t="n">
         <v>0.0079553</v>
       </c>
-      <c r="B769" s="9" t="n">
+      <c r="B769" s="5" t="n">
         <v>0.3176951</v>
       </c>
-      <c r="C769" s="0" t="s">
+      <c r="C769" s="6" t="s">
         <v>687</v>
       </c>
-      <c r="D769" s="0" t="n">
+      <c r="D769" s="6" t="n">
         <v>20</v>
+      </c>
+      <c r="E769" s="6" t="n">
+        <v>0.176</v>
+      </c>
+      <c r="F769" s="6" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="771" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16764,228 +16947,287 @@
       </c>
       <c r="G772" s="4"/>
     </row>
-    <row r="773" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A773" s="9" t="n">
+    <row r="773" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A773" s="5" t="n">
         <v>1.6003E-005</v>
       </c>
-      <c r="B773" s="9" t="n">
+      <c r="B773" s="5" t="n">
         <v>0.0037366</v>
       </c>
-      <c r="C773" s="0" t="s">
+      <c r="C773" s="6" t="s">
         <v>688</v>
       </c>
-      <c r="D773" s="0" t="n">
+      <c r="D773" s="6" t="n">
         <v>21</v>
       </c>
-    </row>
-    <row r="774" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A774" s="9" t="n">
-        <v>2.5648E-005</v>
-      </c>
-      <c r="B774" s="9" t="n">
-        <v>0.0589231</v>
-      </c>
-      <c r="C774" s="0" t="s">
+      <c r="E773" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="774" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A774" s="5" t="n">
+        <v>0.00022423</v>
+      </c>
+      <c r="B774" s="5" t="n">
+        <v>0.0010541</v>
+      </c>
+      <c r="C774" s="6" t="s">
         <v>689</v>
       </c>
-      <c r="D774" s="0" t="n">
-        <v>22</v>
+      <c r="D774" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E774" s="6" t="n">
+        <v>0.071</v>
       </c>
     </row>
     <row r="775" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A775" s="9" t="n">
-        <v>3.3697E-005</v>
+        <v>0.00030474</v>
       </c>
       <c r="B775" s="9" t="n">
-        <v>0.099009</v>
+        <v>0.0011084</v>
       </c>
       <c r="C775" s="0" t="s">
         <v>690</v>
       </c>
       <c r="D775" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E775" s="0" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="776" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A776" s="7" t="n">
+        <v>9.7291E-005</v>
+      </c>
+      <c r="B776" s="7" t="n">
+        <v>0.0021595</v>
+      </c>
+      <c r="C776" s="8" t="s">
+        <v>691</v>
+      </c>
+      <c r="D776" s="8" t="n">
+        <v>25</v>
+      </c>
+      <c r="E776" s="8" t="n">
+        <v>0.526</v>
+      </c>
+    </row>
+    <row r="777" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A777" s="15" t="n">
+        <v>0.00021776</v>
+      </c>
+      <c r="B777" s="15" t="n">
+        <v>0.0079892</v>
+      </c>
+      <c r="C777" s="16" t="s">
+        <v>692</v>
+      </c>
+      <c r="D777" s="16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E777" s="17" t="n">
+        <v>0.148</v>
+      </c>
+      <c r="F777" s="17"/>
+      <c r="G777" s="17"/>
+    </row>
+    <row r="778" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A778" s="5" t="n">
+        <v>0.00030113</v>
+      </c>
+      <c r="B778" s="5" t="n">
+        <v>0.035105</v>
+      </c>
+      <c r="C778" s="6" t="s">
+        <v>693</v>
+      </c>
+      <c r="D778" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E778" s="6" t="n">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="779" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A779" s="5" t="n">
+        <v>0.00034415</v>
+      </c>
+      <c r="B779" s="5" t="n">
+        <v>0.0565636</v>
+      </c>
+      <c r="C779" s="6" t="s">
+        <v>694</v>
+      </c>
+      <c r="D779" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="E779" s="6" t="n">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="780" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A780" s="7" t="n">
+        <v>2.5648E-005</v>
+      </c>
+      <c r="B780" s="7" t="n">
+        <v>0.0589231</v>
+      </c>
+      <c r="C780" s="8" t="s">
+        <v>695</v>
+      </c>
+      <c r="D780" s="8" t="n">
+        <v>22</v>
+      </c>
+      <c r="E780" s="8" t="n">
+        <v>0.286</v>
+      </c>
+    </row>
+    <row r="781" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A781" s="7" t="n">
+        <v>0.0013526</v>
+      </c>
+      <c r="B781" s="7" t="n">
+        <v>0.0715529</v>
+      </c>
+      <c r="C781" s="8" t="s">
+        <v>696</v>
+      </c>
+      <c r="D781" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="E781" s="8" t="n">
+        <v>0.286</v>
+      </c>
+    </row>
+    <row r="782" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A782" s="7" t="n">
+        <v>3.3697E-005</v>
+      </c>
+      <c r="B782" s="7" t="n">
+        <v>0.099009</v>
+      </c>
+      <c r="C782" s="8" t="s">
+        <v>697</v>
+      </c>
+      <c r="D782" s="8" t="n">
         <v>23</v>
       </c>
-    </row>
-    <row r="776" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A776" s="9" t="n">
-        <v>7.9844E-005</v>
-      </c>
-      <c r="B776" s="9" t="n">
-        <v>0.1673231</v>
-      </c>
-      <c r="C776" s="0" t="s">
-        <v>691</v>
-      </c>
-      <c r="D776" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="777" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A777" s="9" t="n">
-        <v>9.7291E-005</v>
-      </c>
-      <c r="B777" s="9" t="n">
-        <v>0.0021595</v>
-      </c>
-      <c r="C777" s="0" t="s">
-        <v>692</v>
-      </c>
-      <c r="D777" s="0" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="778" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A778" s="9" t="n">
-        <v>0.00011905</v>
-      </c>
-      <c r="B778" s="9" t="n">
-        <v>0.2600791</v>
-      </c>
-      <c r="C778" s="0" t="s">
-        <v>693</v>
-      </c>
-      <c r="D778" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="779" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A779" s="9" t="n">
-        <v>0.00021776</v>
-      </c>
-      <c r="B779" s="9" t="n">
-        <v>0.0079892</v>
-      </c>
-      <c r="C779" s="0" t="s">
-        <v>694</v>
-      </c>
-      <c r="D779" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="780" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A780" s="9" t="n">
-        <v>0.00022423</v>
-      </c>
-      <c r="B780" s="9" t="n">
-        <v>0.0010541</v>
-      </c>
-      <c r="C780" s="0" t="s">
-        <v>695</v>
-      </c>
-      <c r="D780" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="781" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A781" s="9" t="n">
-        <v>0.00028016</v>
-      </c>
-      <c r="B781" s="9" t="n">
-        <v>0.1983943</v>
-      </c>
-      <c r="C781" s="0" t="s">
-        <v>696</v>
-      </c>
-      <c r="D781" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="782" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A782" s="9" t="n">
-        <v>0.00030113</v>
-      </c>
-      <c r="B782" s="9" t="n">
-        <v>0.035105</v>
-      </c>
-      <c r="C782" s="0" t="s">
-        <v>697</v>
-      </c>
-      <c r="D782" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="783" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A783" s="9" t="n">
-        <v>0.00030474</v>
-      </c>
-      <c r="B783" s="9" t="n">
-        <v>0.0011084</v>
-      </c>
-      <c r="C783" s="0" t="s">
+      <c r="E782" s="8" t="n">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="783" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A783" s="5" t="n">
+        <v>0.00046493</v>
+      </c>
+      <c r="B783" s="5" t="n">
+        <v>0.105332</v>
+      </c>
+      <c r="C783" s="6" t="s">
         <v>698</v>
       </c>
-      <c r="D783" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="784" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A784" s="9" t="n">
-        <v>0.00034415</v>
-      </c>
-      <c r="B784" s="9" t="n">
-        <v>0.0565636</v>
-      </c>
-      <c r="C784" s="0" t="s">
+      <c r="D783" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E783" s="6" t="n">
+        <v>0.139</v>
+      </c>
+      <c r="F783" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="784" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A784" s="5" t="n">
+        <v>0.00066423</v>
+      </c>
+      <c r="B784" s="5" t="n">
+        <v>0.1420813</v>
+      </c>
+      <c r="C784" s="6" t="s">
         <v>699</v>
       </c>
-      <c r="D784" s="0" t="n">
-        <v>9</v>
+      <c r="D784" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="E784" s="6" t="n">
+        <v>0.245</v>
+      </c>
+      <c r="F784" s="6" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="785" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A785" s="9" t="n">
-        <v>0.00046493</v>
+        <v>7.9844E-005</v>
       </c>
       <c r="B785" s="9" t="n">
-        <v>0.105332</v>
+        <v>0.1673231</v>
       </c>
       <c r="C785" s="0" t="s">
         <v>700</v>
       </c>
       <c r="D785" s="0" t="n">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="E785" s="0" t="n">
+        <v>0.226</v>
       </c>
     </row>
     <row r="786" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A786" s="9" t="n">
-        <v>0.00066423</v>
+        <v>0.00028016</v>
       </c>
       <c r="B786" s="9" t="n">
-        <v>0.1420813</v>
+        <v>0.1983943</v>
       </c>
       <c r="C786" s="0" t="s">
         <v>701</v>
       </c>
       <c r="D786" s="0" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="787" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A787" s="9" t="n">
-        <v>0.0013526</v>
-      </c>
-      <c r="B787" s="9" t="n">
-        <v>0.0715529</v>
-      </c>
-      <c r="C787" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E786" s="0" t="n">
+        <v>0.217</v>
+      </c>
+    </row>
+    <row r="787" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A787" s="5" t="n">
+        <v>0.00011905</v>
+      </c>
+      <c r="B787" s="5" t="n">
+        <v>0.2600791</v>
+      </c>
+      <c r="C787" s="6" t="s">
         <v>702</v>
       </c>
-      <c r="D787" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="788" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A788" s="9" t="n">
+      <c r="D787" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E787" s="6" t="n">
+        <v>0.206</v>
+      </c>
+      <c r="F787" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="788" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A788" s="5" t="n">
         <v>0.0020599</v>
       </c>
-      <c r="B788" s="9" t="n">
+      <c r="B788" s="5" t="n">
         <v>0.0089621</v>
       </c>
-      <c r="C788" s="0" t="s">
+      <c r="C788" s="6" t="s">
         <v>703</v>
       </c>
-      <c r="D788" s="0" t="n">
+      <c r="D788" s="6" t="n">
         <v>16</v>
+      </c>
+      <c r="E788" s="6" t="n">
+        <v>0.121</v>
       </c>
     </row>
     <row r="789" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17001,47 +17243,68 @@
       <c r="D789" s="0" t="n">
         <v>17</v>
       </c>
-    </row>
-    <row r="790" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A790" s="9" t="n">
+      <c r="E789" s="0" t="n">
+        <v>0.238</v>
+      </c>
+    </row>
+    <row r="790" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A790" s="5" t="n">
         <v>0.0063868</v>
       </c>
-      <c r="B790" s="9" t="n">
+      <c r="B790" s="5" t="n">
         <v>0.0833557</v>
       </c>
-      <c r="C790" s="0" t="s">
+      <c r="C790" s="6" t="s">
         <v>705</v>
       </c>
-      <c r="D790" s="0" t="n">
+      <c r="D790" s="6" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="791" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A791" s="9" t="n">
+      <c r="E790" s="6" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="F790" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="791" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A791" s="5" t="n">
         <v>0.0068406</v>
       </c>
-      <c r="B791" s="9" t="n">
+      <c r="B791" s="5" t="n">
         <v>0.2217931</v>
       </c>
-      <c r="C791" s="0" t="s">
+      <c r="C791" s="6" t="s">
         <v>706</v>
       </c>
-      <c r="D791" s="0" t="n">
+      <c r="D791" s="6" t="n">
         <v>19</v>
       </c>
-    </row>
-    <row r="792" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A792" s="9" t="n">
+      <c r="E791" s="6" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="F791" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="792" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A792" s="5" t="n">
         <v>0.0093967</v>
       </c>
-      <c r="B792" s="9" t="n">
+      <c r="B792" s="5" t="n">
         <v>0.00379</v>
       </c>
-      <c r="C792" s="0" t="s">
+      <c r="C792" s="6" t="s">
         <v>707</v>
       </c>
-      <c r="D792" s="0" t="n">
+      <c r="D792" s="6" t="n">
         <v>20</v>
+      </c>
+      <c r="E792" s="6" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="F792" s="6" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="794" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17076,32 +17339,41 @@
       </c>
       <c r="G795" s="4"/>
     </row>
-    <row r="796" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A796" s="9" t="n">
+    <row r="796" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A796" s="5" t="n">
         <v>1.0766E-005</v>
       </c>
-      <c r="B796" s="9" t="n">
+      <c r="B796" s="5" t="n">
         <v>0.1156074</v>
       </c>
-      <c r="C796" s="0" t="s">
+      <c r="C796" s="6" t="s">
         <v>708</v>
       </c>
-      <c r="D796" s="0" t="n">
+      <c r="D796" s="6" t="n">
         <v>21</v>
       </c>
-    </row>
-    <row r="797" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A797" s="9" t="n">
+      <c r="E796" s="6" t="n">
+        <v>0.089</v>
+      </c>
+    </row>
+    <row r="797" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A797" s="5" t="n">
         <v>1.2384E-005</v>
       </c>
-      <c r="B797" s="9" t="n">
+      <c r="B797" s="5" t="n">
         <v>0.0011149</v>
       </c>
-      <c r="C797" s="0" t="s">
+      <c r="C797" s="6" t="s">
         <v>709</v>
       </c>
-      <c r="D797" s="0" t="n">
+      <c r="D797" s="6" t="n">
         <v>22</v>
+      </c>
+      <c r="E797" s="6" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="F797" s="6" t="s">
+        <v>710</v>
       </c>
     </row>
     <row r="798" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17112,38 +17384,47 @@
         <v>0.0663546</v>
       </c>
       <c r="C798" s="0" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="D798" s="0" t="n">
         <v>23</v>
       </c>
-    </row>
-    <row r="799" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A799" s="9" t="n">
+      <c r="E798" s="0" t="n">
+        <v>0.143</v>
+      </c>
+    </row>
+    <row r="799" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A799" s="5" t="n">
         <v>3.0926E-005</v>
       </c>
-      <c r="B799" s="9" t="n">
+      <c r="B799" s="5" t="n">
         <v>0.0031829</v>
       </c>
-      <c r="C799" s="0" t="s">
-        <v>711</v>
-      </c>
-      <c r="D799" s="0" t="n">
+      <c r="C799" s="6" t="s">
+        <v>712</v>
+      </c>
+      <c r="D799" s="6" t="n">
         <v>24</v>
       </c>
-    </row>
-    <row r="800" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A800" s="9" t="n">
+      <c r="E799" s="6" t="n">
+        <v>0.082</v>
+      </c>
+    </row>
+    <row r="800" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A800" s="5" t="n">
         <v>5.2782E-005</v>
       </c>
-      <c r="B800" s="9" t="n">
+      <c r="B800" s="5" t="n">
         <v>0.0015249</v>
       </c>
-      <c r="C800" s="0" t="s">
-        <v>712</v>
-      </c>
-      <c r="D800" s="0" t="n">
+      <c r="C800" s="6" t="s">
+        <v>713</v>
+      </c>
+      <c r="D800" s="6" t="n">
         <v>25</v>
+      </c>
+      <c r="E800" s="6" t="n">
+        <v>0.091</v>
       </c>
     </row>
     <row r="801" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17154,10 +17435,16 @@
         <v>0.0018747</v>
       </c>
       <c r="C801" s="0" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D801" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="E801" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F801" s="0" t="s">
+        <v>715</v>
       </c>
     </row>
     <row r="802" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17168,192 +17455,252 @@
         <v>0.2059166</v>
       </c>
       <c r="C802" s="0" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="D802" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="803" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A803" s="9" t="n">
+    <row r="803" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A803" s="7" t="n">
         <v>0.00011174</v>
       </c>
-      <c r="B803" s="9" t="n">
+      <c r="B803" s="7" t="n">
         <v>0.0021338</v>
       </c>
-      <c r="C803" s="0" t="s">
-        <v>715</v>
-      </c>
-      <c r="D803" s="0" t="n">
+      <c r="C803" s="8" t="s">
+        <v>717</v>
+      </c>
+      <c r="D803" s="8" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="804" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A804" s="9" t="n">
+      <c r="E803" s="8" t="n">
+        <v>0.281</v>
+      </c>
+    </row>
+    <row r="804" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A804" s="5" t="n">
         <v>0.00011868</v>
       </c>
-      <c r="B804" s="9" t="n">
+      <c r="B804" s="5" t="n">
         <v>0.0013809</v>
       </c>
-      <c r="C804" s="0" t="s">
-        <v>716</v>
-      </c>
-      <c r="D804" s="0" t="n">
+      <c r="C804" s="6" t="s">
+        <v>718</v>
+      </c>
+      <c r="D804" s="6" t="n">
         <v>4</v>
       </c>
-    </row>
-    <row r="805" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A805" s="9" t="n">
+      <c r="E804" s="6" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="F804" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="805" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A805" s="7" t="n">
         <v>0.00032365</v>
       </c>
-      <c r="B805" s="9" t="n">
+      <c r="B805" s="7" t="n">
         <v>0.014724</v>
       </c>
-      <c r="C805" s="0" t="s">
-        <v>717</v>
-      </c>
-      <c r="D805" s="0" t="n">
+      <c r="C805" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="D805" s="8" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="806" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A806" s="9" t="n">
+      <c r="E805" s="8" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="806" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A806" s="7" t="n">
         <v>0.00034651</v>
       </c>
-      <c r="B806" s="9" t="n">
+      <c r="B806" s="7" t="n">
         <v>0.0456386</v>
       </c>
-      <c r="C806" s="0" t="s">
-        <v>718</v>
-      </c>
-      <c r="D806" s="0" t="n">
+      <c r="C806" s="8" t="s">
+        <v>720</v>
+      </c>
+      <c r="D806" s="8" t="n">
         <v>6</v>
       </c>
-    </row>
-    <row r="807" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A807" s="9" t="n">
+      <c r="E806" s="8" t="n">
+        <v>0.286</v>
+      </c>
+    </row>
+    <row r="807" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A807" s="7" t="n">
         <v>0.00043861</v>
       </c>
-      <c r="B807" s="9" t="n">
+      <c r="B807" s="7" t="n">
         <v>0.0011856</v>
       </c>
-      <c r="C807" s="0" t="s">
-        <v>719</v>
-      </c>
-      <c r="D807" s="0" t="n">
+      <c r="C807" s="8" t="s">
+        <v>721</v>
+      </c>
+      <c r="D807" s="8" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="808" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A808" s="9" t="n">
+      <c r="E807" s="8" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="808" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A808" s="5" t="n">
         <v>0.0011725</v>
       </c>
-      <c r="B808" s="9" t="n">
+      <c r="B808" s="5" t="n">
         <v>0.0088062</v>
       </c>
-      <c r="C808" s="0" t="s">
-        <v>720</v>
-      </c>
-      <c r="D808" s="0" t="n">
+      <c r="C808" s="6" t="s">
+        <v>722</v>
+      </c>
+      <c r="D808" s="6" t="n">
         <v>10</v>
       </c>
-    </row>
-    <row r="809" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A809" s="9" t="n">
+      <c r="E808" s="6" t="n">
+        <v>0.156</v>
+      </c>
+      <c r="F808" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="809" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A809" s="7" t="n">
         <v>0.0013901</v>
       </c>
-      <c r="B809" s="9" t="n">
+      <c r="B809" s="7" t="n">
         <v>0.0847856</v>
       </c>
-      <c r="C809" s="0" t="s">
-        <v>721</v>
-      </c>
-      <c r="D809" s="0" t="n">
+      <c r="C809" s="8" t="s">
+        <v>723</v>
+      </c>
+      <c r="D809" s="8" t="n">
         <v>11</v>
       </c>
-    </row>
-    <row r="810" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A810" s="9" t="n">
+      <c r="E809" s="8" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="810" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A810" s="5" t="n">
         <v>0.0014098</v>
       </c>
-      <c r="B810" s="9" t="n">
+      <c r="B810" s="5" t="n">
         <v>0.0069111</v>
       </c>
-      <c r="C810" s="0" t="s">
-        <v>722</v>
-      </c>
-      <c r="D810" s="0" t="n">
+      <c r="C810" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="D810" s="6" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="811" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A811" s="9" t="n">
+      <c r="E810" s="6" t="n">
+        <v>0.114</v>
+      </c>
+      <c r="F810" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="811" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A811" s="5" t="n">
         <v>0.0015129</v>
       </c>
-      <c r="B811" s="9" t="n">
+      <c r="B811" s="5" t="n">
         <v>0.0122894</v>
       </c>
-      <c r="C811" s="0" t="s">
-        <v>723</v>
-      </c>
-      <c r="D811" s="0" t="n">
+      <c r="C811" s="6" t="s">
+        <v>725</v>
+      </c>
+      <c r="D811" s="6" t="n">
         <v>16</v>
       </c>
-    </row>
-    <row r="812" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A812" s="9" t="n">
+      <c r="E811" s="6" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="812" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A812" s="5" t="n">
         <v>0.0044888</v>
       </c>
-      <c r="B812" s="9" t="n">
+      <c r="B812" s="5" t="n">
         <v>0.0466439</v>
       </c>
-      <c r="C812" s="0" t="s">
-        <v>724</v>
-      </c>
-      <c r="D812" s="0" t="n">
+      <c r="C812" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="D812" s="6" t="n">
         <v>17</v>
       </c>
-    </row>
-    <row r="813" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A813" s="9" t="n">
+      <c r="E812" s="6" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="F812" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="813" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A813" s="5" t="n">
         <v>0.0045995</v>
       </c>
-      <c r="B813" s="9" t="n">
+      <c r="B813" s="5" t="n">
         <v>0.834387</v>
       </c>
-      <c r="C813" s="0" t="s">
-        <v>725</v>
-      </c>
-      <c r="D813" s="0" t="n">
+      <c r="C813" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D813" s="6" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row r="814" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A814" s="9" t="n">
+      <c r="E813" s="6" t="n">
+        <v>0.106</v>
+      </c>
+      <c r="F813" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="814" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A814" s="5" t="n">
         <v>0.0089622</v>
       </c>
-      <c r="B814" s="9" t="n">
+      <c r="B814" s="5" t="n">
         <v>0.0049203</v>
       </c>
-      <c r="C814" s="0" t="s">
-        <v>726</v>
-      </c>
-      <c r="D814" s="0" t="n">
+      <c r="C814" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="D814" s="6" t="n">
         <v>19</v>
       </c>
-    </row>
-    <row r="815" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A815" s="9" t="n">
+      <c r="E814" s="6" t="n">
+        <v>0.093</v>
+      </c>
+      <c r="F814" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="815" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A815" s="5" t="n">
         <v>0.0095502</v>
       </c>
-      <c r="B815" s="9" t="n">
+      <c r="B815" s="5" t="n">
         <v>0.0032744</v>
       </c>
-      <c r="C815" s="0" t="s">
-        <v>727</v>
-      </c>
-      <c r="D815" s="0" t="n">
+      <c r="C815" s="6" t="s">
+        <v>729</v>
+      </c>
+      <c r="D815" s="6" t="n">
         <v>20</v>
+      </c>
+      <c r="E815" s="6" t="n">
+        <v>0.418</v>
+      </c>
+      <c r="F815" s="6" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="817" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17388,88 +17735,106 @@
       </c>
       <c r="G818" s="4"/>
     </row>
-    <row r="819" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A819" s="9" t="n">
+    <row r="819" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A819" s="7" t="n">
         <v>1.4658E-005</v>
       </c>
-      <c r="B819" s="9" t="n">
+      <c r="B819" s="7" t="n">
         <v>0.9801203</v>
       </c>
-      <c r="C819" s="0" t="s">
-        <v>728</v>
-      </c>
-      <c r="D819" s="0" t="n">
+      <c r="C819" s="8" t="s">
+        <v>730</v>
+      </c>
+      <c r="D819" s="8" t="n">
         <v>21</v>
       </c>
-    </row>
-    <row r="820" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A820" s="9" t="n">
+      <c r="E819" s="8" t="n">
+        <v>0.256</v>
+      </c>
+    </row>
+    <row r="820" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A820" s="5" t="n">
         <v>1.789E-005</v>
       </c>
-      <c r="B820" s="9" t="n">
+      <c r="B820" s="5" t="n">
         <v>0.1856801</v>
       </c>
-      <c r="C820" s="0" t="s">
-        <v>729</v>
-      </c>
-      <c r="D820" s="0" t="n">
+      <c r="C820" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="D820" s="6" t="n">
         <v>22</v>
       </c>
-    </row>
-    <row r="821" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A821" s="9" t="n">
+      <c r="E820" s="6" t="n">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="821" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A821" s="5" t="n">
         <v>2.0804E-005</v>
       </c>
-      <c r="B821" s="9" t="n">
+      <c r="B821" s="5" t="n">
         <v>0.0333956</v>
       </c>
-      <c r="C821" s="0" t="s">
-        <v>730</v>
-      </c>
-      <c r="D821" s="0" t="n">
+      <c r="C821" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="D821" s="6" t="n">
         <v>23</v>
       </c>
-    </row>
-    <row r="822" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A822" s="9" t="n">
+      <c r="E821" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="822" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A822" s="5" t="n">
         <v>2.6244E-005</v>
       </c>
-      <c r="B822" s="9" t="n">
+      <c r="B822" s="5" t="n">
         <v>0.0652882</v>
       </c>
-      <c r="C822" s="0" t="s">
-        <v>731</v>
-      </c>
-      <c r="D822" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="823" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A823" s="9" t="n">
+      <c r="C822" s="6" t="s">
+        <v>733</v>
+      </c>
+      <c r="D822" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E822" s="6" t="n">
+        <v>0.077</v>
+      </c>
+    </row>
+    <row r="823" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A823" s="5" t="n">
         <v>0.00014789</v>
       </c>
-      <c r="B823" s="9" t="n">
+      <c r="B823" s="5" t="n">
         <v>0.0051614</v>
       </c>
-      <c r="C823" s="0" t="s">
-        <v>732</v>
-      </c>
-      <c r="D823" s="0" t="n">
+      <c r="C823" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="D823" s="6" t="n">
         <v>25</v>
       </c>
-    </row>
-    <row r="824" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A824" s="9" t="n">
+      <c r="E823" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="824" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A824" s="5" t="n">
         <v>0.00016985</v>
       </c>
-      <c r="B824" s="9" t="n">
+      <c r="B824" s="5" t="n">
         <v>0.0113498</v>
       </c>
-      <c r="C824" s="0" t="s">
-        <v>733</v>
-      </c>
-      <c r="D824" s="0" t="n">
+      <c r="C824" s="6" t="s">
+        <v>735</v>
+      </c>
+      <c r="D824" s="6" t="n">
         <v>1</v>
+      </c>
+      <c r="E824" s="6" t="n">
+        <v>0.099</v>
       </c>
     </row>
     <row r="825" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17480,24 +17845,27 @@
         <v>0.4389243</v>
       </c>
       <c r="C825" s="0" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="D825" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="826" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A826" s="9" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="826" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A826" s="5" t="n">
         <v>0.00029028</v>
       </c>
-      <c r="B826" s="9" t="n">
+      <c r="B826" s="5" t="n">
         <v>0.0041465</v>
       </c>
-      <c r="C826" s="0" t="s">
-        <v>735</v>
-      </c>
-      <c r="D826" s="0" t="n">
-        <v>3</v>
+      <c r="C826" s="6" t="s">
+        <v>737</v>
+      </c>
+      <c r="D826" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="E826" s="6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="827" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17508,168 +17876,330 @@
         <v>0.0014349</v>
       </c>
       <c r="C827" s="0" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="D827" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="E827" s="0" t="n">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="828" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A828" s="7" t="n">
+        <v>0.00092139</v>
+      </c>
+      <c r="B828" s="7" t="n">
+        <v>0.1588808</v>
+      </c>
+      <c r="C828" s="8" t="s">
+        <v>739</v>
+      </c>
+      <c r="D828" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="E828" s="8" t="n">
+        <v>0.226</v>
+      </c>
+    </row>
+    <row r="829" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A829" s="7" t="n">
+        <v>0.00097997</v>
+      </c>
+      <c r="B829" s="7" t="n">
+        <v>0.0056658</v>
+      </c>
+      <c r="C829" s="8" t="s">
+        <v>740</v>
+      </c>
+      <c r="D829" s="8" t="n">
+        <v>22</v>
+      </c>
+      <c r="E829" s="8" t="n">
+        <v>0.215</v>
+      </c>
+    </row>
+    <row r="830" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A830" s="5" t="n">
+        <v>0.0012963</v>
+      </c>
+      <c r="B830" s="5" t="n">
+        <v>0.1790334</v>
+      </c>
+      <c r="C830" s="6" t="s">
+        <v>741</v>
+      </c>
+      <c r="D830" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="E830" s="6" t="n">
+        <v>0.059</v>
+      </c>
+    </row>
+    <row r="831" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A831" s="15" t="n">
+        <v>0.0025991</v>
+      </c>
+      <c r="B831" s="15" t="n">
+        <v>0.0393241</v>
+      </c>
+      <c r="C831" s="16" t="s">
+        <v>742</v>
+      </c>
+      <c r="D831" s="16" t="n">
+        <v>10</v>
+      </c>
+      <c r="E831" s="16" t="n">
+        <v>0.167</v>
+      </c>
+    </row>
+    <row r="832" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A832" s="5" t="n">
+        <v>0.0033339</v>
+      </c>
+      <c r="B832" s="5" t="n">
+        <v>0.131221</v>
+      </c>
+      <c r="C832" s="6" t="s">
+        <v>743</v>
+      </c>
+      <c r="D832" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="E832" s="6" t="n">
+        <v>0.101</v>
+      </c>
+      <c r="F832" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="833" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A833" s="5" t="n">
+        <v>0.0037212</v>
+      </c>
+      <c r="B833" s="5" t="n">
+        <v>0.0075311</v>
+      </c>
+      <c r="C833" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="D833" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="E833" s="6" t="n">
+        <v>0.119</v>
+      </c>
+      <c r="F833" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="834" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A834" s="5" t="n">
+        <v>0.0039612</v>
+      </c>
+      <c r="B834" s="5" t="n">
+        <v>0.0032546</v>
+      </c>
+      <c r="C834" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="D834" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="E834" s="6" t="n">
+        <v>0.136</v>
+      </c>
+      <c r="F834" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="835" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A835" s="5" t="n">
+        <v>0.0050502</v>
+      </c>
+      <c r="B835" s="5" t="n">
+        <v>0.0020429</v>
+      </c>
+      <c r="C835" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="D835" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="E835" s="6" t="n">
+        <v>0.826</v>
+      </c>
+      <c r="F835" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="836" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A836" s="15" t="n">
+        <v>0.0054268</v>
+      </c>
+      <c r="B836" s="15" t="n">
+        <v>0.0015947</v>
+      </c>
+      <c r="C836" s="16" t="s">
+        <v>747</v>
+      </c>
+      <c r="D836" s="16" t="n">
+        <v>18</v>
+      </c>
+      <c r="E836" s="16" t="n">
+        <v>0.167</v>
+      </c>
+    </row>
+    <row r="837" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A837" s="5" t="n">
+        <v>0.0063049</v>
+      </c>
+      <c r="B837" s="5" t="n">
+        <v>0.0852885</v>
+      </c>
+      <c r="C837" s="6" t="s">
+        <v>748</v>
+      </c>
+      <c r="D837" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="E837" s="6" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="F837" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="838" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A838" s="5" t="n">
+        <v>0.008088</v>
+      </c>
+      <c r="B838" s="5" t="n">
+        <v>0.0026024</v>
+      </c>
+      <c r="C838" s="6" t="s">
+        <v>749</v>
+      </c>
+      <c r="D838" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E838" s="6" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="F838" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="841" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A841" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B841" s="11"/>
+      <c r="C841" s="11"/>
+      <c r="D841" s="11"/>
+      <c r="E841" s="11"/>
+      <c r="F841" s="11"/>
+      <c r="G841" s="11"/>
+    </row>
+    <row r="842" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A842" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B842" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C842" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="828" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A828" s="9" t="n">
-        <v>0.00092139</v>
-      </c>
-      <c r="B828" s="9" t="n">
-        <v>0.1588808</v>
-      </c>
-      <c r="C828" s="0" t="s">
-        <v>737</v>
-      </c>
-      <c r="D828" s="0" t="n">
+      <c r="D842" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="829" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A829" s="9" t="n">
-        <v>0.00097997</v>
-      </c>
-      <c r="B829" s="9" t="n">
-        <v>0.0056658</v>
-      </c>
-      <c r="C829" s="0" t="s">
-        <v>738</v>
-      </c>
-      <c r="D829" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="830" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A830" s="9" t="n">
-        <v>0.0012963</v>
-      </c>
-      <c r="B830" s="9" t="n">
-        <v>0.1790334</v>
-      </c>
-      <c r="C830" s="0" t="s">
-        <v>739</v>
-      </c>
-      <c r="D830" s="0" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="831" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A831" s="9" t="n">
-        <v>0.0025991</v>
-      </c>
-      <c r="B831" s="9" t="n">
-        <v>0.0393241</v>
-      </c>
-      <c r="C831" s="0" t="s">
-        <v>740</v>
-      </c>
-      <c r="D831" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="832" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A832" s="9" t="n">
-        <v>0.0033339</v>
-      </c>
-      <c r="B832" s="9" t="n">
-        <v>0.131221</v>
-      </c>
-      <c r="C832" s="0" t="s">
-        <v>741</v>
-      </c>
-      <c r="D832" s="0" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="833" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A833" s="9" t="n">
-        <v>0.0037212</v>
-      </c>
-      <c r="B833" s="9" t="n">
-        <v>0.0075311</v>
-      </c>
-      <c r="C833" s="0" t="s">
-        <v>742</v>
-      </c>
-      <c r="D833" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="834" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A834" s="9" t="n">
-        <v>0.0039612</v>
-      </c>
-      <c r="B834" s="9" t="n">
-        <v>0.0032546</v>
-      </c>
-      <c r="C834" s="0" t="s">
-        <v>743</v>
-      </c>
-      <c r="D834" s="0" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="835" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A835" s="9" t="n">
-        <v>0.0050502</v>
-      </c>
-      <c r="B835" s="9" t="n">
-        <v>0.0020429</v>
-      </c>
-      <c r="C835" s="0" t="s">
-        <v>744</v>
-      </c>
-      <c r="D835" s="0" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="836" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A836" s="9" t="n">
-        <v>0.0054268</v>
-      </c>
-      <c r="B836" s="9" t="n">
-        <v>0.0015947</v>
-      </c>
-      <c r="C836" s="0" t="s">
-        <v>745</v>
-      </c>
-      <c r="D836" s="0" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="837" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A837" s="9" t="n">
-        <v>0.0063049</v>
-      </c>
-      <c r="B837" s="9" t="n">
-        <v>0.0852885</v>
-      </c>
-      <c r="C837" s="0" t="s">
-        <v>746</v>
-      </c>
-      <c r="D837" s="0" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="838" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A838" s="9" t="n">
-        <v>0.008088</v>
-      </c>
-      <c r="B838" s="9" t="n">
-        <v>0.0026024</v>
-      </c>
-      <c r="C838" s="0" t="s">
-        <v>747</v>
-      </c>
-      <c r="D838" s="0" t="n">
-        <v>20</v>
+      <c r="E842" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="F842" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="843" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A843" s="9" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="B843" s="9" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C843" s="0" t="s">
+        <v>750</v>
+      </c>
+      <c r="D843" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="F843" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="844" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A844" s="9" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="B844" s="9" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C844" s="0" t="s">
+        <v>751</v>
+      </c>
+      <c r="D844" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="F844" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="845" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A845" s="9" t="n">
+        <v>7E-005</v>
+      </c>
+      <c r="B845" s="9" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="C845" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="D845" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="F845" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="846" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A846" s="9"/>
+      <c r="B846" s="9"/>
+      <c r="C846" s="0" t="s">
+        <v>753</v>
+      </c>
+      <c r="D846" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F846" s="0" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="847" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A847" s="9"/>
+      <c r="B847" s="9"/>
+      <c r="C847" s="0" t="s">
+        <v>754</v>
+      </c>
+      <c r="D847" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F847" s="0" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="46">
+  <mergeCells count="47">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A41:K41"/>
@@ -17716,6 +18246,7 @@
     <mergeCell ref="A771:G771"/>
     <mergeCell ref="A794:G794"/>
     <mergeCell ref="A817:G817"/>
+    <mergeCell ref="A841:G841"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>